<commit_message>
initial commit - workplan - day 1
</commit_message>
<xml_diff>
--- a/Workplan.xlsx
+++ b/Workplan.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="52">
   <si>
     <t>ACTIVITIES</t>
   </si>
@@ -153,12 +153,6 @@
     <t>Status</t>
   </si>
   <si>
-    <t>Overall Project Percentage</t>
-  </si>
-  <si>
-    <t>Percentage as a component of the project</t>
-  </si>
-  <si>
     <t>DAY 1 - JULY 14, 2016</t>
   </si>
   <si>
@@ -169,6 +163,98 @@
   </si>
   <si>
     <t>Reviewed by:</t>
+  </si>
+  <si>
+    <t>Percentage</t>
+  </si>
+  <si>
+    <t>Completed</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Team Lead/CI-CD: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Angelo Q. De Rivera     </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">CI-CD: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Patrick Ian A. Limpin</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">   Dev/CI-CD:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Rhodenel  S. Omaña   </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Document Writers:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Bianca Denise A. Del Puerto   Angela Lynne G. Lapus</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -745,7 +831,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="96">
+  <cellXfs count="94">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -795,12 +881,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -846,15 +926,6 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="5"/>
     </xf>
@@ -891,30 +962,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="3" fillId="3" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="3" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="3" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="5" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -923,15 +973,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="3" fillId="6" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -943,40 +984,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -999,9 +1016,6 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1011,19 +1025,85 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="3" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="3" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="3" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="5" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1325,10 +1405,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I25"/>
+  <dimension ref="A1:H25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1338,207 +1418,235 @@
     <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.140625" customWidth="1"/>
     <col min="5" max="5" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.28515625" style="64" customWidth="1"/>
-    <col min="7" max="7" width="11.42578125" customWidth="1"/>
-    <col min="8" max="8" width="10.85546875" customWidth="1"/>
-    <col min="9" max="9" width="39.5703125" customWidth="1"/>
+    <col min="6" max="6" width="11.42578125" customWidth="1"/>
+    <col min="7" max="7" width="10.85546875" customWidth="1"/>
+    <col min="8" max="8" width="54.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="64" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="91" t="s">
-        <v>48</v>
-      </c>
-      <c r="B1" s="91"/>
-      <c r="C1" s="91"/>
-      <c r="D1" s="91"/>
-      <c r="E1" s="91"/>
-      <c r="F1" s="91"/>
-      <c r="G1" s="91"/>
-      <c r="H1" s="91"/>
-      <c r="I1" s="91"/>
-    </row>
-    <row r="2" spans="1:9" s="64" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="75" t="s">
+    <row r="1" spans="1:8" s="49" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="77" t="s">
+        <v>46</v>
+      </c>
+      <c r="B1" s="77"/>
+      <c r="C1" s="77"/>
+      <c r="D1" s="77"/>
+      <c r="E1" s="77"/>
+      <c r="F1" s="77"/>
+      <c r="G1" s="77"/>
+      <c r="H1" s="77"/>
+    </row>
+    <row r="2" spans="1:8" s="49" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="73" t="s">
         <v>38</v>
       </c>
-      <c r="B3" s="73" t="s">
-        <v>47</v>
-      </c>
-      <c r="C3" s="70"/>
-      <c r="D3" s="70"/>
-      <c r="E3" s="70"/>
-      <c r="F3" s="70"/>
-      <c r="G3" s="70"/>
-      <c r="H3" s="71"/>
-      <c r="I3" s="77" t="s">
+      <c r="B3" s="70" t="s">
+        <v>45</v>
+      </c>
+      <c r="C3" s="71"/>
+      <c r="D3" s="71"/>
+      <c r="E3" s="71"/>
+      <c r="F3" s="71"/>
+      <c r="G3" s="72"/>
+      <c r="H3" s="75" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="48" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="76"/>
-      <c r="B4" s="74" t="s">
+    <row r="4" spans="1:8" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="74"/>
+      <c r="B4" s="55" t="s">
         <v>40</v>
       </c>
-      <c r="C4" s="69" t="s">
+      <c r="C4" s="53" t="s">
         <v>41</v>
       </c>
-      <c r="D4" s="69" t="s">
+      <c r="D4" s="53" t="s">
         <v>42</v>
       </c>
-      <c r="E4" s="69" t="s">
+      <c r="E4" s="53" t="s">
         <v>43</v>
       </c>
-      <c r="F4" s="69" t="s">
-        <v>46</v>
-      </c>
-      <c r="G4" s="69" t="s">
-        <v>45</v>
-      </c>
-      <c r="H4" s="72" t="s">
+      <c r="F4" s="53" t="s">
+        <v>49</v>
+      </c>
+      <c r="G4" s="54" t="s">
         <v>44</v>
       </c>
-      <c r="I4" s="78"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="83"/>
-      <c r="B5" s="79"/>
-      <c r="C5" s="67"/>
-      <c r="D5" s="67"/>
-      <c r="E5" s="67"/>
-      <c r="F5" s="67"/>
-      <c r="G5" s="68"/>
-      <c r="H5" s="86"/>
-      <c r="I5" s="90"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="84"/>
-      <c r="B6" s="80"/>
-      <c r="C6" s="65"/>
-      <c r="D6" s="65"/>
-      <c r="E6" s="65"/>
-      <c r="F6" s="65"/>
-      <c r="G6" s="10"/>
-      <c r="H6" s="87"/>
-      <c r="I6" s="84"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="84"/>
-      <c r="B7" s="80"/>
-      <c r="C7" s="65"/>
-      <c r="D7" s="65"/>
-      <c r="E7" s="10"/>
-      <c r="F7" s="10"/>
-      <c r="G7" s="10"/>
-      <c r="H7" s="88"/>
-      <c r="I7" s="84"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="84"/>
-      <c r="B8" s="80"/>
-      <c r="C8" s="65"/>
-      <c r="D8" s="65"/>
+      <c r="H4" s="76"/>
+    </row>
+    <row r="5" spans="1:8" ht="83.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="60" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="56">
+        <v>42565</v>
+      </c>
+      <c r="C5" s="56">
+        <v>42565</v>
+      </c>
+      <c r="D5" s="56">
+        <v>42565</v>
+      </c>
+      <c r="E5" s="56">
+        <v>42565</v>
+      </c>
+      <c r="F5" s="52">
+        <v>100</v>
+      </c>
+      <c r="G5" s="63" t="s">
+        <v>50</v>
+      </c>
+      <c r="H5" s="66" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="61" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="56">
+        <v>42565</v>
+      </c>
+      <c r="C6" s="56">
+        <v>42565</v>
+      </c>
+      <c r="D6" s="56">
+        <v>42565</v>
+      </c>
+      <c r="E6" s="56">
+        <v>42565</v>
+      </c>
+      <c r="F6" s="10">
+        <v>100</v>
+      </c>
+      <c r="G6" s="63" t="s">
+        <v>50</v>
+      </c>
+      <c r="H6" s="61"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="61" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="56">
+        <v>42565</v>
+      </c>
+      <c r="C7" s="56">
+        <v>42565</v>
+      </c>
+      <c r="D7" s="56">
+        <v>42565</v>
+      </c>
+      <c r="E7" s="56">
+        <v>42565</v>
+      </c>
+      <c r="F7" s="10">
+        <v>100</v>
+      </c>
+      <c r="G7" s="63" t="s">
+        <v>50</v>
+      </c>
+      <c r="H7" s="61"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="61"/>
+      <c r="B8" s="57"/>
+      <c r="C8" s="50"/>
+      <c r="D8" s="50"/>
       <c r="E8" s="10"/>
       <c r="F8" s="10"/>
-      <c r="G8" s="10"/>
-      <c r="H8" s="88"/>
-      <c r="I8" s="84"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="84"/>
-      <c r="B9" s="81"/>
+      <c r="G8" s="64"/>
+      <c r="H8" s="61"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="61"/>
+      <c r="B9" s="58"/>
       <c r="C9" s="10"/>
       <c r="D9" s="10"/>
       <c r="E9" s="10"/>
       <c r="F9" s="10"/>
-      <c r="G9" s="10"/>
-      <c r="H9" s="88"/>
-      <c r="I9" s="84"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="84"/>
-      <c r="B10" s="81"/>
+      <c r="G9" s="64"/>
+      <c r="H9" s="61"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="61"/>
+      <c r="B10" s="58"/>
       <c r="C10" s="10"/>
       <c r="D10" s="10"/>
       <c r="E10" s="10"/>
       <c r="F10" s="10"/>
-      <c r="G10" s="10"/>
-      <c r="H10" s="88"/>
-      <c r="I10" s="84"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="84"/>
-      <c r="B11" s="81"/>
+      <c r="G10" s="64"/>
+      <c r="H10" s="61"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="61"/>
+      <c r="B11" s="58"/>
       <c r="C11" s="10"/>
       <c r="D11" s="10"/>
       <c r="E11" s="10"/>
       <c r="F11" s="10"/>
-      <c r="G11" s="10"/>
-      <c r="H11" s="88"/>
-      <c r="I11" s="84"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="84"/>
-      <c r="B12" s="81"/>
+      <c r="G11" s="64"/>
+      <c r="H11" s="61"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="61"/>
+      <c r="B12" s="58"/>
       <c r="C12" s="10"/>
       <c r="D12" s="10"/>
       <c r="E12" s="10"/>
       <c r="F12" s="10"/>
-      <c r="G12" s="10"/>
-      <c r="H12" s="88"/>
-      <c r="I12" s="84"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="84"/>
-      <c r="B13" s="81"/>
+      <c r="G12" s="64"/>
+      <c r="H12" s="61"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="61"/>
+      <c r="B13" s="58"/>
       <c r="C13" s="10"/>
       <c r="D13" s="10"/>
       <c r="E13" s="10"/>
       <c r="F13" s="10"/>
-      <c r="G13" s="10"/>
-      <c r="H13" s="88"/>
-      <c r="I13" s="84"/>
-    </row>
-    <row r="14" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="85"/>
-      <c r="B14" s="82"/>
-      <c r="C14" s="66"/>
-      <c r="D14" s="66"/>
-      <c r="E14" s="66"/>
-      <c r="F14" s="66"/>
-      <c r="G14" s="66"/>
-      <c r="H14" s="89"/>
-      <c r="I14" s="85"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="95" t="s">
-        <v>49</v>
+      <c r="G13" s="64"/>
+      <c r="H13" s="61"/>
+    </row>
+    <row r="14" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="62"/>
+      <c r="B14" s="59"/>
+      <c r="C14" s="51"/>
+      <c r="D14" s="51"/>
+      <c r="E14" s="51"/>
+      <c r="F14" s="51"/>
+      <c r="G14" s="65"/>
+      <c r="H14" s="62"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="68" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B18" s="93" t="s">
+      <c r="B18" s="78" t="s">
         <v>11</v>
       </c>
-      <c r="C18" s="93"/>
-      <c r="D18" s="93"/>
+      <c r="C18" s="78"/>
+      <c r="D18" s="78"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="92" t="s">
+      <c r="A19" s="67" t="s">
         <v>20</v>
       </c>
-      <c r="B19" s="94" t="s">
+      <c r="B19" s="69" t="s">
         <v>20</v>
       </c>
-      <c r="C19" s="94"/>
-      <c r="D19" s="94"/>
-    </row>
-    <row r="21" spans="1:4" s="64" customFormat="1" x14ac:dyDescent="0.25"/>
+      <c r="C19" s="69"/>
+      <c r="D19" s="69"/>
+    </row>
+    <row r="21" spans="1:4" s="49" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="95" t="s">
-        <v>50</v>
+      <c r="A22" s="68" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -1547,17 +1655,17 @@
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="92" t="s">
+      <c r="A25" s="67" t="s">
         <v>18</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="6">
     <mergeCell ref="B19:D19"/>
-    <mergeCell ref="B3:H3"/>
+    <mergeCell ref="B3:G3"/>
     <mergeCell ref="A3:A4"/>
-    <mergeCell ref="I3:I4"/>
-    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="H3:H4"/>
+    <mergeCell ref="A1:H1"/>
     <mergeCell ref="B18:D18"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1570,7 +1678,7 @@
   <dimension ref="A1:F49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1584,441 +1692,441 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="24" t="s">
+      <c r="C1" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="39" t="s">
+      <c r="D1" s="34" t="s">
         <v>28</v>
       </c>
-      <c r="E1" s="50" t="s">
+      <c r="E1" s="44" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="60" t="s">
+      <c r="A2" s="82" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="20">
+      <c r="C2" s="18">
         <v>1</v>
       </c>
-      <c r="D2" s="40">
+      <c r="D2" s="35">
         <f>((C2/3)*100)</f>
         <v>33.333333333333329</v>
       </c>
-      <c r="E2" s="51">
+      <c r="E2" s="85">
         <f>(AVERAGE(C2:C4))*100</f>
         <v>66.666666666666657</v>
       </c>
       <c r="F2" s="5"/>
     </row>
     <row r="3" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="61"/>
+      <c r="A3" s="83"/>
       <c r="B3" s="8" t="s">
         <v>5</v>
       </c>
       <c r="C3" s="9">
         <v>1</v>
       </c>
-      <c r="D3" s="41">
+      <c r="D3" s="36">
         <f t="shared" ref="D3:D4" si="0">((C3/3)*100)</f>
         <v>33.333333333333329</v>
       </c>
-      <c r="E3" s="52"/>
+      <c r="E3" s="86"/>
       <c r="F3" s="5"/>
     </row>
     <row r="4" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="62"/>
-      <c r="B4" s="21" t="s">
+      <c r="A4" s="84"/>
+      <c r="B4" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="22">
+      <c r="C4" s="20">
         <v>0</v>
       </c>
-      <c r="D4" s="42">
+      <c r="D4" s="37">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E4" s="53"/>
+      <c r="E4" s="87"/>
       <c r="F4" s="5"/>
     </row>
     <row r="5" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="34" t="s">
+      <c r="A5" s="88" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="30" t="s">
+      <c r="B5" s="28" t="s">
         <v>29</v>
       </c>
-      <c r="C5" s="31"/>
-      <c r="D5" s="43">
+      <c r="C5" s="29"/>
+      <c r="D5" s="38">
         <f>(AVERAGE(C6:C13)*100)*0.5</f>
         <v>0</v>
       </c>
-      <c r="E5" s="54">
+      <c r="E5" s="91">
         <f>D5+D14</f>
         <v>0</v>
       </c>
       <c r="F5" s="5"/>
     </row>
     <row r="6" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="36"/>
-      <c r="B6" s="37" t="s">
+      <c r="A6" s="89"/>
+      <c r="B6" s="32" t="s">
         <v>30</v>
       </c>
-      <c r="C6" s="38">
+      <c r="C6" s="33">
         <v>0</v>
       </c>
-      <c r="D6" s="44">
+      <c r="D6" s="39">
         <f>(C6/8)*100</f>
         <v>0</v>
       </c>
-      <c r="E6" s="55"/>
+      <c r="E6" s="92"/>
       <c r="F6" s="5"/>
     </row>
     <row r="7" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="36"/>
-      <c r="B7" s="37" t="s">
+      <c r="A7" s="89"/>
+      <c r="B7" s="32" t="s">
         <v>31</v>
       </c>
-      <c r="C7" s="38">
+      <c r="C7" s="33">
         <v>0</v>
       </c>
-      <c r="D7" s="44">
+      <c r="D7" s="39">
         <f t="shared" ref="D7:D13" si="1">(C7/8)*100</f>
         <v>0</v>
       </c>
-      <c r="E7" s="55"/>
+      <c r="E7" s="92"/>
       <c r="F7" s="5"/>
     </row>
     <row r="8" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="36"/>
-      <c r="B8" s="37" t="s">
+      <c r="A8" s="89"/>
+      <c r="B8" s="32" t="s">
         <v>32</v>
       </c>
-      <c r="C8" s="38">
+      <c r="C8" s="33">
         <v>0</v>
       </c>
-      <c r="D8" s="44">
+      <c r="D8" s="39">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="E8" s="55"/>
+      <c r="E8" s="92"/>
       <c r="F8" s="5"/>
     </row>
     <row r="9" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="36"/>
-      <c r="B9" s="37" t="s">
+      <c r="A9" s="89"/>
+      <c r="B9" s="32" t="s">
         <v>33</v>
       </c>
-      <c r="C9" s="38">
+      <c r="C9" s="33">
         <v>0</v>
       </c>
-      <c r="D9" s="44">
+      <c r="D9" s="39">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="E9" s="55"/>
+      <c r="E9" s="92"/>
       <c r="F9" s="5"/>
     </row>
     <row r="10" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="36"/>
-      <c r="B10" s="37" t="s">
+      <c r="A10" s="89"/>
+      <c r="B10" s="32" t="s">
         <v>34</v>
       </c>
-      <c r="C10" s="38">
+      <c r="C10" s="33">
         <v>0</v>
       </c>
-      <c r="D10" s="44">
+      <c r="D10" s="39">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="E10" s="55"/>
+      <c r="E10" s="92"/>
       <c r="F10" s="5"/>
     </row>
     <row r="11" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="36"/>
-      <c r="B11" s="37" t="s">
+      <c r="A11" s="89"/>
+      <c r="B11" s="32" t="s">
         <v>35</v>
       </c>
-      <c r="C11" s="38">
+      <c r="C11" s="33">
         <v>0</v>
       </c>
-      <c r="D11" s="44">
+      <c r="D11" s="39">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="E11" s="55"/>
+      <c r="E11" s="92"/>
       <c r="F11" s="5"/>
     </row>
     <row r="12" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="36"/>
-      <c r="B12" s="37" t="s">
+      <c r="A12" s="89"/>
+      <c r="B12" s="32" t="s">
         <v>36</v>
       </c>
-      <c r="C12" s="38">
+      <c r="C12" s="33">
         <v>0</v>
       </c>
-      <c r="D12" s="44">
+      <c r="D12" s="39">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="E12" s="55"/>
+      <c r="E12" s="92"/>
       <c r="F12" s="5"/>
     </row>
     <row r="13" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="36"/>
-      <c r="B13" s="37" t="s">
+      <c r="A13" s="89"/>
+      <c r="B13" s="32" t="s">
         <v>37</v>
       </c>
-      <c r="C13" s="38">
+      <c r="C13" s="33">
         <v>0</v>
       </c>
-      <c r="D13" s="44">
+      <c r="D13" s="39">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="E13" s="55"/>
+      <c r="E13" s="92"/>
       <c r="F13" s="5"/>
     </row>
     <row r="14" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="35"/>
-      <c r="B14" s="32" t="s">
+      <c r="A14" s="90"/>
+      <c r="B14" s="30" t="s">
         <v>26</v>
       </c>
-      <c r="C14" s="33">
+      <c r="C14" s="31">
         <v>0</v>
       </c>
-      <c r="D14" s="45">
+      <c r="D14" s="40">
         <f>(C14/2)*100</f>
         <v>0</v>
       </c>
-      <c r="E14" s="56"/>
+      <c r="E14" s="93"/>
       <c r="F14" s="5"/>
     </row>
     <row r="15" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="27"/>
-      <c r="B15" s="28"/>
-      <c r="C15" s="29"/>
-      <c r="D15" s="46"/>
-      <c r="E15" s="57"/>
+      <c r="A15" s="25"/>
+      <c r="B15" s="26"/>
+      <c r="C15" s="27"/>
+      <c r="D15" s="41"/>
+      <c r="E15" s="45"/>
       <c r="F15" s="5"/>
     </row>
     <row r="16" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="25"/>
+      <c r="A16" s="23"/>
       <c r="B16" s="6"/>
       <c r="C16" s="7"/>
-      <c r="D16" s="47"/>
-      <c r="E16" s="58"/>
+      <c r="D16" s="42"/>
+      <c r="E16" s="46"/>
       <c r="F16" s="5"/>
     </row>
     <row r="17" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="25"/>
+      <c r="A17" s="23"/>
       <c r="B17" s="6"/>
       <c r="C17" s="7"/>
-      <c r="D17" s="47"/>
-      <c r="E17" s="58"/>
+      <c r="D17" s="42"/>
+      <c r="E17" s="46"/>
       <c r="F17" s="5"/>
     </row>
     <row r="18" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="25"/>
+      <c r="A18" s="23"/>
       <c r="B18" s="6"/>
       <c r="C18" s="7"/>
-      <c r="D18" s="47"/>
-      <c r="E18" s="58"/>
+      <c r="D18" s="42"/>
+      <c r="E18" s="46"/>
       <c r="F18" s="5"/>
     </row>
     <row r="19" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="25"/>
+      <c r="A19" s="23"/>
       <c r="B19" s="6"/>
       <c r="C19" s="7"/>
-      <c r="D19" s="47"/>
-      <c r="E19" s="58"/>
+      <c r="D19" s="42"/>
+      <c r="E19" s="46"/>
       <c r="F19" s="5"/>
     </row>
     <row r="20" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="25"/>
+      <c r="A20" s="23"/>
       <c r="B20" s="6"/>
       <c r="C20" s="7"/>
-      <c r="D20" s="47"/>
-      <c r="E20" s="58"/>
+      <c r="D20" s="42"/>
+      <c r="E20" s="46"/>
       <c r="F20" s="5"/>
     </row>
     <row r="21" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="25"/>
+      <c r="A21" s="23"/>
       <c r="B21" s="6"/>
       <c r="C21" s="7"/>
-      <c r="D21" s="47"/>
-      <c r="E21" s="58"/>
+      <c r="D21" s="42"/>
+      <c r="E21" s="46"/>
       <c r="F21" s="5"/>
     </row>
     <row r="22" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A22" s="25"/>
+      <c r="A22" s="23"/>
       <c r="B22" s="6"/>
       <c r="C22" s="7"/>
-      <c r="D22" s="47"/>
-      <c r="E22" s="58"/>
+      <c r="D22" s="42"/>
+      <c r="E22" s="46"/>
       <c r="F22" s="5"/>
     </row>
     <row r="23" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A23" s="25"/>
+      <c r="A23" s="23"/>
       <c r="B23" s="6"/>
       <c r="C23" s="7"/>
-      <c r="D23" s="47"/>
-      <c r="E23" s="58"/>
+      <c r="D23" s="42"/>
+      <c r="E23" s="46"/>
       <c r="F23" s="5"/>
     </row>
     <row r="24" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A24" s="25"/>
+      <c r="A24" s="23"/>
       <c r="B24" s="6"/>
       <c r="C24" s="7"/>
-      <c r="D24" s="47"/>
-      <c r="E24" s="58"/>
+      <c r="D24" s="42"/>
+      <c r="E24" s="46"/>
       <c r="F24" s="5"/>
     </row>
     <row r="25" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A25" s="25"/>
+      <c r="A25" s="23"/>
       <c r="B25" s="6"/>
       <c r="C25" s="7"/>
-      <c r="D25" s="47"/>
-      <c r="E25" s="58"/>
+      <c r="D25" s="42"/>
+      <c r="E25" s="46"/>
       <c r="F25" s="5"/>
     </row>
     <row r="26" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A26" s="25"/>
+      <c r="A26" s="23"/>
       <c r="B26" s="6"/>
       <c r="C26" s="7"/>
-      <c r="D26" s="47"/>
-      <c r="E26" s="58"/>
+      <c r="D26" s="42"/>
+      <c r="E26" s="46"/>
       <c r="F26" s="5"/>
     </row>
     <row r="27" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A27" s="25"/>
+      <c r="A27" s="23"/>
       <c r="B27" s="6"/>
       <c r="C27" s="7"/>
-      <c r="D27" s="47"/>
-      <c r="E27" s="58"/>
+      <c r="D27" s="42"/>
+      <c r="E27" s="46"/>
       <c r="F27" s="5"/>
     </row>
     <row r="28" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A28" s="25"/>
+      <c r="A28" s="23"/>
       <c r="B28" s="6"/>
       <c r="C28" s="7"/>
-      <c r="D28" s="47"/>
-      <c r="E28" s="58"/>
+      <c r="D28" s="42"/>
+      <c r="E28" s="46"/>
       <c r="F28" s="5"/>
     </row>
     <row r="29" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A29" s="25"/>
+      <c r="A29" s="23"/>
       <c r="B29" s="6"/>
       <c r="C29" s="7"/>
-      <c r="D29" s="47"/>
-      <c r="E29" s="58"/>
+      <c r="D29" s="42"/>
+      <c r="E29" s="46"/>
       <c r="F29" s="5"/>
     </row>
     <row r="30" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A30" s="25"/>
+      <c r="A30" s="23"/>
       <c r="B30" s="6"/>
       <c r="C30" s="7"/>
-      <c r="D30" s="47"/>
-      <c r="E30" s="58"/>
+      <c r="D30" s="42"/>
+      <c r="E30" s="46"/>
       <c r="F30" s="5"/>
     </row>
     <row r="31" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A31" s="25"/>
+      <c r="A31" s="23"/>
       <c r="B31" s="6"/>
       <c r="C31" s="7"/>
-      <c r="D31" s="47"/>
-      <c r="E31" s="58"/>
+      <c r="D31" s="42"/>
+      <c r="E31" s="46"/>
       <c r="F31" s="5"/>
     </row>
     <row r="32" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A32" s="25"/>
+      <c r="A32" s="23"/>
       <c r="B32" s="6"/>
       <c r="C32" s="7"/>
-      <c r="D32" s="47"/>
-      <c r="E32" s="58"/>
+      <c r="D32" s="42"/>
+      <c r="E32" s="46"/>
       <c r="F32" s="5"/>
     </row>
     <row r="33" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A33" s="25"/>
+      <c r="A33" s="23"/>
       <c r="B33" s="6"/>
       <c r="C33" s="7"/>
-      <c r="D33" s="47"/>
-      <c r="E33" s="58"/>
+      <c r="D33" s="42"/>
+      <c r="E33" s="46"/>
       <c r="F33" s="5"/>
     </row>
     <row r="34" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A34" s="25"/>
+      <c r="A34" s="23"/>
       <c r="B34" s="6"/>
       <c r="C34" s="7"/>
-      <c r="D34" s="47"/>
-      <c r="E34" s="58"/>
+      <c r="D34" s="42"/>
+      <c r="E34" s="46"/>
       <c r="F34" s="5"/>
     </row>
     <row r="35" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A35" s="25"/>
+      <c r="A35" s="23"/>
       <c r="B35" s="6"/>
       <c r="C35" s="7"/>
-      <c r="D35" s="47"/>
-      <c r="E35" s="58"/>
+      <c r="D35" s="42"/>
+      <c r="E35" s="46"/>
       <c r="F35" s="5"/>
     </row>
     <row r="36" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A36" s="25"/>
+      <c r="A36" s="23"/>
       <c r="B36" s="6"/>
       <c r="C36" s="7"/>
-      <c r="D36" s="47"/>
-      <c r="E36" s="58"/>
+      <c r="D36" s="42"/>
+      <c r="E36" s="46"/>
       <c r="F36" s="5"/>
     </row>
     <row r="37" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A37" s="25"/>
+      <c r="A37" s="23"/>
       <c r="B37" s="6"/>
       <c r="C37" s="7"/>
-      <c r="D37" s="47"/>
-      <c r="E37" s="58"/>
+      <c r="D37" s="42"/>
+      <c r="E37" s="46"/>
       <c r="F37" s="5"/>
     </row>
     <row r="38" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A38" s="25"/>
+      <c r="A38" s="23"/>
       <c r="B38" s="6"/>
       <c r="C38" s="7"/>
-      <c r="D38" s="47"/>
-      <c r="E38" s="58"/>
+      <c r="D38" s="42"/>
+      <c r="E38" s="46"/>
       <c r="F38" s="5"/>
     </row>
     <row r="39" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A39" s="25"/>
+      <c r="A39" s="23"/>
       <c r="B39" s="6"/>
       <c r="C39" s="7"/>
-      <c r="D39" s="47"/>
-      <c r="E39" s="58"/>
+      <c r="D39" s="42"/>
+      <c r="E39" s="46"/>
       <c r="F39" s="5"/>
     </row>
     <row r="40" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="26"/>
+      <c r="A40" s="24"/>
       <c r="B40" s="16"/>
       <c r="C40" s="15"/>
-      <c r="D40" s="48"/>
-      <c r="E40" s="59"/>
+      <c r="D40" s="43"/>
+      <c r="E40" s="47"/>
       <c r="F40" s="5"/>
     </row>
     <row r="41" spans="1:6" ht="24" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="17" t="s">
+      <c r="A41" s="79" t="s">
         <v>27</v>
       </c>
-      <c r="B41" s="18"/>
-      <c r="C41" s="18"/>
-      <c r="D41" s="49"/>
-      <c r="E41" s="63">
+      <c r="B41" s="80"/>
+      <c r="C41" s="80"/>
+      <c r="D41" s="81"/>
+      <c r="E41" s="48">
         <f>(AVERAGE(E2,E5))</f>
         <v>33.333333333333329</v>
       </c>
@@ -2106,7 +2214,7 @@
   <dimension ref="B2:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+      <selection activeCell="B3" sqref="B3:B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Second commit - Workplan - Template
</commit_message>
<xml_diff>
--- a/Workplan.xlsx
+++ b/Workplan.xlsx
@@ -151,9 +151,6 @@
   </si>
   <si>
     <t>Status</t>
-  </si>
-  <si>
-    <t>DAY 1 - JULY 14, 2016</t>
   </si>
   <si>
     <t>PROJECT SIMULATION WORKPLAN</t>
@@ -255,6 +252,9 @@
       </rPr>
       <t xml:space="preserve"> Bianca Denise A. Del Puerto   Angela Lynne G. Lapus</t>
     </r>
+  </si>
+  <si>
+    <t>DAY</t>
   </si>
 </sst>
 </file>
@@ -352,7 +352,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="36">
+  <borders count="41">
     <border>
       <left/>
       <right/>
@@ -784,9 +784,7 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
+      <top/>
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
@@ -798,7 +796,7 @@
         <color indexed="64"/>
       </right>
       <top/>
-      <bottom style="medium">
+      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -808,6 +806,56 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
       <top/>
       <bottom style="thin">
         <color indexed="64"/>
@@ -816,22 +864,33 @@
     </border>
     <border>
       <left/>
-      <right style="thin">
+      <right style="medium">
         <color indexed="64"/>
       </right>
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="94">
+  <cellXfs count="101">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -987,16 +1046,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -1005,11 +1055,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
@@ -1032,15 +1079,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1102,6 +1140,44 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1405,268 +1481,345 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H25"/>
+  <dimension ref="A1:I30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="44" customWidth="1"/>
-    <col min="2" max="2" width="11.7109375" customWidth="1"/>
-    <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.140625" customWidth="1"/>
-    <col min="5" max="5" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.42578125" customWidth="1"/>
-    <col min="7" max="7" width="10.85546875" customWidth="1"/>
-    <col min="8" max="8" width="54.5703125" customWidth="1"/>
+    <col min="1" max="1" width="7.42578125" style="49" customWidth="1"/>
+    <col min="2" max="2" width="44" customWidth="1"/>
+    <col min="3" max="3" width="10.28515625" customWidth="1"/>
+    <col min="4" max="4" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.140625" customWidth="1"/>
+    <col min="6" max="6" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.42578125" customWidth="1"/>
+    <col min="8" max="8" width="12.140625" customWidth="1"/>
+    <col min="9" max="9" width="45.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="49" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="77" t="s">
+    <row r="1" spans="1:9" s="49" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B1" s="70" t="s">
+        <v>45</v>
+      </c>
+      <c r="C1" s="70"/>
+      <c r="D1" s="70"/>
+      <c r="E1" s="70"/>
+      <c r="F1" s="70"/>
+      <c r="G1" s="70"/>
+      <c r="H1" s="70"/>
+      <c r="I1" s="70"/>
+    </row>
+    <row r="2" spans="1:9" s="49" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="66" t="s">
+        <v>51</v>
+      </c>
+      <c r="B3" s="93" t="s">
+        <v>38</v>
+      </c>
+      <c r="C3" s="90" t="s">
+        <v>40</v>
+      </c>
+      <c r="D3" s="91" t="s">
+        <v>41</v>
+      </c>
+      <c r="E3" s="91" t="s">
+        <v>42</v>
+      </c>
+      <c r="F3" s="91" t="s">
+        <v>43</v>
+      </c>
+      <c r="G3" s="91" t="s">
+        <v>48</v>
+      </c>
+      <c r="H3" s="92" t="s">
+        <v>44</v>
+      </c>
+      <c r="I3" s="68" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="67"/>
+      <c r="B4" s="94"/>
+      <c r="C4" s="89"/>
+      <c r="D4" s="88"/>
+      <c r="E4" s="88"/>
+      <c r="F4" s="88"/>
+      <c r="G4" s="88"/>
+      <c r="H4" s="87"/>
+      <c r="I4" s="69"/>
+    </row>
+    <row r="5" spans="1:9" ht="83.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="98">
+        <v>1</v>
+      </c>
+      <c r="B5" s="95" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="53">
+        <v>42565</v>
+      </c>
+      <c r="D5" s="53">
+        <v>42565</v>
+      </c>
+      <c r="E5" s="53">
+        <v>42565</v>
+      </c>
+      <c r="F5" s="53">
+        <v>42565</v>
+      </c>
+      <c r="G5" s="52">
+        <v>100</v>
+      </c>
+      <c r="H5" s="59" t="s">
+        <v>49</v>
+      </c>
+      <c r="I5" s="62" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="99"/>
+      <c r="B6" s="96" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="53">
+        <v>42565</v>
+      </c>
+      <c r="D6" s="53">
+        <v>42565</v>
+      </c>
+      <c r="E6" s="53">
+        <v>42565</v>
+      </c>
+      <c r="F6" s="53">
+        <v>42565</v>
+      </c>
+      <c r="G6" s="10">
+        <v>100</v>
+      </c>
+      <c r="H6" s="59" t="s">
+        <v>49</v>
+      </c>
+      <c r="I6" s="57"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="100"/>
+      <c r="B7" s="96" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="53">
+        <v>42565</v>
+      </c>
+      <c r="D7" s="53">
+        <v>42565</v>
+      </c>
+      <c r="E7" s="53">
+        <v>42565</v>
+      </c>
+      <c r="F7" s="53">
+        <v>42565</v>
+      </c>
+      <c r="G7" s="10">
+        <v>100</v>
+      </c>
+      <c r="H7" s="59" t="s">
+        <v>49</v>
+      </c>
+      <c r="I7" s="57"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="57"/>
+      <c r="B8" s="96"/>
+      <c r="C8" s="54"/>
+      <c r="D8" s="50"/>
+      <c r="E8" s="50"/>
+      <c r="F8" s="10"/>
+      <c r="G8" s="10"/>
+      <c r="H8" s="60"/>
+      <c r="I8" s="57"/>
+    </row>
+    <row r="9" spans="1:9" s="49" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="57"/>
+      <c r="B9" s="96"/>
+      <c r="C9" s="54"/>
+      <c r="D9" s="50"/>
+      <c r="E9" s="50"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="60"/>
+      <c r="I9" s="57"/>
+    </row>
+    <row r="10" spans="1:9" s="49" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="57"/>
+      <c r="B10" s="96"/>
+      <c r="C10" s="54"/>
+      <c r="D10" s="50"/>
+      <c r="E10" s="50"/>
+      <c r="F10" s="10"/>
+      <c r="G10" s="10"/>
+      <c r="H10" s="60"/>
+      <c r="I10" s="57"/>
+    </row>
+    <row r="11" spans="1:9" s="49" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="57"/>
+      <c r="B11" s="96"/>
+      <c r="C11" s="54"/>
+      <c r="D11" s="50"/>
+      <c r="E11" s="50"/>
+      <c r="F11" s="10"/>
+      <c r="G11" s="10"/>
+      <c r="H11" s="60"/>
+      <c r="I11" s="57"/>
+    </row>
+    <row r="12" spans="1:9" s="49" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="57"/>
+      <c r="B12" s="96"/>
+      <c r="C12" s="54"/>
+      <c r="D12" s="50"/>
+      <c r="E12" s="50"/>
+      <c r="F12" s="10"/>
+      <c r="G12" s="10"/>
+      <c r="H12" s="60"/>
+      <c r="I12" s="57"/>
+    </row>
+    <row r="13" spans="1:9" s="49" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="57"/>
+      <c r="B13" s="96"/>
+      <c r="C13" s="54"/>
+      <c r="D13" s="50"/>
+      <c r="E13" s="50"/>
+      <c r="F13" s="10"/>
+      <c r="G13" s="10"/>
+      <c r="H13" s="60"/>
+      <c r="I13" s="57"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="57"/>
+      <c r="B14" s="96"/>
+      <c r="C14" s="55"/>
+      <c r="D14" s="10"/>
+      <c r="E14" s="10"/>
+      <c r="F14" s="10"/>
+      <c r="G14" s="10"/>
+      <c r="H14" s="60"/>
+      <c r="I14" s="57"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="57"/>
+      <c r="B15" s="96"/>
+      <c r="C15" s="55"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="10"/>
+      <c r="F15" s="10"/>
+      <c r="G15" s="10"/>
+      <c r="H15" s="60"/>
+      <c r="I15" s="57"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="57"/>
+      <c r="B16" s="96"/>
+      <c r="C16" s="55"/>
+      <c r="D16" s="10"/>
+      <c r="E16" s="10"/>
+      <c r="F16" s="10"/>
+      <c r="G16" s="10"/>
+      <c r="H16" s="60"/>
+      <c r="I16" s="57"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="57"/>
+      <c r="B17" s="96"/>
+      <c r="C17" s="55"/>
+      <c r="D17" s="10"/>
+      <c r="E17" s="10"/>
+      <c r="F17" s="10"/>
+      <c r="G17" s="10"/>
+      <c r="H17" s="60"/>
+      <c r="I17" s="57"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="57"/>
+      <c r="B18" s="96"/>
+      <c r="C18" s="55"/>
+      <c r="D18" s="10"/>
+      <c r="E18" s="10"/>
+      <c r="F18" s="10"/>
+      <c r="G18" s="10"/>
+      <c r="H18" s="60"/>
+      <c r="I18" s="57"/>
+    </row>
+    <row r="19" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="58"/>
+      <c r="B19" s="97"/>
+      <c r="C19" s="56"/>
+      <c r="D19" s="51"/>
+      <c r="E19" s="51"/>
+      <c r="F19" s="51"/>
+      <c r="G19" s="51"/>
+      <c r="H19" s="61"/>
+      <c r="I19" s="58"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B21" s="64" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="77"/>
-      <c r="C1" s="77"/>
-      <c r="D1" s="77"/>
-      <c r="E1" s="77"/>
-      <c r="F1" s="77"/>
-      <c r="G1" s="77"/>
-      <c r="H1" s="77"/>
-    </row>
-    <row r="2" spans="1:8" s="49" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="73" t="s">
-        <v>38</v>
-      </c>
-      <c r="B3" s="70" t="s">
-        <v>45</v>
-      </c>
-      <c r="C3" s="71"/>
-      <c r="D3" s="71"/>
-      <c r="E3" s="71"/>
-      <c r="F3" s="71"/>
-      <c r="G3" s="72"/>
-      <c r="H3" s="75" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="74"/>
-      <c r="B4" s="55" t="s">
-        <v>40</v>
-      </c>
-      <c r="C4" s="53" t="s">
-        <v>41</v>
-      </c>
-      <c r="D4" s="53" t="s">
-        <v>42</v>
-      </c>
-      <c r="E4" s="53" t="s">
-        <v>43</v>
-      </c>
-      <c r="F4" s="53" t="s">
-        <v>49</v>
-      </c>
-      <c r="G4" s="54" t="s">
-        <v>44</v>
-      </c>
-      <c r="H4" s="76"/>
-    </row>
-    <row r="5" spans="1:8" ht="83.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="60" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="56">
-        <v>42565</v>
-      </c>
-      <c r="C5" s="56">
-        <v>42565</v>
-      </c>
-      <c r="D5" s="56">
-        <v>42565</v>
-      </c>
-      <c r="E5" s="56">
-        <v>42565</v>
-      </c>
-      <c r="F5" s="52">
-        <v>100</v>
-      </c>
-      <c r="G5" s="63" t="s">
-        <v>50</v>
-      </c>
-      <c r="H5" s="66" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="61" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" s="56">
-        <v>42565</v>
-      </c>
-      <c r="C6" s="56">
-        <v>42565</v>
-      </c>
-      <c r="D6" s="56">
-        <v>42565</v>
-      </c>
-      <c r="E6" s="56">
-        <v>42565</v>
-      </c>
-      <c r="F6" s="10">
-        <v>100</v>
-      </c>
-      <c r="G6" s="63" t="s">
-        <v>50</v>
-      </c>
-      <c r="H6" s="61"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="61" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="56">
-        <v>42565</v>
-      </c>
-      <c r="C7" s="56">
-        <v>42565</v>
-      </c>
-      <c r="D7" s="56">
-        <v>42565</v>
-      </c>
-      <c r="E7" s="56">
-        <v>42565</v>
-      </c>
-      <c r="F7" s="10">
-        <v>100</v>
-      </c>
-      <c r="G7" s="63" t="s">
-        <v>50</v>
-      </c>
-      <c r="H7" s="61"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="61"/>
-      <c r="B8" s="57"/>
-      <c r="C8" s="50"/>
-      <c r="D8" s="50"/>
-      <c r="E8" s="10"/>
-      <c r="F8" s="10"/>
-      <c r="G8" s="64"/>
-      <c r="H8" s="61"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="61"/>
-      <c r="B9" s="58"/>
-      <c r="C9" s="10"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="10"/>
-      <c r="F9" s="10"/>
-      <c r="G9" s="64"/>
-      <c r="H9" s="61"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="61"/>
-      <c r="B10" s="58"/>
-      <c r="C10" s="10"/>
-      <c r="D10" s="10"/>
-      <c r="E10" s="10"/>
-      <c r="F10" s="10"/>
-      <c r="G10" s="64"/>
-      <c r="H10" s="61"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="61"/>
-      <c r="B11" s="58"/>
-      <c r="C11" s="10"/>
-      <c r="D11" s="10"/>
-      <c r="E11" s="10"/>
-      <c r="F11" s="10"/>
-      <c r="G11" s="64"/>
-      <c r="H11" s="61"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="61"/>
-      <c r="B12" s="58"/>
-      <c r="C12" s="10"/>
-      <c r="D12" s="10"/>
-      <c r="E12" s="10"/>
-      <c r="F12" s="10"/>
-      <c r="G12" s="64"/>
-      <c r="H12" s="61"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="61"/>
-      <c r="B13" s="58"/>
-      <c r="C13" s="10"/>
-      <c r="D13" s="10"/>
-      <c r="E13" s="10"/>
-      <c r="F13" s="10"/>
-      <c r="G13" s="64"/>
-      <c r="H13" s="61"/>
-    </row>
-    <row r="14" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="62"/>
-      <c r="B14" s="59"/>
-      <c r="C14" s="51"/>
-      <c r="D14" s="51"/>
-      <c r="E14" s="51"/>
-      <c r="F14" s="51"/>
-      <c r="G14" s="65"/>
-      <c r="H14" s="62"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="68" t="s">
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B23" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C23" s="71" t="s">
+        <v>11</v>
+      </c>
+      <c r="D23" s="71"/>
+      <c r="E23" s="71"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B24" s="63" t="s">
+        <v>20</v>
+      </c>
+      <c r="C24" s="65" t="s">
+        <v>20</v>
+      </c>
+      <c r="D24" s="65"/>
+      <c r="E24" s="65"/>
+    </row>
+    <row r="26" spans="1:9" s="49" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B27" s="64" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B18" s="78" t="s">
-        <v>11</v>
-      </c>
-      <c r="C18" s="78"/>
-      <c r="D18" s="78"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="67" t="s">
-        <v>20</v>
-      </c>
-      <c r="B19" s="69" t="s">
-        <v>20</v>
-      </c>
-      <c r="C19" s="69"/>
-      <c r="D19" s="69"/>
-    </row>
-    <row r="21" spans="1:4" s="49" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="68" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B29" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="67" t="s">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B30" s="63" t="s">
         <v>18</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="B19:D19"/>
-    <mergeCell ref="B3:G3"/>
+  <mergeCells count="13">
     <mergeCell ref="A3:A4"/>
+    <mergeCell ref="A5:A7"/>
+    <mergeCell ref="C24:E24"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="I3:I4"/>
+    <mergeCell ref="B1:I1"/>
+    <mergeCell ref="C23:E23"/>
     <mergeCell ref="H3:H4"/>
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="B18:D18"/>
+    <mergeCell ref="G3:G4"/>
+    <mergeCell ref="F3:F4"/>
+    <mergeCell ref="E3:E4"/>
+    <mergeCell ref="D3:D4"/>
+    <mergeCell ref="C3:C4"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="5" orientation="landscape" r:id="rId1"/>
@@ -1709,7 +1862,7 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="82" t="s">
+      <c r="A2" s="75" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="17" t="s">
@@ -1722,14 +1875,14 @@
         <f>((C2/3)*100)</f>
         <v>33.333333333333329</v>
       </c>
-      <c r="E2" s="85">
+      <c r="E2" s="78">
         <f>(AVERAGE(C2:C4))*100</f>
         <v>66.666666666666657</v>
       </c>
       <c r="F2" s="5"/>
     </row>
     <row r="3" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="83"/>
+      <c r="A3" s="76"/>
       <c r="B3" s="8" t="s">
         <v>5</v>
       </c>
@@ -1740,11 +1893,11 @@
         <f t="shared" ref="D3:D4" si="0">((C3/3)*100)</f>
         <v>33.333333333333329</v>
       </c>
-      <c r="E3" s="86"/>
+      <c r="E3" s="79"/>
       <c r="F3" s="5"/>
     </row>
     <row r="4" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="84"/>
+      <c r="A4" s="77"/>
       <c r="B4" s="19" t="s">
         <v>6</v>
       </c>
@@ -1755,11 +1908,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E4" s="87"/>
+      <c r="E4" s="80"/>
       <c r="F4" s="5"/>
     </row>
     <row r="5" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="88" t="s">
+      <c r="A5" s="81" t="s">
         <v>7</v>
       </c>
       <c r="B5" s="28" t="s">
@@ -1770,14 +1923,14 @@
         <f>(AVERAGE(C6:C13)*100)*0.5</f>
         <v>0</v>
       </c>
-      <c r="E5" s="91">
+      <c r="E5" s="84">
         <f>D5+D14</f>
         <v>0</v>
       </c>
       <c r="F5" s="5"/>
     </row>
     <row r="6" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="89"/>
+      <c r="A6" s="82"/>
       <c r="B6" s="32" t="s">
         <v>30</v>
       </c>
@@ -1788,11 +1941,11 @@
         <f>(C6/8)*100</f>
         <v>0</v>
       </c>
-      <c r="E6" s="92"/>
+      <c r="E6" s="85"/>
       <c r="F6" s="5"/>
     </row>
     <row r="7" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="89"/>
+      <c r="A7" s="82"/>
       <c r="B7" s="32" t="s">
         <v>31</v>
       </c>
@@ -1803,11 +1956,11 @@
         <f t="shared" ref="D7:D13" si="1">(C7/8)*100</f>
         <v>0</v>
       </c>
-      <c r="E7" s="92"/>
+      <c r="E7" s="85"/>
       <c r="F7" s="5"/>
     </row>
     <row r="8" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="89"/>
+      <c r="A8" s="82"/>
       <c r="B8" s="32" t="s">
         <v>32</v>
       </c>
@@ -1818,11 +1971,11 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="E8" s="92"/>
+      <c r="E8" s="85"/>
       <c r="F8" s="5"/>
     </row>
     <row r="9" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="89"/>
+      <c r="A9" s="82"/>
       <c r="B9" s="32" t="s">
         <v>33</v>
       </c>
@@ -1833,11 +1986,11 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="E9" s="92"/>
+      <c r="E9" s="85"/>
       <c r="F9" s="5"/>
     </row>
     <row r="10" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="89"/>
+      <c r="A10" s="82"/>
       <c r="B10" s="32" t="s">
         <v>34</v>
       </c>
@@ -1848,11 +2001,11 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="E10" s="92"/>
+      <c r="E10" s="85"/>
       <c r="F10" s="5"/>
     </row>
     <row r="11" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="89"/>
+      <c r="A11" s="82"/>
       <c r="B11" s="32" t="s">
         <v>35</v>
       </c>
@@ -1863,11 +2016,11 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="E11" s="92"/>
+      <c r="E11" s="85"/>
       <c r="F11" s="5"/>
     </row>
     <row r="12" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="89"/>
+      <c r="A12" s="82"/>
       <c r="B12" s="32" t="s">
         <v>36</v>
       </c>
@@ -1878,11 +2031,11 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="E12" s="92"/>
+      <c r="E12" s="85"/>
       <c r="F12" s="5"/>
     </row>
     <row r="13" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="89"/>
+      <c r="A13" s="82"/>
       <c r="B13" s="32" t="s">
         <v>37</v>
       </c>
@@ -1893,11 +2046,11 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="E13" s="92"/>
+      <c r="E13" s="85"/>
       <c r="F13" s="5"/>
     </row>
     <row r="14" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="90"/>
+      <c r="A14" s="83"/>
       <c r="B14" s="30" t="s">
         <v>26</v>
       </c>
@@ -1908,7 +2061,7 @@
         <f>(C14/2)*100</f>
         <v>0</v>
       </c>
-      <c r="E14" s="93"/>
+      <c r="E14" s="86"/>
       <c r="F14" s="5"/>
     </row>
     <row r="15" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -2120,12 +2273,12 @@
       <c r="F40" s="5"/>
     </row>
     <row r="41" spans="1:6" ht="24" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="79" t="s">
+      <c r="A41" s="72" t="s">
         <v>27</v>
       </c>
-      <c r="B41" s="80"/>
-      <c r="C41" s="80"/>
-      <c r="D41" s="81"/>
+      <c r="B41" s="73"/>
+      <c r="C41" s="73"/>
+      <c r="D41" s="74"/>
       <c r="E41" s="48">
         <f>(AVERAGE(E2,E5))</f>
         <v>33.333333333333329</v>

</xml_diff>

<commit_message>
Third Commit - Workplan
</commit_message>
<xml_diff>
--- a/Workplan.xlsx
+++ b/Workplan.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="55">
   <si>
     <t>ACTIVITIES</t>
   </si>
@@ -256,12 +256,21 @@
   <si>
     <t>DAY</t>
   </si>
+  <si>
+    <t>Code Development</t>
+  </si>
+  <si>
+    <t>Javascript Calculator</t>
+  </si>
+  <si>
+    <t>CI-CD</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -307,8 +316,30 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -351,8 +382,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="41">
+  <borders count="29">
     <border>
       <left/>
       <right/>
@@ -415,19 +458,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
@@ -752,137 +782,6 @@
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
       <bottom/>
       <diagonal/>
     </border>
@@ -890,7 +789,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="101">
+  <cellXfs count="87">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -940,31 +839,31 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -973,16 +872,16 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -991,195 +890,153 @@
     <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="2" fontId="3" fillId="3" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="2" fontId="3" fillId="3" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="3" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="3" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="5" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="3" fillId="5" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="3" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="3" fillId="5" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="3" fillId="5" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="6" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="3" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="3" fillId="3" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="3" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="3" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="3" fillId="3" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="3" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="3" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="3" fillId="5" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="3" fillId="5" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="6" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="4"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1481,10 +1338,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I30"/>
+  <dimension ref="A1:I72"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1501,319 +1358,520 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="49" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B1" s="70" t="s">
+      <c r="B1" s="53" t="s">
         <v>45</v>
       </c>
-      <c r="C1" s="70"/>
-      <c r="D1" s="70"/>
-      <c r="E1" s="70"/>
-      <c r="F1" s="70"/>
-      <c r="G1" s="70"/>
-      <c r="H1" s="70"/>
-      <c r="I1" s="70"/>
-    </row>
-    <row r="2" spans="1:9" s="49" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+      <c r="C1" s="53"/>
+      <c r="D1" s="53"/>
+      <c r="E1" s="53"/>
+      <c r="F1" s="53"/>
+      <c r="G1" s="53"/>
+      <c r="H1" s="53"/>
+      <c r="I1" s="53"/>
+    </row>
+    <row r="2" spans="1:9" s="49" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="66" t="s">
+      <c r="A3" s="74" t="s">
         <v>51</v>
       </c>
-      <c r="B3" s="93" t="s">
+      <c r="B3" s="74" t="s">
         <v>38</v>
       </c>
-      <c r="C3" s="90" t="s">
+      <c r="C3" s="75" t="s">
         <v>40</v>
       </c>
-      <c r="D3" s="91" t="s">
+      <c r="D3" s="75" t="s">
         <v>41</v>
       </c>
-      <c r="E3" s="91" t="s">
+      <c r="E3" s="75" t="s">
         <v>42</v>
       </c>
-      <c r="F3" s="91" t="s">
+      <c r="F3" s="75" t="s">
         <v>43</v>
       </c>
-      <c r="G3" s="91" t="s">
+      <c r="G3" s="75" t="s">
         <v>48</v>
       </c>
-      <c r="H3" s="92" t="s">
+      <c r="H3" s="75" t="s">
         <v>44</v>
       </c>
-      <c r="I3" s="68" t="s">
+      <c r="I3" s="75" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="67"/>
-      <c r="B4" s="94"/>
-      <c r="C4" s="89"/>
-      <c r="D4" s="88"/>
-      <c r="E4" s="88"/>
-      <c r="F4" s="88"/>
-      <c r="G4" s="88"/>
-      <c r="H4" s="87"/>
-      <c r="I4" s="69"/>
-    </row>
-    <row r="5" spans="1:9" ht="83.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="98">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="74"/>
+      <c r="B4" s="74"/>
+      <c r="C4" s="75"/>
+      <c r="D4" s="75"/>
+      <c r="E4" s="75"/>
+      <c r="F4" s="75"/>
+      <c r="G4" s="75"/>
+      <c r="H4" s="75"/>
+      <c r="I4" s="75"/>
+    </row>
+    <row r="5" spans="1:9" s="49" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="71">
         <v>1</v>
       </c>
-      <c r="B5" s="95" t="s">
+      <c r="B5" s="84" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="78"/>
+      <c r="D5" s="78"/>
+      <c r="E5" s="78"/>
+      <c r="F5" s="78"/>
+      <c r="G5" s="78"/>
+      <c r="H5" s="78"/>
+      <c r="I5" s="78"/>
+    </row>
+    <row r="6" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="A6" s="71"/>
+      <c r="B6" s="77" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="53">
-        <v>42565</v>
-      </c>
-      <c r="D5" s="53">
-        <v>42565</v>
-      </c>
-      <c r="E5" s="53">
-        <v>42565</v>
-      </c>
-      <c r="F5" s="53">
-        <v>42565</v>
-      </c>
-      <c r="G5" s="52">
-        <v>100</v>
-      </c>
-      <c r="H5" s="59" t="s">
-        <v>49</v>
-      </c>
-      <c r="I5" s="62" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="99"/>
-      <c r="B6" s="96" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" s="53">
-        <v>42565</v>
-      </c>
-      <c r="D6" s="53">
-        <v>42565</v>
-      </c>
-      <c r="E6" s="53">
-        <v>42565</v>
-      </c>
-      <c r="F6" s="53">
+      <c r="C6" s="50">
+        <v>42565</v>
+      </c>
+      <c r="D6" s="50">
+        <v>42565</v>
+      </c>
+      <c r="E6" s="50">
+        <v>42565</v>
+      </c>
+      <c r="F6" s="50">
         <v>42565</v>
       </c>
       <c r="G6" s="10">
         <v>100</v>
       </c>
-      <c r="H6" s="59" t="s">
+      <c r="H6" s="50" t="s">
         <v>49</v>
       </c>
-      <c r="I6" s="57"/>
+      <c r="I6" s="76" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="100"/>
-      <c r="B7" s="96" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" s="53">
-        <v>42565</v>
-      </c>
-      <c r="D7" s="53">
-        <v>42565</v>
-      </c>
-      <c r="E7" s="53">
-        <v>42565</v>
-      </c>
-      <c r="F7" s="53">
+      <c r="A7" s="71"/>
+      <c r="B7" s="73" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="50">
+        <v>42565</v>
+      </c>
+      <c r="D7" s="50">
+        <v>42565</v>
+      </c>
+      <c r="E7" s="50">
+        <v>42565</v>
+      </c>
+      <c r="F7" s="50">
         <v>42565</v>
       </c>
       <c r="G7" s="10">
         <v>100</v>
       </c>
-      <c r="H7" s="59" t="s">
+      <c r="H7" s="50" t="s">
         <v>49</v>
       </c>
-      <c r="I7" s="57"/>
+      <c r="I7" s="72"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="57"/>
-      <c r="B8" s="96"/>
-      <c r="C8" s="54"/>
-      <c r="D8" s="50"/>
-      <c r="E8" s="50"/>
-      <c r="F8" s="10"/>
-      <c r="G8" s="10"/>
-      <c r="H8" s="60"/>
-      <c r="I8" s="57"/>
-    </row>
-    <row r="9" spans="1:9" s="49" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="57"/>
-      <c r="B9" s="96"/>
-      <c r="C9" s="54"/>
-      <c r="D9" s="50"/>
-      <c r="E9" s="50"/>
-      <c r="F9" s="10"/>
-      <c r="G9" s="10"/>
-      <c r="H9" s="60"/>
-      <c r="I9" s="57"/>
-    </row>
-    <row r="10" spans="1:9" s="49" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="57"/>
-      <c r="B10" s="96"/>
-      <c r="C10" s="54"/>
-      <c r="D10" s="50"/>
+      <c r="A8" s="71"/>
+      <c r="B8" s="73" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="50">
+        <v>42565</v>
+      </c>
+      <c r="D8" s="50">
+        <v>42565</v>
+      </c>
+      <c r="E8" s="50">
+        <v>42565</v>
+      </c>
+      <c r="F8" s="50">
+        <v>42565</v>
+      </c>
+      <c r="G8" s="10">
+        <v>100</v>
+      </c>
+      <c r="H8" s="50" t="s">
+        <v>49</v>
+      </c>
+      <c r="I8" s="72"/>
+    </row>
+    <row r="9" spans="1:9" s="83" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="71"/>
+      <c r="B9" s="85" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="79"/>
+      <c r="D9" s="79"/>
+      <c r="E9" s="79"/>
+      <c r="F9" s="79"/>
+      <c r="G9" s="80"/>
+      <c r="H9" s="79"/>
+      <c r="I9" s="81"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="71"/>
+      <c r="B10" s="73" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10" s="50">
+        <v>42565</v>
+      </c>
+      <c r="D10" s="50">
+        <v>42565</v>
+      </c>
       <c r="E10" s="50"/>
       <c r="F10" s="10"/>
       <c r="G10" s="10"/>
-      <c r="H10" s="60"/>
-      <c r="I10" s="57"/>
+      <c r="H10" s="10"/>
+      <c r="I10" s="72"/>
     </row>
     <row r="11" spans="1:9" s="49" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="57"/>
-      <c r="B11" s="96"/>
-      <c r="C11" s="54"/>
-      <c r="D11" s="50"/>
+      <c r="A11" s="71"/>
+      <c r="B11" s="82" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11" s="50">
+        <v>42565</v>
+      </c>
+      <c r="D11" s="50">
+        <v>42565</v>
+      </c>
       <c r="E11" s="50"/>
       <c r="F11" s="10"/>
       <c r="G11" s="10"/>
-      <c r="H11" s="60"/>
-      <c r="I11" s="57"/>
+      <c r="H11" s="10"/>
+      <c r="I11" s="72"/>
     </row>
     <row r="12" spans="1:9" s="49" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="57"/>
-      <c r="B12" s="96"/>
-      <c r="C12" s="54"/>
-      <c r="D12" s="50"/>
+      <c r="A12" s="71"/>
+      <c r="B12" s="82" t="s">
+        <v>31</v>
+      </c>
+      <c r="C12" s="50">
+        <v>42565</v>
+      </c>
+      <c r="D12" s="50">
+        <v>42565</v>
+      </c>
       <c r="E12" s="50"/>
       <c r="F12" s="10"/>
       <c r="G12" s="10"/>
-      <c r="H12" s="60"/>
-      <c r="I12" s="57"/>
-    </row>
-    <row r="13" spans="1:9" s="49" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="57"/>
-      <c r="B13" s="96"/>
-      <c r="C13" s="54"/>
-      <c r="D13" s="50"/>
-      <c r="E13" s="50"/>
+      <c r="H12" s="10"/>
+      <c r="I12" s="72"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="71"/>
+      <c r="B13" s="82" t="s">
+        <v>35</v>
+      </c>
+      <c r="C13" s="50">
+        <v>42565</v>
+      </c>
+      <c r="D13" s="50">
+        <v>42565</v>
+      </c>
+      <c r="E13" s="10"/>
       <c r="F13" s="10"/>
       <c r="G13" s="10"/>
-      <c r="H13" s="60"/>
-      <c r="I13" s="57"/>
+      <c r="H13" s="10"/>
+      <c r="I13" s="72"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="57"/>
-      <c r="B14" s="96"/>
-      <c r="C14" s="55"/>
-      <c r="D14" s="10"/>
+      <c r="A14" s="71"/>
+      <c r="B14" s="82" t="s">
+        <v>36</v>
+      </c>
+      <c r="C14" s="50">
+        <v>42565</v>
+      </c>
+      <c r="D14" s="50">
+        <v>42565</v>
+      </c>
       <c r="E14" s="10"/>
       <c r="F14" s="10"/>
       <c r="G14" s="10"/>
-      <c r="H14" s="60"/>
-      <c r="I14" s="57"/>
+      <c r="H14" s="10"/>
+      <c r="I14" s="72"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="57"/>
-      <c r="B15" s="96"/>
-      <c r="C15" s="55"/>
-      <c r="D15" s="10"/>
+      <c r="A15" s="71"/>
+      <c r="B15" s="82" t="s">
+        <v>37</v>
+      </c>
+      <c r="C15" s="50">
+        <v>42565</v>
+      </c>
+      <c r="D15" s="50">
+        <v>42565</v>
+      </c>
       <c r="E15" s="10"/>
       <c r="F15" s="10"/>
       <c r="G15" s="10"/>
-      <c r="H15" s="60"/>
-      <c r="I15" s="57"/>
+      <c r="H15" s="10"/>
+      <c r="I15" s="72"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="57"/>
-      <c r="B16" s="96"/>
-      <c r="C16" s="55"/>
-      <c r="D16" s="10"/>
+      <c r="A16" s="71"/>
+      <c r="B16" s="73" t="s">
+        <v>26</v>
+      </c>
+      <c r="C16" s="50">
+        <v>42565</v>
+      </c>
+      <c r="D16" s="50">
+        <v>42565</v>
+      </c>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="60"/>
-      <c r="I16" s="57"/>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="57"/>
-      <c r="B17" s="96"/>
-      <c r="C17" s="55"/>
-      <c r="D17" s="10"/>
-      <c r="E17" s="10"/>
-      <c r="F17" s="10"/>
-      <c r="G17" s="10"/>
-      <c r="H17" s="60"/>
-      <c r="I17" s="57"/>
+      <c r="H16" s="10"/>
+      <c r="I16" s="72"/>
+    </row>
+    <row r="17" spans="1:9" s="83" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A17" s="71"/>
+      <c r="B17" s="86" t="s">
+        <v>52</v>
+      </c>
+      <c r="C17" s="79"/>
+      <c r="D17" s="79"/>
+      <c r="E17" s="80"/>
+      <c r="F17" s="80"/>
+      <c r="G17" s="80"/>
+      <c r="H17" s="80"/>
+      <c r="I17" s="81"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="57"/>
-      <c r="B18" s="96"/>
-      <c r="C18" s="55"/>
-      <c r="D18" s="10"/>
+      <c r="A18" s="71"/>
+      <c r="B18" s="72" t="s">
+        <v>53</v>
+      </c>
+      <c r="C18" s="50">
+        <v>42565</v>
+      </c>
+      <c r="D18" s="50">
+        <v>42565</v>
+      </c>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="60"/>
-      <c r="I18" s="57"/>
-    </row>
-    <row r="19" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="58"/>
-      <c r="B19" s="97"/>
-      <c r="C19" s="56"/>
-      <c r="D19" s="51"/>
-      <c r="E19" s="51"/>
-      <c r="F19" s="51"/>
-      <c r="G19" s="51"/>
-      <c r="H19" s="61"/>
-      <c r="I19" s="58"/>
+      <c r="H18" s="10"/>
+      <c r="I18" s="72"/>
+    </row>
+    <row r="19" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A19" s="11"/>
+      <c r="B19" s="86" t="s">
+        <v>54</v>
+      </c>
+      <c r="C19" s="80"/>
+      <c r="D19" s="80"/>
+      <c r="E19" s="80"/>
+      <c r="F19" s="80"/>
+      <c r="G19" s="80"/>
+      <c r="H19" s="80"/>
+      <c r="I19" s="81"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B20" s="72"/>
+      <c r="C20" s="72"/>
+      <c r="D20" s="72"/>
+      <c r="E20" s="72"/>
+      <c r="F20" s="72"/>
+      <c r="G20" s="72"/>
+      <c r="H20" s="72"/>
+      <c r="I20" s="72"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B21" s="64" t="s">
+      <c r="B21" s="72"/>
+      <c r="C21" s="72"/>
+      <c r="D21" s="72"/>
+      <c r="E21" s="72"/>
+      <c r="F21" s="72"/>
+      <c r="G21" s="72"/>
+      <c r="H21" s="72"/>
+      <c r="I21" s="72"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B22" s="72"/>
+      <c r="C22" s="72"/>
+      <c r="D22" s="72"/>
+      <c r="E22" s="72"/>
+      <c r="F22" s="72"/>
+      <c r="G22" s="72"/>
+      <c r="H22" s="72"/>
+      <c r="I22" s="72"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B23" s="72"/>
+      <c r="C23" s="72"/>
+      <c r="D23" s="72"/>
+      <c r="E23" s="72"/>
+      <c r="F23" s="72"/>
+      <c r="G23" s="72"/>
+      <c r="H23" s="72"/>
+      <c r="I23" s="72"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B24" s="72"/>
+      <c r="C24" s="72"/>
+      <c r="D24" s="72"/>
+      <c r="E24" s="72"/>
+      <c r="F24" s="72"/>
+      <c r="G24" s="72"/>
+      <c r="H24" s="72"/>
+      <c r="I24" s="72"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B25" s="72"/>
+      <c r="C25" s="72"/>
+      <c r="D25" s="72"/>
+      <c r="E25" s="72"/>
+      <c r="F25" s="72"/>
+      <c r="G25" s="72"/>
+      <c r="H25" s="72"/>
+      <c r="I25" s="72"/>
+    </row>
+    <row r="26" spans="1:9" s="49" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B26" s="72"/>
+      <c r="C26" s="72"/>
+      <c r="D26" s="72"/>
+      <c r="E26" s="72"/>
+      <c r="F26" s="72"/>
+      <c r="G26" s="72"/>
+      <c r="H26" s="72"/>
+      <c r="I26" s="72"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B27" s="72"/>
+      <c r="C27" s="72"/>
+      <c r="D27" s="72"/>
+      <c r="E27" s="72"/>
+      <c r="F27" s="72"/>
+      <c r="G27" s="72"/>
+      <c r="H27" s="72"/>
+      <c r="I27" s="72"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B28" s="72"/>
+      <c r="C28" s="72"/>
+      <c r="D28" s="72"/>
+      <c r="E28" s="72"/>
+      <c r="F28" s="72"/>
+      <c r="G28" s="72"/>
+      <c r="H28" s="72"/>
+      <c r="I28" s="72"/>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B29" s="72"/>
+      <c r="C29" s="72"/>
+      <c r="D29" s="72"/>
+      <c r="E29" s="72"/>
+      <c r="F29" s="72"/>
+      <c r="G29" s="72"/>
+      <c r="H29" s="72"/>
+      <c r="I29" s="72"/>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B30" s="72"/>
+      <c r="C30" s="72"/>
+      <c r="D30" s="72"/>
+      <c r="E30" s="72"/>
+      <c r="F30" s="72"/>
+      <c r="G30" s="72"/>
+      <c r="H30" s="72"/>
+      <c r="I30" s="72"/>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B31" s="72"/>
+      <c r="C31" s="72"/>
+      <c r="D31" s="72"/>
+      <c r="E31" s="72"/>
+      <c r="F31" s="72"/>
+      <c r="G31" s="72"/>
+      <c r="H31" s="72"/>
+      <c r="I31" s="72"/>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B32" s="72"/>
+      <c r="C32" s="72"/>
+      <c r="D32" s="72"/>
+      <c r="E32" s="72"/>
+      <c r="F32" s="72"/>
+      <c r="G32" s="72"/>
+      <c r="H32" s="72"/>
+      <c r="I32" s="72"/>
+    </row>
+    <row r="33" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B33" s="72"/>
+      <c r="C33" s="72"/>
+      <c r="D33" s="72"/>
+      <c r="E33" s="72"/>
+      <c r="F33" s="72"/>
+      <c r="G33" s="72"/>
+      <c r="H33" s="72"/>
+      <c r="I33" s="72"/>
+    </row>
+    <row r="63" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B63" s="52" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B23" s="2" t="s">
+    <row r="65" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B65" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C23" s="71" t="s">
+      <c r="C65" s="54" t="s">
         <v>11</v>
       </c>
-      <c r="D23" s="71"/>
-      <c r="E23" s="71"/>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B24" s="63" t="s">
+      <c r="D65" s="54"/>
+      <c r="E65" s="54"/>
+    </row>
+    <row r="66" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B66" s="51" t="s">
         <v>20</v>
       </c>
-      <c r="C24" s="65" t="s">
+      <c r="C66" s="55" t="s">
         <v>20</v>
       </c>
-      <c r="D24" s="65"/>
-      <c r="E24" s="65"/>
-    </row>
-    <row r="26" spans="1:9" s="49" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B27" s="64" t="s">
+      <c r="D66" s="55"/>
+      <c r="E66" s="55"/>
+    </row>
+    <row r="68" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B68" s="49"/>
+      <c r="C68" s="49"/>
+      <c r="D68" s="49"/>
+      <c r="E68" s="49"/>
+    </row>
+    <row r="69" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B69" s="52" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B29" s="1" t="s">
+    <row r="71" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B71" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B30" s="63" t="s">
+    <row r="72" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B72" s="51" t="s">
         <v>18</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="13">
     <mergeCell ref="A3:A4"/>
-    <mergeCell ref="A5:A7"/>
-    <mergeCell ref="C24:E24"/>
+    <mergeCell ref="C66:E66"/>
     <mergeCell ref="B3:B4"/>
     <mergeCell ref="I3:I4"/>
+    <mergeCell ref="A5:A18"/>
     <mergeCell ref="B1:I1"/>
-    <mergeCell ref="C23:E23"/>
+    <mergeCell ref="C65:E65"/>
     <mergeCell ref="H3:H4"/>
     <mergeCell ref="G3:G4"/>
     <mergeCell ref="F3:F4"/>
@@ -1831,7 +1889,7 @@
   <dimension ref="A1:F49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1862,7 +1920,7 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="75" t="s">
+      <c r="A2" s="59" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="17" t="s">
@@ -1875,14 +1933,14 @@
         <f>((C2/3)*100)</f>
         <v>33.333333333333329</v>
       </c>
-      <c r="E2" s="78">
+      <c r="E2" s="62">
         <f>(AVERAGE(C2:C4))*100</f>
         <v>66.666666666666657</v>
       </c>
       <c r="F2" s="5"/>
     </row>
     <row r="3" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="76"/>
+      <c r="A3" s="60"/>
       <c r="B3" s="8" t="s">
         <v>5</v>
       </c>
@@ -1893,11 +1951,11 @@
         <f t="shared" ref="D3:D4" si="0">((C3/3)*100)</f>
         <v>33.333333333333329</v>
       </c>
-      <c r="E3" s="79"/>
+      <c r="E3" s="63"/>
       <c r="F3" s="5"/>
     </row>
     <row r="4" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="77"/>
+      <c r="A4" s="61"/>
       <c r="B4" s="19" t="s">
         <v>6</v>
       </c>
@@ -1908,11 +1966,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E4" s="80"/>
+      <c r="E4" s="64"/>
       <c r="F4" s="5"/>
     </row>
     <row r="5" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="81" t="s">
+      <c r="A5" s="65" t="s">
         <v>7</v>
       </c>
       <c r="B5" s="28" t="s">
@@ -1923,14 +1981,14 @@
         <f>(AVERAGE(C6:C13)*100)*0.5</f>
         <v>0</v>
       </c>
-      <c r="E5" s="84">
+      <c r="E5" s="68">
         <f>D5+D14</f>
         <v>0</v>
       </c>
       <c r="F5" s="5"/>
     </row>
     <row r="6" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="82"/>
+      <c r="A6" s="66"/>
       <c r="B6" s="32" t="s">
         <v>30</v>
       </c>
@@ -1941,11 +1999,11 @@
         <f>(C6/8)*100</f>
         <v>0</v>
       </c>
-      <c r="E6" s="85"/>
+      <c r="E6" s="69"/>
       <c r="F6" s="5"/>
     </row>
     <row r="7" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="82"/>
+      <c r="A7" s="66"/>
       <c r="B7" s="32" t="s">
         <v>31</v>
       </c>
@@ -1956,11 +2014,11 @@
         <f t="shared" ref="D7:D13" si="1">(C7/8)*100</f>
         <v>0</v>
       </c>
-      <c r="E7" s="85"/>
+      <c r="E7" s="69"/>
       <c r="F7" s="5"/>
     </row>
     <row r="8" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="82"/>
+      <c r="A8" s="66"/>
       <c r="B8" s="32" t="s">
         <v>32</v>
       </c>
@@ -1971,11 +2029,11 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="E8" s="85"/>
+      <c r="E8" s="69"/>
       <c r="F8" s="5"/>
     </row>
     <row r="9" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="82"/>
+      <c r="A9" s="66"/>
       <c r="B9" s="32" t="s">
         <v>33</v>
       </c>
@@ -1986,11 +2044,11 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="E9" s="85"/>
+      <c r="E9" s="69"/>
       <c r="F9" s="5"/>
     </row>
     <row r="10" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="82"/>
+      <c r="A10" s="66"/>
       <c r="B10" s="32" t="s">
         <v>34</v>
       </c>
@@ -2001,11 +2059,11 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="E10" s="85"/>
+      <c r="E10" s="69"/>
       <c r="F10" s="5"/>
     </row>
     <row r="11" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="82"/>
+      <c r="A11" s="66"/>
       <c r="B11" s="32" t="s">
         <v>35</v>
       </c>
@@ -2016,11 +2074,11 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="E11" s="85"/>
+      <c r="E11" s="69"/>
       <c r="F11" s="5"/>
     </row>
     <row r="12" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="82"/>
+      <c r="A12" s="66"/>
       <c r="B12" s="32" t="s">
         <v>36</v>
       </c>
@@ -2031,11 +2089,11 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="E12" s="85"/>
+      <c r="E12" s="69"/>
       <c r="F12" s="5"/>
     </row>
     <row r="13" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="82"/>
+      <c r="A13" s="66"/>
       <c r="B13" s="32" t="s">
         <v>37</v>
       </c>
@@ -2046,11 +2104,11 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="E13" s="85"/>
+      <c r="E13" s="69"/>
       <c r="F13" s="5"/>
     </row>
     <row r="14" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="83"/>
+      <c r="A14" s="67"/>
       <c r="B14" s="30" t="s">
         <v>26</v>
       </c>
@@ -2061,7 +2119,7 @@
         <f>(C14/2)*100</f>
         <v>0</v>
       </c>
-      <c r="E14" s="86"/>
+      <c r="E14" s="70"/>
       <c r="F14" s="5"/>
     </row>
     <row r="15" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -2273,12 +2331,12 @@
       <c r="F40" s="5"/>
     </row>
     <row r="41" spans="1:6" ht="24" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="72" t="s">
+      <c r="A41" s="56" t="s">
         <v>27</v>
       </c>
-      <c r="B41" s="73"/>
-      <c r="C41" s="73"/>
-      <c r="D41" s="74"/>
+      <c r="B41" s="57"/>
+      <c r="C41" s="57"/>
+      <c r="D41" s="58"/>
       <c r="E41" s="48">
         <f>(AVERAGE(E2,E5))</f>
         <v>33.333333333333329</v>

</xml_diff>

<commit_message>
Fourth Commit - Workplan
</commit_message>
<xml_diff>
--- a/Workplan.xlsx
+++ b/Workplan.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="66">
   <si>
     <t>ACTIVITIES</t>
   </si>
@@ -162,10 +162,55 @@
     <t>Reviewed by:</t>
   </si>
   <si>
-    <t>Percentage</t>
-  </si>
-  <si>
     <t>Completed</t>
+  </si>
+  <si>
+    <t>DAY</t>
+  </si>
+  <si>
+    <t>Code Development</t>
+  </si>
+  <si>
+    <t>Javascript Calculator</t>
+  </si>
+  <si>
+    <t>CI-CD</t>
+  </si>
+  <si>
+    <t>Developer Check-in code to Repository</t>
+  </si>
+  <si>
+    <t>Configure GitLab and Jenkins</t>
+  </si>
+  <si>
+    <t>Configure Jenkins and Maven</t>
+  </si>
+  <si>
+    <t>Configure Jenkins and Sonarqube</t>
+  </si>
+  <si>
+    <t>Deploy App from Ansible to Tomcat</t>
+  </si>
+  <si>
+    <t>Test app using Selenium</t>
+  </si>
+  <si>
+    <t>Debugging</t>
+  </si>
+  <si>
+    <t>Percent Complete</t>
+  </si>
+  <si>
+    <t>Developer</t>
+  </si>
+  <si>
+    <t>Debug Project Pipeline</t>
+  </si>
+  <si>
+    <t>Finalize Documents</t>
+  </si>
+  <si>
+    <t>DEVOPS BOOTCAMP</t>
   </si>
   <si>
     <r>
@@ -187,7 +232,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">Angelo Q. De Rivera     </t>
+      <t xml:space="preserve">Angelo Q. De Rivera                                          </t>
     </r>
     <r>
       <rPr>
@@ -219,7 +264,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">   Dev/CI-CD:</t>
+      <t xml:space="preserve">                                                  Dev/CI-CD:</t>
     </r>
     <r>
       <rPr>
@@ -229,7 +274,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> Rhodenel  S. Omaña   </t>
+      <t xml:space="preserve"> Rhodenel  S. Omaña                                       </t>
     </r>
     <r>
       <rPr>
@@ -253,24 +298,12 @@
       <t xml:space="preserve"> Bianca Denise A. Del Puerto   Angela Lynne G. Lapus</t>
     </r>
   </si>
-  <si>
-    <t>DAY</t>
-  </si>
-  <si>
-    <t>Code Development</t>
-  </si>
-  <si>
-    <t>Javascript Calculator</t>
-  </si>
-  <si>
-    <t>CI-CD</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -310,13 +343,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="9"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
@@ -334,6 +360,29 @@
       <b/>
       <sz val="12"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -395,7 +444,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="29">
+  <borders count="32">
     <border>
       <left/>
       <right/>
@@ -785,16 +834,58 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="87">
+  <cellXfs count="136">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -936,21 +1027,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
@@ -997,46 +1079,175 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="8" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="6"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="6" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="4"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="8" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="8" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1338,18 +1549,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I72"/>
+  <dimension ref="A1:I45"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+      <selection activeCell="G43" sqref="G43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.42578125" style="49" customWidth="1"/>
+    <col min="1" max="1" width="7.42578125" style="48" customWidth="1"/>
     <col min="2" max="2" width="44" customWidth="1"/>
     <col min="3" max="3" width="10.28515625" customWidth="1"/>
-    <col min="4" max="4" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.7109375" customWidth="1"/>
     <col min="5" max="5" width="11.140625" customWidth="1"/>
     <col min="6" max="6" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.42578125" customWidth="1"/>
@@ -1357,529 +1568,661 @@
     <col min="9" max="9" width="45.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="49" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B1" s="53" t="s">
+    <row r="1" spans="1:9" s="48" customFormat="1" ht="21" x14ac:dyDescent="0.35">
+      <c r="A1" s="67" t="s">
+        <v>64</v>
+      </c>
+      <c r="B1" s="67"/>
+      <c r="C1" s="67"/>
+      <c r="D1" s="67"/>
+      <c r="E1" s="67"/>
+      <c r="F1" s="67"/>
+      <c r="G1" s="67"/>
+      <c r="H1" s="67"/>
+      <c r="I1" s="67"/>
+    </row>
+    <row r="2" spans="1:9" s="48" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A2" s="51" t="s">
         <v>45</v>
       </c>
-      <c r="C1" s="53"/>
-      <c r="D1" s="53"/>
-      <c r="E1" s="53"/>
-      <c r="F1" s="53"/>
-      <c r="G1" s="53"/>
-      <c r="H1" s="53"/>
-      <c r="I1" s="53"/>
-    </row>
-    <row r="2" spans="1:9" s="49" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="74" t="s">
+      <c r="B2" s="51"/>
+      <c r="C2" s="51"/>
+      <c r="D2" s="51"/>
+      <c r="E2" s="51"/>
+      <c r="F2" s="51"/>
+      <c r="G2" s="51"/>
+      <c r="H2" s="51"/>
+      <c r="I2" s="51"/>
+    </row>
+    <row r="3" spans="1:9" s="48" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="49"/>
+      <c r="C3" s="49"/>
+      <c r="D3" s="49"/>
+      <c r="E3" s="49"/>
+      <c r="F3" s="49"/>
+      <c r="G3" s="49"/>
+      <c r="H3" s="49"/>
+      <c r="I3" s="49"/>
+    </row>
+    <row r="4" spans="1:9" s="48" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="77" t="s">
+        <v>49</v>
+      </c>
+      <c r="B5" s="77" t="s">
+        <v>38</v>
+      </c>
+      <c r="C5" s="109" t="s">
+        <v>40</v>
+      </c>
+      <c r="D5" s="73" t="s">
+        <v>41</v>
+      </c>
+      <c r="E5" s="109" t="s">
+        <v>42</v>
+      </c>
+      <c r="F5" s="73" t="s">
+        <v>43</v>
+      </c>
+      <c r="G5" s="94" t="s">
+        <v>60</v>
+      </c>
+      <c r="H5" s="94" t="s">
+        <v>44</v>
+      </c>
+      <c r="I5" s="94" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="78"/>
+      <c r="B6" s="78"/>
+      <c r="C6" s="110"/>
+      <c r="D6" s="76"/>
+      <c r="E6" s="110"/>
+      <c r="F6" s="76"/>
+      <c r="G6" s="95"/>
+      <c r="H6" s="95"/>
+      <c r="I6" s="95"/>
+    </row>
+    <row r="7" spans="1:9" s="48" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="81">
+        <v>1</v>
+      </c>
+      <c r="B7" s="85" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="111"/>
+      <c r="D7" s="82"/>
+      <c r="E7" s="111"/>
+      <c r="F7" s="82"/>
+      <c r="G7" s="96"/>
+      <c r="H7" s="96"/>
+      <c r="I7" s="96"/>
+    </row>
+    <row r="8" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+      <c r="A8" s="79"/>
+      <c r="B8" s="86" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="112">
+        <v>42565</v>
+      </c>
+      <c r="D8" s="113">
+        <v>42565</v>
+      </c>
+      <c r="E8" s="112">
+        <v>42565</v>
+      </c>
+      <c r="F8" s="113">
+        <v>42565</v>
+      </c>
+      <c r="G8" s="100">
+        <v>100</v>
+      </c>
+      <c r="H8" s="104" t="s">
+        <v>48</v>
+      </c>
+      <c r="I8" s="97" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="79"/>
+      <c r="B9" s="87" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="112">
+        <v>42565</v>
+      </c>
+      <c r="D9" s="113">
+        <v>42565</v>
+      </c>
+      <c r="E9" s="112">
+        <v>42565</v>
+      </c>
+      <c r="F9" s="113">
+        <v>42565</v>
+      </c>
+      <c r="G9" s="100">
+        <v>100</v>
+      </c>
+      <c r="H9" s="104" t="s">
+        <v>48</v>
+      </c>
+      <c r="I9" s="92"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="79"/>
+      <c r="B10" s="87" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" s="112">
+        <v>42565</v>
+      </c>
+      <c r="D10" s="113">
+        <v>42565</v>
+      </c>
+      <c r="E10" s="112">
+        <v>42565</v>
+      </c>
+      <c r="F10" s="113">
+        <v>42565</v>
+      </c>
+      <c r="G10" s="100">
+        <v>100</v>
+      </c>
+      <c r="H10" s="104" t="s">
+        <v>48</v>
+      </c>
+      <c r="I10" s="92"/>
+    </row>
+    <row r="11" spans="1:9" s="50" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="79"/>
+      <c r="B11" s="88" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" s="114"/>
+      <c r="D11" s="115"/>
+      <c r="E11" s="114"/>
+      <c r="F11" s="115"/>
+      <c r="G11" s="101"/>
+      <c r="H11" s="105"/>
+      <c r="I11" s="98"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="79"/>
+      <c r="B12" s="87" t="s">
+        <v>29</v>
+      </c>
+      <c r="C12" s="112">
+        <v>42565</v>
+      </c>
+      <c r="D12" s="113">
+        <v>42565</v>
+      </c>
+      <c r="E12" s="112"/>
+      <c r="F12" s="124"/>
+      <c r="G12" s="100"/>
+      <c r="H12" s="100"/>
+      <c r="I12" s="92"/>
+    </row>
+    <row r="13" spans="1:9" s="48" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="79"/>
+      <c r="B13" s="108" t="s">
+        <v>30</v>
+      </c>
+      <c r="C13" s="112">
+        <v>42565</v>
+      </c>
+      <c r="D13" s="113">
+        <v>42565</v>
+      </c>
+      <c r="E13" s="112"/>
+      <c r="F13" s="124"/>
+      <c r="G13" s="100"/>
+      <c r="H13" s="100"/>
+      <c r="I13" s="92"/>
+    </row>
+    <row r="14" spans="1:9" s="48" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="79"/>
+      <c r="B14" s="108" t="s">
+        <v>31</v>
+      </c>
+      <c r="C14" s="112">
+        <v>42565</v>
+      </c>
+      <c r="D14" s="113">
+        <v>42565</v>
+      </c>
+      <c r="E14" s="112"/>
+      <c r="F14" s="124"/>
+      <c r="G14" s="100"/>
+      <c r="H14" s="100"/>
+      <c r="I14" s="92"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="79"/>
+      <c r="B15" s="108" t="s">
+        <v>35</v>
+      </c>
+      <c r="C15" s="112">
+        <v>42565</v>
+      </c>
+      <c r="D15" s="113">
+        <v>42565</v>
+      </c>
+      <c r="E15" s="125"/>
+      <c r="F15" s="124"/>
+      <c r="G15" s="100"/>
+      <c r="H15" s="100"/>
+      <c r="I15" s="92"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="79"/>
+      <c r="B16" s="108" t="s">
+        <v>36</v>
+      </c>
+      <c r="C16" s="112">
+        <v>42565</v>
+      </c>
+      <c r="D16" s="113">
+        <v>42565</v>
+      </c>
+      <c r="E16" s="125"/>
+      <c r="F16" s="124"/>
+      <c r="G16" s="100"/>
+      <c r="H16" s="100"/>
+      <c r="I16" s="92"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="79"/>
+      <c r="B17" s="108" t="s">
+        <v>37</v>
+      </c>
+      <c r="C17" s="112">
+        <v>42565</v>
+      </c>
+      <c r="D17" s="113">
+        <v>42565</v>
+      </c>
+      <c r="E17" s="125"/>
+      <c r="F17" s="124"/>
+      <c r="G17" s="100"/>
+      <c r="H17" s="100"/>
+      <c r="I17" s="92"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="79"/>
+      <c r="B18" s="87" t="s">
+        <v>26</v>
+      </c>
+      <c r="C18" s="112">
+        <v>42565</v>
+      </c>
+      <c r="D18" s="113">
+        <v>42565</v>
+      </c>
+      <c r="E18" s="125"/>
+      <c r="F18" s="124"/>
+      <c r="G18" s="100"/>
+      <c r="H18" s="100"/>
+      <c r="I18" s="92"/>
+    </row>
+    <row r="19" spans="1:9" s="50" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A19" s="79"/>
+      <c r="B19" s="89" t="s">
+        <v>50</v>
+      </c>
+      <c r="C19" s="114"/>
+      <c r="D19" s="115"/>
+      <c r="E19" s="126"/>
+      <c r="F19" s="127"/>
+      <c r="G19" s="101"/>
+      <c r="H19" s="101"/>
+      <c r="I19" s="98"/>
+    </row>
+    <row r="20" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="80"/>
+      <c r="B20" s="106" t="s">
         <v>51</v>
       </c>
-      <c r="B3" s="74" t="s">
-        <v>38</v>
-      </c>
-      <c r="C3" s="75" t="s">
-        <v>40</v>
-      </c>
-      <c r="D3" s="75" t="s">
-        <v>41</v>
-      </c>
-      <c r="E3" s="75" t="s">
-        <v>42</v>
-      </c>
-      <c r="F3" s="75" t="s">
-        <v>43</v>
-      </c>
-      <c r="G3" s="75" t="s">
-        <v>48</v>
-      </c>
-      <c r="H3" s="75" t="s">
-        <v>44</v>
-      </c>
-      <c r="I3" s="75" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="74"/>
-      <c r="B4" s="74"/>
-      <c r="C4" s="75"/>
-      <c r="D4" s="75"/>
-      <c r="E4" s="75"/>
-      <c r="F4" s="75"/>
-      <c r="G4" s="75"/>
-      <c r="H4" s="75"/>
-      <c r="I4" s="75"/>
-    </row>
-    <row r="5" spans="1:9" s="49" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="71">
-        <v>1</v>
-      </c>
-      <c r="B5" s="84" t="s">
+      <c r="C20" s="116">
+        <v>42565</v>
+      </c>
+      <c r="D20" s="117">
+        <v>42565</v>
+      </c>
+      <c r="E20" s="128"/>
+      <c r="F20" s="129"/>
+      <c r="G20" s="102"/>
+      <c r="H20" s="102"/>
+      <c r="I20" s="90"/>
+    </row>
+    <row r="21" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A21" s="81">
+        <v>2</v>
+      </c>
+      <c r="B21" s="91" t="s">
+        <v>52</v>
+      </c>
+      <c r="C21" s="118"/>
+      <c r="D21" s="119"/>
+      <c r="E21" s="118"/>
+      <c r="F21" s="119"/>
+      <c r="G21" s="103"/>
+      <c r="H21" s="103"/>
+      <c r="I21" s="99"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" s="79"/>
+      <c r="B22" s="87" t="s">
+        <v>53</v>
+      </c>
+      <c r="C22" s="120"/>
+      <c r="D22" s="74"/>
+      <c r="E22" s="120"/>
+      <c r="F22" s="74"/>
+      <c r="G22" s="92"/>
+      <c r="H22" s="92"/>
+      <c r="I22" s="92"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" s="79"/>
+      <c r="B23" s="87" t="s">
+        <v>54</v>
+      </c>
+      <c r="C23" s="120"/>
+      <c r="D23" s="74"/>
+      <c r="E23" s="120"/>
+      <c r="F23" s="74"/>
+      <c r="G23" s="92"/>
+      <c r="H23" s="92"/>
+      <c r="I23" s="92"/>
+    </row>
+    <row r="24" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="80"/>
+      <c r="B24" s="106" t="s">
+        <v>55</v>
+      </c>
+      <c r="C24" s="121"/>
+      <c r="D24" s="75"/>
+      <c r="E24" s="121"/>
+      <c r="F24" s="75"/>
+      <c r="G24" s="90"/>
+      <c r="H24" s="90"/>
+      <c r="I24" s="90"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" s="81">
+        <v>3</v>
+      </c>
+      <c r="B25" s="107" t="s">
+        <v>56</v>
+      </c>
+      <c r="C25" s="122"/>
+      <c r="D25" s="84"/>
+      <c r="E25" s="122"/>
+      <c r="F25" s="84"/>
+      <c r="G25" s="93"/>
+      <c r="H25" s="93"/>
+      <c r="I25" s="93"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" s="79"/>
+      <c r="B26" s="87" t="s">
+        <v>57</v>
+      </c>
+      <c r="C26" s="120"/>
+      <c r="D26" s="74"/>
+      <c r="E26" s="120"/>
+      <c r="F26" s="74"/>
+      <c r="G26" s="92"/>
+      <c r="H26" s="92"/>
+      <c r="I26" s="92"/>
+    </row>
+    <row r="27" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="80"/>
+      <c r="B27" s="106" t="s">
+        <v>58</v>
+      </c>
+      <c r="C27" s="121"/>
+      <c r="D27" s="75"/>
+      <c r="E27" s="121"/>
+      <c r="F27" s="75"/>
+      <c r="G27" s="90"/>
+      <c r="H27" s="90"/>
+      <c r="I27" s="90"/>
+    </row>
+    <row r="28" spans="1:9" s="48" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A28" s="81">
         <v>4</v>
       </c>
-      <c r="C5" s="78"/>
-      <c r="D5" s="78"/>
-      <c r="E5" s="78"/>
-      <c r="F5" s="78"/>
-      <c r="G5" s="78"/>
-      <c r="H5" s="78"/>
-      <c r="I5" s="78"/>
-    </row>
-    <row r="6" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="A6" s="71"/>
-      <c r="B6" s="77" t="s">
-        <v>3</v>
-      </c>
-      <c r="C6" s="50">
-        <v>42565</v>
-      </c>
-      <c r="D6" s="50">
-        <v>42565</v>
-      </c>
-      <c r="E6" s="50">
-        <v>42565</v>
-      </c>
-      <c r="F6" s="50">
-        <v>42565</v>
-      </c>
-      <c r="G6" s="10">
-        <v>100</v>
-      </c>
-      <c r="H6" s="50" t="s">
-        <v>49</v>
-      </c>
-      <c r="I6" s="76" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="71"/>
-      <c r="B7" s="73" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" s="50">
-        <v>42565</v>
-      </c>
-      <c r="D7" s="50">
-        <v>42565</v>
-      </c>
-      <c r="E7" s="50">
-        <v>42565</v>
-      </c>
-      <c r="F7" s="50">
-        <v>42565</v>
-      </c>
-      <c r="G7" s="10">
-        <v>100</v>
-      </c>
-      <c r="H7" s="50" t="s">
-        <v>49</v>
-      </c>
-      <c r="I7" s="72"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="71"/>
-      <c r="B8" s="73" t="s">
-        <v>6</v>
-      </c>
-      <c r="C8" s="50">
-        <v>42565</v>
-      </c>
-      <c r="D8" s="50">
-        <v>42565</v>
-      </c>
-      <c r="E8" s="50">
-        <v>42565</v>
-      </c>
-      <c r="F8" s="50">
-        <v>42565</v>
-      </c>
-      <c r="G8" s="10">
-        <v>100</v>
-      </c>
-      <c r="H8" s="50" t="s">
-        <v>49</v>
-      </c>
-      <c r="I8" s="72"/>
-    </row>
-    <row r="9" spans="1:9" s="83" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="71"/>
-      <c r="B9" s="85" t="s">
-        <v>7</v>
-      </c>
-      <c r="C9" s="79"/>
-      <c r="D9" s="79"/>
-      <c r="E9" s="79"/>
-      <c r="F9" s="79"/>
-      <c r="G9" s="80"/>
-      <c r="H9" s="79"/>
-      <c r="I9" s="81"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="71"/>
-      <c r="B10" s="73" t="s">
-        <v>29</v>
-      </c>
-      <c r="C10" s="50">
-        <v>42565</v>
-      </c>
-      <c r="D10" s="50">
-        <v>42565</v>
-      </c>
-      <c r="E10" s="50"/>
-      <c r="F10" s="10"/>
-      <c r="G10" s="10"/>
-      <c r="H10" s="10"/>
-      <c r="I10" s="72"/>
-    </row>
-    <row r="11" spans="1:9" s="49" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="71"/>
-      <c r="B11" s="82" t="s">
-        <v>30</v>
-      </c>
-      <c r="C11" s="50">
-        <v>42565</v>
-      </c>
-      <c r="D11" s="50">
-        <v>42565</v>
-      </c>
-      <c r="E11" s="50"/>
-      <c r="F11" s="10"/>
-      <c r="G11" s="10"/>
-      <c r="H11" s="10"/>
-      <c r="I11" s="72"/>
-    </row>
-    <row r="12" spans="1:9" s="49" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="71"/>
-      <c r="B12" s="82" t="s">
-        <v>31</v>
-      </c>
-      <c r="C12" s="50">
-        <v>42565</v>
-      </c>
-      <c r="D12" s="50">
-        <v>42565</v>
-      </c>
-      <c r="E12" s="50"/>
-      <c r="F12" s="10"/>
-      <c r="G12" s="10"/>
-      <c r="H12" s="10"/>
-      <c r="I12" s="72"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="71"/>
-      <c r="B13" s="82" t="s">
-        <v>35</v>
-      </c>
-      <c r="C13" s="50">
-        <v>42565</v>
-      </c>
-      <c r="D13" s="50">
-        <v>42565</v>
-      </c>
-      <c r="E13" s="10"/>
-      <c r="F13" s="10"/>
-      <c r="G13" s="10"/>
-      <c r="H13" s="10"/>
-      <c r="I13" s="72"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="71"/>
-      <c r="B14" s="82" t="s">
-        <v>36</v>
-      </c>
-      <c r="C14" s="50">
-        <v>42565</v>
-      </c>
-      <c r="D14" s="50">
-        <v>42565</v>
-      </c>
-      <c r="E14" s="10"/>
-      <c r="F14" s="10"/>
-      <c r="G14" s="10"/>
-      <c r="H14" s="10"/>
-      <c r="I14" s="72"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="71"/>
-      <c r="B15" s="82" t="s">
-        <v>37</v>
-      </c>
-      <c r="C15" s="50">
-        <v>42565</v>
-      </c>
-      <c r="D15" s="50">
-        <v>42565</v>
-      </c>
-      <c r="E15" s="10"/>
-      <c r="F15" s="10"/>
-      <c r="G15" s="10"/>
-      <c r="H15" s="10"/>
-      <c r="I15" s="72"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="71"/>
-      <c r="B16" s="73" t="s">
-        <v>26</v>
-      </c>
-      <c r="C16" s="50">
-        <v>42565</v>
-      </c>
-      <c r="D16" s="50">
-        <v>42565</v>
-      </c>
-      <c r="E16" s="10"/>
-      <c r="F16" s="10"/>
-      <c r="G16" s="10"/>
-      <c r="H16" s="10"/>
-      <c r="I16" s="72"/>
-    </row>
-    <row r="17" spans="1:9" s="83" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="71"/>
-      <c r="B17" s="86" t="s">
+      <c r="B28" s="91" t="s">
+        <v>59</v>
+      </c>
+      <c r="C28" s="123"/>
+      <c r="D28" s="83"/>
+      <c r="E28" s="123"/>
+      <c r="F28" s="83"/>
+      <c r="G28" s="99"/>
+      <c r="H28" s="99"/>
+      <c r="I28" s="99"/>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" s="79"/>
+      <c r="B29" s="87" t="s">
+        <v>62</v>
+      </c>
+      <c r="C29" s="120"/>
+      <c r="D29" s="74"/>
+      <c r="E29" s="120"/>
+      <c r="F29" s="74"/>
+      <c r="G29" s="92"/>
+      <c r="H29" s="92"/>
+      <c r="I29" s="92"/>
+    </row>
+    <row r="30" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="80"/>
+      <c r="B30" s="106" t="s">
+        <v>63</v>
+      </c>
+      <c r="C30" s="121"/>
+      <c r="D30" s="75"/>
+      <c r="E30" s="121"/>
+      <c r="F30" s="75"/>
+      <c r="G30" s="90"/>
+      <c r="H30" s="90"/>
+      <c r="I30" s="90"/>
+    </row>
+    <row r="31" spans="1:9" s="48" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="68"/>
+      <c r="B31" s="69"/>
+      <c r="C31" s="69"/>
+      <c r="D31" s="69"/>
+      <c r="E31" s="69"/>
+      <c r="F31" s="69"/>
+      <c r="G31" s="69"/>
+      <c r="H31" s="69"/>
+      <c r="I31" s="69"/>
+    </row>
+    <row r="33" spans="2:9" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B33" s="130" t="s">
+        <v>46</v>
+      </c>
+      <c r="C33" s="71"/>
+      <c r="D33" s="71"/>
+      <c r="E33" s="71"/>
+      <c r="F33" s="71"/>
+      <c r="G33" s="130" t="s">
+        <v>47</v>
+      </c>
+      <c r="H33" s="71"/>
+      <c r="I33" s="71"/>
+    </row>
+    <row r="34" spans="2:9" s="48" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B34" s="70"/>
+      <c r="C34" s="71"/>
+      <c r="D34" s="71"/>
+      <c r="E34" s="71"/>
+      <c r="F34" s="71"/>
+      <c r="G34" s="70"/>
+      <c r="H34" s="71"/>
+      <c r="I34" s="71"/>
+    </row>
+    <row r="35" spans="2:9" s="48" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B35" s="70"/>
+      <c r="C35" s="71"/>
+      <c r="D35" s="71"/>
+      <c r="E35" s="71"/>
+      <c r="F35" s="71"/>
+      <c r="G35" s="71"/>
+      <c r="H35" s="71"/>
+      <c r="I35" s="71"/>
+    </row>
+    <row r="36" spans="2:9" s="48" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B36" s="133" t="s">
+        <v>12</v>
+      </c>
+      <c r="C36" s="134" t="s">
+        <v>8</v>
+      </c>
+      <c r="D36" s="134"/>
+      <c r="E36" s="134"/>
+      <c r="F36" s="71"/>
+      <c r="G36" s="70"/>
+      <c r="H36" s="135" t="s">
+        <v>10</v>
+      </c>
+      <c r="I36" s="71"/>
+    </row>
+    <row r="37" spans="2:9" s="48" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B37" s="131" t="s">
         <v>52</v>
       </c>
-      <c r="C17" s="79"/>
-      <c r="D17" s="79"/>
-      <c r="E17" s="80"/>
-      <c r="F17" s="80"/>
-      <c r="G17" s="80"/>
-      <c r="H17" s="80"/>
-      <c r="I17" s="81"/>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="71"/>
-      <c r="B18" s="72" t="s">
-        <v>53</v>
-      </c>
-      <c r="C18" s="50">
-        <v>42565</v>
-      </c>
-      <c r="D18" s="50">
-        <v>42565</v>
-      </c>
-      <c r="E18" s="10"/>
-      <c r="F18" s="10"/>
-      <c r="G18" s="10"/>
-      <c r="H18" s="10"/>
-      <c r="I18" s="72"/>
-    </row>
-    <row r="19" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="11"/>
-      <c r="B19" s="86" t="s">
-        <v>54</v>
-      </c>
-      <c r="C19" s="80"/>
-      <c r="D19" s="80"/>
-      <c r="E19" s="80"/>
-      <c r="F19" s="80"/>
-      <c r="G19" s="80"/>
-      <c r="H19" s="80"/>
-      <c r="I19" s="81"/>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B20" s="72"/>
-      <c r="C20" s="72"/>
-      <c r="D20" s="72"/>
-      <c r="E20" s="72"/>
-      <c r="F20" s="72"/>
-      <c r="G20" s="72"/>
-      <c r="H20" s="72"/>
-      <c r="I20" s="72"/>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B21" s="72"/>
-      <c r="C21" s="72"/>
-      <c r="D21" s="72"/>
-      <c r="E21" s="72"/>
-      <c r="F21" s="72"/>
-      <c r="G21" s="72"/>
-      <c r="H21" s="72"/>
-      <c r="I21" s="72"/>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B22" s="72"/>
-      <c r="C22" s="72"/>
-      <c r="D22" s="72"/>
-      <c r="E22" s="72"/>
-      <c r="F22" s="72"/>
-      <c r="G22" s="72"/>
-      <c r="H22" s="72"/>
-      <c r="I22" s="72"/>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B23" s="72"/>
-      <c r="C23" s="72"/>
-      <c r="D23" s="72"/>
-      <c r="E23" s="72"/>
-      <c r="F23" s="72"/>
-      <c r="G23" s="72"/>
-      <c r="H23" s="72"/>
-      <c r="I23" s="72"/>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B24" s="72"/>
-      <c r="C24" s="72"/>
-      <c r="D24" s="72"/>
-      <c r="E24" s="72"/>
-      <c r="F24" s="72"/>
-      <c r="G24" s="72"/>
-      <c r="H24" s="72"/>
-      <c r="I24" s="72"/>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B25" s="72"/>
-      <c r="C25" s="72"/>
-      <c r="D25" s="72"/>
-      <c r="E25" s="72"/>
-      <c r="F25" s="72"/>
-      <c r="G25" s="72"/>
-      <c r="H25" s="72"/>
-      <c r="I25" s="72"/>
-    </row>
-    <row r="26" spans="1:9" s="49" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="72"/>
-      <c r="C26" s="72"/>
-      <c r="D26" s="72"/>
-      <c r="E26" s="72"/>
-      <c r="F26" s="72"/>
-      <c r="G26" s="72"/>
-      <c r="H26" s="72"/>
-      <c r="I26" s="72"/>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B27" s="72"/>
-      <c r="C27" s="72"/>
-      <c r="D27" s="72"/>
-      <c r="E27" s="72"/>
-      <c r="F27" s="72"/>
-      <c r="G27" s="72"/>
-      <c r="H27" s="72"/>
-      <c r="I27" s="72"/>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B28" s="72"/>
-      <c r="C28" s="72"/>
-      <c r="D28" s="72"/>
-      <c r="E28" s="72"/>
-      <c r="F28" s="72"/>
-      <c r="G28" s="72"/>
-      <c r="H28" s="72"/>
-      <c r="I28" s="72"/>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B29" s="72"/>
-      <c r="C29" s="72"/>
-      <c r="D29" s="72"/>
-      <c r="E29" s="72"/>
-      <c r="F29" s="72"/>
-      <c r="G29" s="72"/>
-      <c r="H29" s="72"/>
-      <c r="I29" s="72"/>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B30" s="72"/>
-      <c r="C30" s="72"/>
-      <c r="D30" s="72"/>
-      <c r="E30" s="72"/>
-      <c r="F30" s="72"/>
-      <c r="G30" s="72"/>
-      <c r="H30" s="72"/>
-      <c r="I30" s="72"/>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B31" s="72"/>
-      <c r="C31" s="72"/>
-      <c r="D31" s="72"/>
-      <c r="E31" s="72"/>
-      <c r="F31" s="72"/>
-      <c r="G31" s="72"/>
-      <c r="H31" s="72"/>
-      <c r="I31" s="72"/>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B32" s="72"/>
-      <c r="C32" s="72"/>
-      <c r="D32" s="72"/>
-      <c r="E32" s="72"/>
-      <c r="F32" s="72"/>
-      <c r="G32" s="72"/>
-      <c r="H32" s="72"/>
-      <c r="I32" s="72"/>
-    </row>
-    <row r="33" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B33" s="72"/>
-      <c r="C33" s="72"/>
-      <c r="D33" s="72"/>
-      <c r="E33" s="72"/>
-      <c r="F33" s="72"/>
-      <c r="G33" s="72"/>
-      <c r="H33" s="72"/>
-      <c r="I33" s="72"/>
-    </row>
-    <row r="63" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B63" s="52" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="65" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B65" s="2" t="s">
+      <c r="C37" s="132" t="s">
+        <v>61</v>
+      </c>
+      <c r="D37" s="132"/>
+      <c r="E37" s="132"/>
+      <c r="F37" s="71"/>
+      <c r="G37" s="71"/>
+      <c r="H37" s="131" t="s">
+        <v>18</v>
+      </c>
+      <c r="I37" s="71"/>
+    </row>
+    <row r="38" spans="2:9" s="48" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B38" s="72"/>
+      <c r="C38" s="72"/>
+      <c r="D38" s="72"/>
+      <c r="E38" s="72"/>
+      <c r="F38" s="71"/>
+      <c r="G38" s="71"/>
+      <c r="H38" s="72"/>
+      <c r="I38" s="71"/>
+    </row>
+    <row r="39" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B39" s="71"/>
+      <c r="C39" s="71"/>
+      <c r="D39" s="71"/>
+      <c r="E39" s="71"/>
+      <c r="F39" s="71"/>
+      <c r="G39" s="71"/>
+      <c r="H39" s="71"/>
+      <c r="I39" s="71"/>
+    </row>
+    <row r="40" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B40" s="133" t="s">
         <v>9</v>
       </c>
-      <c r="C65" s="54" t="s">
+      <c r="C40" s="134" t="s">
         <v>11</v>
       </c>
-      <c r="D65" s="54"/>
-      <c r="E65" s="54"/>
-    </row>
-    <row r="66" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B66" s="51" t="s">
+      <c r="D40" s="134"/>
+      <c r="E40" s="134"/>
+      <c r="F40" s="71"/>
+      <c r="G40" s="71"/>
+      <c r="H40" s="71"/>
+      <c r="I40" s="71"/>
+    </row>
+    <row r="41" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B41" s="131" t="s">
         <v>20</v>
       </c>
-      <c r="C66" s="55" t="s">
+      <c r="C41" s="132" t="s">
         <v>20</v>
       </c>
-      <c r="D66" s="55"/>
-      <c r="E66" s="55"/>
-    </row>
-    <row r="68" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B68" s="49"/>
-      <c r="C68" s="49"/>
-      <c r="D68" s="49"/>
-      <c r="E68" s="49"/>
-    </row>
-    <row r="69" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B69" s="52" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="71" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B71" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="72" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B72" s="51" t="s">
-        <v>18</v>
-      </c>
+      <c r="D41" s="132"/>
+      <c r="E41" s="132"/>
+      <c r="F41" s="71"/>
+      <c r="G41" s="71"/>
+      <c r="H41" s="71"/>
+      <c r="I41" s="71"/>
+    </row>
+    <row r="42" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B42" s="71"/>
+      <c r="C42" s="71"/>
+      <c r="D42" s="71"/>
+      <c r="E42" s="71"/>
+      <c r="F42" s="71"/>
+      <c r="G42" s="71"/>
+      <c r="H42" s="71"/>
+      <c r="I42" s="71"/>
+    </row>
+    <row r="43" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B43" s="71"/>
+      <c r="C43" s="71"/>
+      <c r="D43" s="71"/>
+      <c r="E43" s="71"/>
+      <c r="F43" s="71"/>
+      <c r="G43" s="71"/>
+      <c r="H43" s="71"/>
+      <c r="I43" s="71"/>
+    </row>
+    <row r="44" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B44" s="71"/>
+      <c r="C44" s="71"/>
+      <c r="D44" s="71"/>
+      <c r="E44" s="71"/>
+      <c r="F44" s="71"/>
+      <c r="G44" s="71"/>
+      <c r="H44" s="71"/>
+      <c r="I44" s="71"/>
+    </row>
+    <row r="45" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B45" s="71"/>
+      <c r="C45" s="71"/>
+      <c r="D45" s="71"/>
+      <c r="E45" s="71"/>
+      <c r="F45" s="71"/>
+      <c r="G45" s="71"/>
+      <c r="H45" s="71"/>
+      <c r="I45" s="71"/>
     </row>
   </sheetData>
-  <mergeCells count="13">
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="C66:E66"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="I3:I4"/>
-    <mergeCell ref="A5:A18"/>
-    <mergeCell ref="B1:I1"/>
-    <mergeCell ref="C65:E65"/>
-    <mergeCell ref="H3:H4"/>
-    <mergeCell ref="G3:G4"/>
-    <mergeCell ref="F3:F4"/>
-    <mergeCell ref="E3:E4"/>
-    <mergeCell ref="D3:D4"/>
-    <mergeCell ref="C3:C4"/>
+  <mergeCells count="19">
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="C40:E40"/>
+    <mergeCell ref="H5:H6"/>
+    <mergeCell ref="G5:G6"/>
+    <mergeCell ref="F5:F6"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="C36:E36"/>
+    <mergeCell ref="C37:E37"/>
+    <mergeCell ref="A2:I2"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="C41:E41"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="I5:I6"/>
+    <mergeCell ref="A7:A20"/>
+    <mergeCell ref="A21:A24"/>
+    <mergeCell ref="A25:A27"/>
+    <mergeCell ref="A28:A30"/>
   </mergeCells>
-  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.25" right="0.25" top="1" bottom="1" header="0.3" footer="0.3"/>
   <pageSetup paperSize="5" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
@@ -1894,518 +2237,518 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.7109375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="66.140625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="16.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.85546875" style="2" customWidth="1"/>
-    <col min="5" max="5" width="27.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="1" width="22.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="66.140625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="16.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.85546875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="22" t="s">
+      <c r="B1" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="22" t="s">
+      <c r="C1" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="34" t="s">
+      <c r="D1" s="33" t="s">
         <v>28</v>
       </c>
-      <c r="E1" s="44" t="s">
+      <c r="E1" s="43" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="59" t="s">
+      <c r="A2" s="55" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="18">
+      <c r="C2" s="17">
         <v>1</v>
       </c>
-      <c r="D2" s="35">
+      <c r="D2" s="34">
         <f>((C2/3)*100)</f>
         <v>33.333333333333329</v>
       </c>
-      <c r="E2" s="62">
+      <c r="E2" s="58">
         <f>(AVERAGE(C2:C4))*100</f>
         <v>66.666666666666657</v>
       </c>
-      <c r="F2" s="5"/>
+      <c r="F2" s="4"/>
     </row>
     <row r="3" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="60"/>
-      <c r="B3" s="8" t="s">
+      <c r="A3" s="56"/>
+      <c r="B3" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="9">
+      <c r="C3" s="8">
         <v>1</v>
       </c>
-      <c r="D3" s="36">
+      <c r="D3" s="35">
         <f t="shared" ref="D3:D4" si="0">((C3/3)*100)</f>
         <v>33.333333333333329</v>
       </c>
-      <c r="E3" s="63"/>
-      <c r="F3" s="5"/>
+      <c r="E3" s="59"/>
+      <c r="F3" s="4"/>
     </row>
     <row r="4" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="61"/>
-      <c r="B4" s="19" t="s">
+      <c r="A4" s="57"/>
+      <c r="B4" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="20">
+      <c r="C4" s="19">
         <v>0</v>
       </c>
-      <c r="D4" s="37">
+      <c r="D4" s="36">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E4" s="64"/>
-      <c r="F4" s="5"/>
+      <c r="E4" s="60"/>
+      <c r="F4" s="4"/>
     </row>
     <row r="5" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="65" t="s">
+      <c r="A5" s="61" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="28" t="s">
+      <c r="B5" s="27" t="s">
         <v>29</v>
       </c>
-      <c r="C5" s="29"/>
-      <c r="D5" s="38">
+      <c r="C5" s="28"/>
+      <c r="D5" s="37">
         <f>(AVERAGE(C6:C13)*100)*0.5</f>
         <v>0</v>
       </c>
-      <c r="E5" s="68">
+      <c r="E5" s="64">
         <f>D5+D14</f>
         <v>0</v>
       </c>
-      <c r="F5" s="5"/>
+      <c r="F5" s="4"/>
     </row>
     <row r="6" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="66"/>
-      <c r="B6" s="32" t="s">
+      <c r="A6" s="62"/>
+      <c r="B6" s="31" t="s">
         <v>30</v>
       </c>
-      <c r="C6" s="33">
+      <c r="C6" s="32">
         <v>0</v>
       </c>
-      <c r="D6" s="39">
+      <c r="D6" s="38">
         <f>(C6/8)*100</f>
         <v>0</v>
       </c>
-      <c r="E6" s="69"/>
-      <c r="F6" s="5"/>
+      <c r="E6" s="65"/>
+      <c r="F6" s="4"/>
     </row>
     <row r="7" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="66"/>
-      <c r="B7" s="32" t="s">
+      <c r="A7" s="62"/>
+      <c r="B7" s="31" t="s">
         <v>31</v>
       </c>
-      <c r="C7" s="33">
+      <c r="C7" s="32">
         <v>0</v>
       </c>
-      <c r="D7" s="39">
+      <c r="D7" s="38">
         <f t="shared" ref="D7:D13" si="1">(C7/8)*100</f>
         <v>0</v>
       </c>
-      <c r="E7" s="69"/>
-      <c r="F7" s="5"/>
+      <c r="E7" s="65"/>
+      <c r="F7" s="4"/>
     </row>
     <row r="8" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="66"/>
-      <c r="B8" s="32" t="s">
+      <c r="A8" s="62"/>
+      <c r="B8" s="31" t="s">
         <v>32</v>
       </c>
-      <c r="C8" s="33">
+      <c r="C8" s="32">
         <v>0</v>
       </c>
-      <c r="D8" s="39">
+      <c r="D8" s="38">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="E8" s="69"/>
-      <c r="F8" s="5"/>
+      <c r="E8" s="65"/>
+      <c r="F8" s="4"/>
     </row>
     <row r="9" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="66"/>
-      <c r="B9" s="32" t="s">
+      <c r="A9" s="62"/>
+      <c r="B9" s="31" t="s">
         <v>33</v>
       </c>
-      <c r="C9" s="33">
+      <c r="C9" s="32">
         <v>0</v>
       </c>
-      <c r="D9" s="39">
+      <c r="D9" s="38">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="E9" s="69"/>
-      <c r="F9" s="5"/>
+      <c r="E9" s="65"/>
+      <c r="F9" s="4"/>
     </row>
     <row r="10" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="66"/>
-      <c r="B10" s="32" t="s">
+      <c r="A10" s="62"/>
+      <c r="B10" s="31" t="s">
         <v>34</v>
       </c>
-      <c r="C10" s="33">
+      <c r="C10" s="32">
         <v>0</v>
       </c>
-      <c r="D10" s="39">
+      <c r="D10" s="38">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="E10" s="69"/>
-      <c r="F10" s="5"/>
+      <c r="E10" s="65"/>
+      <c r="F10" s="4"/>
     </row>
     <row r="11" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="66"/>
-      <c r="B11" s="32" t="s">
+      <c r="A11" s="62"/>
+      <c r="B11" s="31" t="s">
         <v>35</v>
       </c>
-      <c r="C11" s="33">
+      <c r="C11" s="32">
         <v>0</v>
       </c>
-      <c r="D11" s="39">
+      <c r="D11" s="38">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="E11" s="69"/>
-      <c r="F11" s="5"/>
+      <c r="E11" s="65"/>
+      <c r="F11" s="4"/>
     </row>
     <row r="12" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="66"/>
-      <c r="B12" s="32" t="s">
+      <c r="A12" s="62"/>
+      <c r="B12" s="31" t="s">
         <v>36</v>
       </c>
-      <c r="C12" s="33">
+      <c r="C12" s="32">
         <v>0</v>
       </c>
-      <c r="D12" s="39">
+      <c r="D12" s="38">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="E12" s="69"/>
-      <c r="F12" s="5"/>
+      <c r="E12" s="65"/>
+      <c r="F12" s="4"/>
     </row>
     <row r="13" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="66"/>
-      <c r="B13" s="32" t="s">
+      <c r="A13" s="62"/>
+      <c r="B13" s="31" t="s">
         <v>37</v>
       </c>
-      <c r="C13" s="33">
+      <c r="C13" s="32">
         <v>0</v>
       </c>
-      <c r="D13" s="39">
+      <c r="D13" s="38">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="E13" s="69"/>
-      <c r="F13" s="5"/>
+      <c r="E13" s="65"/>
+      <c r="F13" s="4"/>
     </row>
     <row r="14" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="67"/>
-      <c r="B14" s="30" t="s">
+      <c r="A14" s="63"/>
+      <c r="B14" s="29" t="s">
         <v>26</v>
       </c>
-      <c r="C14" s="31">
+      <c r="C14" s="30">
         <v>0</v>
       </c>
-      <c r="D14" s="40">
+      <c r="D14" s="39">
         <f>(C14/2)*100</f>
         <v>0</v>
       </c>
-      <c r="E14" s="70"/>
-      <c r="F14" s="5"/>
+      <c r="E14" s="66"/>
+      <c r="F14" s="4"/>
     </row>
     <row r="15" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="25"/>
-      <c r="B15" s="26"/>
-      <c r="C15" s="27"/>
-      <c r="D15" s="41"/>
-      <c r="E15" s="45"/>
-      <c r="F15" s="5"/>
+      <c r="A15" s="24"/>
+      <c r="B15" s="25"/>
+      <c r="C15" s="26"/>
+      <c r="D15" s="40"/>
+      <c r="E15" s="44"/>
+      <c r="F15" s="4"/>
     </row>
     <row r="16" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="23"/>
-      <c r="B16" s="6"/>
-      <c r="C16" s="7"/>
-      <c r="D16" s="42"/>
-      <c r="E16" s="46"/>
-      <c r="F16" s="5"/>
+      <c r="A16" s="22"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="41"/>
+      <c r="E16" s="45"/>
+      <c r="F16" s="4"/>
     </row>
     <row r="17" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="23"/>
-      <c r="B17" s="6"/>
-      <c r="C17" s="7"/>
-      <c r="D17" s="42"/>
-      <c r="E17" s="46"/>
-      <c r="F17" s="5"/>
+      <c r="A17" s="22"/>
+      <c r="B17" s="5"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="41"/>
+      <c r="E17" s="45"/>
+      <c r="F17" s="4"/>
     </row>
     <row r="18" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="23"/>
-      <c r="B18" s="6"/>
-      <c r="C18" s="7"/>
-      <c r="D18" s="42"/>
-      <c r="E18" s="46"/>
-      <c r="F18" s="5"/>
+      <c r="A18" s="22"/>
+      <c r="B18" s="5"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="41"/>
+      <c r="E18" s="45"/>
+      <c r="F18" s="4"/>
     </row>
     <row r="19" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="23"/>
-      <c r="B19" s="6"/>
-      <c r="C19" s="7"/>
-      <c r="D19" s="42"/>
-      <c r="E19" s="46"/>
-      <c r="F19" s="5"/>
+      <c r="A19" s="22"/>
+      <c r="B19" s="5"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="41"/>
+      <c r="E19" s="45"/>
+      <c r="F19" s="4"/>
     </row>
     <row r="20" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="23"/>
-      <c r="B20" s="6"/>
-      <c r="C20" s="7"/>
-      <c r="D20" s="42"/>
-      <c r="E20" s="46"/>
-      <c r="F20" s="5"/>
+      <c r="A20" s="22"/>
+      <c r="B20" s="5"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="41"/>
+      <c r="E20" s="45"/>
+      <c r="F20" s="4"/>
     </row>
     <row r="21" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="23"/>
-      <c r="B21" s="6"/>
-      <c r="C21" s="7"/>
-      <c r="D21" s="42"/>
-      <c r="E21" s="46"/>
-      <c r="F21" s="5"/>
+      <c r="A21" s="22"/>
+      <c r="B21" s="5"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="41"/>
+      <c r="E21" s="45"/>
+      <c r="F21" s="4"/>
     </row>
     <row r="22" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A22" s="23"/>
-      <c r="B22" s="6"/>
-      <c r="C22" s="7"/>
-      <c r="D22" s="42"/>
-      <c r="E22" s="46"/>
-      <c r="F22" s="5"/>
+      <c r="A22" s="22"/>
+      <c r="B22" s="5"/>
+      <c r="C22" s="6"/>
+      <c r="D22" s="41"/>
+      <c r="E22" s="45"/>
+      <c r="F22" s="4"/>
     </row>
     <row r="23" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A23" s="23"/>
-      <c r="B23" s="6"/>
-      <c r="C23" s="7"/>
-      <c r="D23" s="42"/>
-      <c r="E23" s="46"/>
-      <c r="F23" s="5"/>
+      <c r="A23" s="22"/>
+      <c r="B23" s="5"/>
+      <c r="C23" s="6"/>
+      <c r="D23" s="41"/>
+      <c r="E23" s="45"/>
+      <c r="F23" s="4"/>
     </row>
     <row r="24" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A24" s="23"/>
-      <c r="B24" s="6"/>
-      <c r="C24" s="7"/>
-      <c r="D24" s="42"/>
-      <c r="E24" s="46"/>
-      <c r="F24" s="5"/>
+      <c r="A24" s="22"/>
+      <c r="B24" s="5"/>
+      <c r="C24" s="6"/>
+      <c r="D24" s="41"/>
+      <c r="E24" s="45"/>
+      <c r="F24" s="4"/>
     </row>
     <row r="25" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A25" s="23"/>
-      <c r="B25" s="6"/>
-      <c r="C25" s="7"/>
-      <c r="D25" s="42"/>
-      <c r="E25" s="46"/>
-      <c r="F25" s="5"/>
+      <c r="A25" s="22"/>
+      <c r="B25" s="5"/>
+      <c r="C25" s="6"/>
+      <c r="D25" s="41"/>
+      <c r="E25" s="45"/>
+      <c r="F25" s="4"/>
     </row>
     <row r="26" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A26" s="23"/>
-      <c r="B26" s="6"/>
-      <c r="C26" s="7"/>
-      <c r="D26" s="42"/>
-      <c r="E26" s="46"/>
-      <c r="F26" s="5"/>
+      <c r="A26" s="22"/>
+      <c r="B26" s="5"/>
+      <c r="C26" s="6"/>
+      <c r="D26" s="41"/>
+      <c r="E26" s="45"/>
+      <c r="F26" s="4"/>
     </row>
     <row r="27" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A27" s="23"/>
-      <c r="B27" s="6"/>
-      <c r="C27" s="7"/>
-      <c r="D27" s="42"/>
-      <c r="E27" s="46"/>
-      <c r="F27" s="5"/>
+      <c r="A27" s="22"/>
+      <c r="B27" s="5"/>
+      <c r="C27" s="6"/>
+      <c r="D27" s="41"/>
+      <c r="E27" s="45"/>
+      <c r="F27" s="4"/>
     </row>
     <row r="28" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A28" s="23"/>
-      <c r="B28" s="6"/>
-      <c r="C28" s="7"/>
-      <c r="D28" s="42"/>
-      <c r="E28" s="46"/>
-      <c r="F28" s="5"/>
+      <c r="A28" s="22"/>
+      <c r="B28" s="5"/>
+      <c r="C28" s="6"/>
+      <c r="D28" s="41"/>
+      <c r="E28" s="45"/>
+      <c r="F28" s="4"/>
     </row>
     <row r="29" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A29" s="23"/>
-      <c r="B29" s="6"/>
-      <c r="C29" s="7"/>
-      <c r="D29" s="42"/>
-      <c r="E29" s="46"/>
-      <c r="F29" s="5"/>
+      <c r="A29" s="22"/>
+      <c r="B29" s="5"/>
+      <c r="C29" s="6"/>
+      <c r="D29" s="41"/>
+      <c r="E29" s="45"/>
+      <c r="F29" s="4"/>
     </row>
     <row r="30" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A30" s="23"/>
-      <c r="B30" s="6"/>
-      <c r="C30" s="7"/>
-      <c r="D30" s="42"/>
-      <c r="E30" s="46"/>
-      <c r="F30" s="5"/>
+      <c r="A30" s="22"/>
+      <c r="B30" s="5"/>
+      <c r="C30" s="6"/>
+      <c r="D30" s="41"/>
+      <c r="E30" s="45"/>
+      <c r="F30" s="4"/>
     </row>
     <row r="31" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A31" s="23"/>
-      <c r="B31" s="6"/>
-      <c r="C31" s="7"/>
-      <c r="D31" s="42"/>
-      <c r="E31" s="46"/>
-      <c r="F31" s="5"/>
+      <c r="A31" s="22"/>
+      <c r="B31" s="5"/>
+      <c r="C31" s="6"/>
+      <c r="D31" s="41"/>
+      <c r="E31" s="45"/>
+      <c r="F31" s="4"/>
     </row>
     <row r="32" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A32" s="23"/>
-      <c r="B32" s="6"/>
-      <c r="C32" s="7"/>
-      <c r="D32" s="42"/>
-      <c r="E32" s="46"/>
-      <c r="F32" s="5"/>
+      <c r="A32" s="22"/>
+      <c r="B32" s="5"/>
+      <c r="C32" s="6"/>
+      <c r="D32" s="41"/>
+      <c r="E32" s="45"/>
+      <c r="F32" s="4"/>
     </row>
     <row r="33" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A33" s="23"/>
-      <c r="B33" s="6"/>
-      <c r="C33" s="7"/>
-      <c r="D33" s="42"/>
-      <c r="E33" s="46"/>
-      <c r="F33" s="5"/>
+      <c r="A33" s="22"/>
+      <c r="B33" s="5"/>
+      <c r="C33" s="6"/>
+      <c r="D33" s="41"/>
+      <c r="E33" s="45"/>
+      <c r="F33" s="4"/>
     </row>
     <row r="34" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A34" s="23"/>
-      <c r="B34" s="6"/>
-      <c r="C34" s="7"/>
-      <c r="D34" s="42"/>
-      <c r="E34" s="46"/>
-      <c r="F34" s="5"/>
+      <c r="A34" s="22"/>
+      <c r="B34" s="5"/>
+      <c r="C34" s="6"/>
+      <c r="D34" s="41"/>
+      <c r="E34" s="45"/>
+      <c r="F34" s="4"/>
     </row>
     <row r="35" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A35" s="23"/>
-      <c r="B35" s="6"/>
-      <c r="C35" s="7"/>
-      <c r="D35" s="42"/>
-      <c r="E35" s="46"/>
-      <c r="F35" s="5"/>
+      <c r="A35" s="22"/>
+      <c r="B35" s="5"/>
+      <c r="C35" s="6"/>
+      <c r="D35" s="41"/>
+      <c r="E35" s="45"/>
+      <c r="F35" s="4"/>
     </row>
     <row r="36" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A36" s="23"/>
-      <c r="B36" s="6"/>
-      <c r="C36" s="7"/>
-      <c r="D36" s="42"/>
-      <c r="E36" s="46"/>
-      <c r="F36" s="5"/>
+      <c r="A36" s="22"/>
+      <c r="B36" s="5"/>
+      <c r="C36" s="6"/>
+      <c r="D36" s="41"/>
+      <c r="E36" s="45"/>
+      <c r="F36" s="4"/>
     </row>
     <row r="37" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A37" s="23"/>
-      <c r="B37" s="6"/>
-      <c r="C37" s="7"/>
-      <c r="D37" s="42"/>
-      <c r="E37" s="46"/>
-      <c r="F37" s="5"/>
+      <c r="A37" s="22"/>
+      <c r="B37" s="5"/>
+      <c r="C37" s="6"/>
+      <c r="D37" s="41"/>
+      <c r="E37" s="45"/>
+      <c r="F37" s="4"/>
     </row>
     <row r="38" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A38" s="23"/>
-      <c r="B38" s="6"/>
-      <c r="C38" s="7"/>
-      <c r="D38" s="42"/>
-      <c r="E38" s="46"/>
-      <c r="F38" s="5"/>
+      <c r="A38" s="22"/>
+      <c r="B38" s="5"/>
+      <c r="C38" s="6"/>
+      <c r="D38" s="41"/>
+      <c r="E38" s="45"/>
+      <c r="F38" s="4"/>
     </row>
     <row r="39" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A39" s="23"/>
-      <c r="B39" s="6"/>
-      <c r="C39" s="7"/>
-      <c r="D39" s="42"/>
-      <c r="E39" s="46"/>
-      <c r="F39" s="5"/>
+      <c r="A39" s="22"/>
+      <c r="B39" s="5"/>
+      <c r="C39" s="6"/>
+      <c r="D39" s="41"/>
+      <c r="E39" s="45"/>
+      <c r="F39" s="4"/>
     </row>
     <row r="40" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="24"/>
-      <c r="B40" s="16"/>
-      <c r="C40" s="15"/>
-      <c r="D40" s="43"/>
-      <c r="E40" s="47"/>
-      <c r="F40" s="5"/>
+      <c r="A40" s="23"/>
+      <c r="B40" s="15"/>
+      <c r="C40" s="14"/>
+      <c r="D40" s="42"/>
+      <c r="E40" s="46"/>
+      <c r="F40" s="4"/>
     </row>
     <row r="41" spans="1:6" ht="24" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="56" t="s">
+      <c r="A41" s="52" t="s">
         <v>27</v>
       </c>
-      <c r="B41" s="57"/>
-      <c r="C41" s="57"/>
-      <c r="D41" s="58"/>
-      <c r="E41" s="48">
+      <c r="B41" s="53"/>
+      <c r="C41" s="53"/>
+      <c r="D41" s="54"/>
+      <c r="E41" s="47">
         <f>(AVERAGE(E2,E5))</f>
         <v>33.333333333333329</v>
       </c>
-      <c r="F41" s="5"/>
+      <c r="F41" s="4"/>
     </row>
     <row r="42" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A42" s="5"/>
-      <c r="B42" s="4"/>
-      <c r="C42" s="5"/>
-      <c r="D42" s="5"/>
-      <c r="E42" s="5"/>
-      <c r="F42" s="5"/>
+      <c r="A42" s="4"/>
+      <c r="B42" s="3"/>
+      <c r="C42" s="4"/>
+      <c r="D42" s="4"/>
+      <c r="E42" s="4"/>
+      <c r="F42" s="4"/>
     </row>
     <row r="43" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A43" s="5"/>
-      <c r="B43" s="4"/>
-      <c r="C43" s="5"/>
-      <c r="D43" s="5"/>
-      <c r="E43" s="5"/>
-      <c r="F43" s="5"/>
+      <c r="A43" s="4"/>
+      <c r="B43" s="3"/>
+      <c r="C43" s="4"/>
+      <c r="D43" s="4"/>
+      <c r="E43" s="4"/>
+      <c r="F43" s="4"/>
     </row>
     <row r="44" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A44" s="5"/>
-      <c r="B44" s="4"/>
-      <c r="C44" s="5"/>
-      <c r="D44" s="5"/>
-      <c r="E44" s="5"/>
-      <c r="F44" s="5"/>
+      <c r="A44" s="4"/>
+      <c r="B44" s="3"/>
+      <c r="C44" s="4"/>
+      <c r="D44" s="4"/>
+      <c r="E44" s="4"/>
+      <c r="F44" s="4"/>
     </row>
     <row r="45" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A45" s="5"/>
-      <c r="B45" s="4"/>
-      <c r="C45" s="5"/>
-      <c r="D45" s="5"/>
-      <c r="E45" s="5"/>
-      <c r="F45" s="5"/>
+      <c r="A45" s="4"/>
+      <c r="B45" s="3"/>
+      <c r="C45" s="4"/>
+      <c r="D45" s="4"/>
+      <c r="E45" s="4"/>
+      <c r="F45" s="4"/>
     </row>
     <row r="46" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A46" s="5"/>
-      <c r="B46" s="4"/>
-      <c r="C46" s="5"/>
-      <c r="D46" s="5"/>
-      <c r="E46" s="5"/>
-      <c r="F46" s="5"/>
+      <c r="A46" s="4"/>
+      <c r="B46" s="3"/>
+      <c r="C46" s="4"/>
+      <c r="D46" s="4"/>
+      <c r="E46" s="4"/>
+      <c r="F46" s="4"/>
     </row>
     <row r="47" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A47" s="5"/>
-      <c r="B47" s="4"/>
-      <c r="C47" s="5"/>
-      <c r="D47" s="5"/>
-      <c r="E47" s="5"/>
-      <c r="F47" s="5"/>
+      <c r="A47" s="4"/>
+      <c r="B47" s="3"/>
+      <c r="C47" s="4"/>
+      <c r="D47" s="4"/>
+      <c r="E47" s="4"/>
+      <c r="F47" s="4"/>
     </row>
     <row r="48" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A48" s="5"/>
-      <c r="B48" s="4"/>
-      <c r="C48" s="5"/>
-      <c r="D48" s="5"/>
-      <c r="E48" s="5"/>
-      <c r="F48" s="5"/>
+      <c r="A48" s="4"/>
+      <c r="B48" s="3"/>
+      <c r="C48" s="4"/>
+      <c r="D48" s="4"/>
+      <c r="E48" s="4"/>
+      <c r="F48" s="4"/>
     </row>
     <row r="49" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A49" s="5"/>
-      <c r="B49" s="4"/>
-      <c r="C49" s="5"/>
-      <c r="D49" s="5"/>
-      <c r="E49" s="5"/>
-      <c r="F49" s="5"/>
+      <c r="A49" s="4"/>
+      <c r="B49" s="3"/>
+      <c r="C49" s="4"/>
+      <c r="D49" s="4"/>
+      <c r="E49" s="4"/>
+      <c r="F49" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -2436,68 +2779,68 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:4" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="C2" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="D2" s="12" t="s">
+      <c r="D2" s="11" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B3" s="13" t="s">
+      <c r="B3" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="C3" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="14" t="s">
+      <c r="D3" s="13" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="11" t="s">
+      <c r="C4" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="10" t="s">
+      <c r="D4" s="9" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B5" s="13" t="s">
+      <c r="B5" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="13" t="s">
+      <c r="C5" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="14" t="s">
+      <c r="D5" s="13" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B6" s="11" t="s">
+      <c r="B6" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="11" t="s">
+      <c r="C6" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="10" t="s">
+      <c r="D6" s="9" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B7" s="13" t="s">
+      <c r="B7" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="13" t="s">
+      <c r="C7" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="D7" s="14" t="s">
+      <c r="D7" s="13" t="s">
         <v>20</v>
       </c>
     </row>

</xml_diff>

<commit_message>
5th commit - Workplan - Day1
</commit_message>
<xml_diff>
--- a/Workplan.xlsx
+++ b/Workplan.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="68">
   <si>
     <t>ACTIVITIES</t>
   </si>
@@ -297,6 +297,12 @@
       </rPr>
       <t xml:space="preserve"> Bianca Denise A. Del Puerto   Angela Lynne G. Lapus</t>
     </r>
+  </si>
+  <si>
+    <t>Environment Setup (Cloud Formation)</t>
+  </si>
+  <si>
+    <t>In Progress</t>
   </si>
 </sst>
 </file>
@@ -444,7 +450,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="32">
+  <borders count="35">
     <border>
       <left/>
       <right/>
@@ -875,6 +881,43 @@
         <color indexed="64"/>
       </top>
       <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -1031,57 +1074,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="3" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="3" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="3" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="5" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1091,29 +1083,8 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="8" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1136,12 +1107,6 @@
     <xf numFmtId="0" fontId="7" fillId="8" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="8" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1176,12 +1141,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="6"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1214,39 +1173,123 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="8" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="3" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="3" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="3" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="5" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="8" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1551,8 +1594,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I45"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G43" sqref="G43"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1569,30 +1612,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="48" customFormat="1" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="67" t="s">
+      <c r="A1" s="102" t="s">
         <v>64</v>
       </c>
-      <c r="B1" s="67"/>
-      <c r="C1" s="67"/>
-      <c r="D1" s="67"/>
-      <c r="E1" s="67"/>
-      <c r="F1" s="67"/>
-      <c r="G1" s="67"/>
-      <c r="H1" s="67"/>
-      <c r="I1" s="67"/>
+      <c r="B1" s="102"/>
+      <c r="C1" s="102"/>
+      <c r="D1" s="102"/>
+      <c r="E1" s="102"/>
+      <c r="F1" s="102"/>
+      <c r="G1" s="102"/>
+      <c r="H1" s="102"/>
+      <c r="I1" s="102"/>
     </row>
     <row r="2" spans="1:9" s="48" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A2" s="51" t="s">
+      <c r="A2" s="111" t="s">
         <v>45</v>
       </c>
-      <c r="B2" s="51"/>
-      <c r="C2" s="51"/>
-      <c r="D2" s="51"/>
-      <c r="E2" s="51"/>
-      <c r="F2" s="51"/>
-      <c r="G2" s="51"/>
-      <c r="H2" s="51"/>
-      <c r="I2" s="51"/>
+      <c r="B2" s="111"/>
+      <c r="C2" s="111"/>
+      <c r="D2" s="111"/>
+      <c r="E2" s="111"/>
+      <c r="F2" s="111"/>
+      <c r="G2" s="111"/>
+      <c r="H2" s="111"/>
+      <c r="I2" s="111"/>
     </row>
     <row r="3" spans="1:9" s="48" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="49"/>
@@ -1606,602 +1649,662 @@
     </row>
     <row r="4" spans="1:9" s="48" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="77" t="s">
+      <c r="A5" s="112" t="s">
         <v>49</v>
       </c>
-      <c r="B5" s="77" t="s">
+      <c r="B5" s="112" t="s">
         <v>38</v>
       </c>
-      <c r="C5" s="109" t="s">
+      <c r="C5" s="108" t="s">
         <v>40</v>
       </c>
-      <c r="D5" s="73" t="s">
+      <c r="D5" s="106" t="s">
         <v>41</v>
       </c>
-      <c r="E5" s="109" t="s">
+      <c r="E5" s="108" t="s">
         <v>42</v>
       </c>
-      <c r="F5" s="73" t="s">
+      <c r="F5" s="106" t="s">
         <v>43</v>
       </c>
-      <c r="G5" s="94" t="s">
+      <c r="G5" s="104" t="s">
         <v>60</v>
       </c>
-      <c r="H5" s="94" t="s">
+      <c r="H5" s="104" t="s">
         <v>44</v>
       </c>
-      <c r="I5" s="94" t="s">
+      <c r="I5" s="104" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="78"/>
-      <c r="B6" s="78"/>
-      <c r="C6" s="110"/>
-      <c r="D6" s="76"/>
-      <c r="E6" s="110"/>
-      <c r="F6" s="76"/>
-      <c r="G6" s="95"/>
-      <c r="H6" s="95"/>
-      <c r="I6" s="95"/>
+      <c r="A6" s="113"/>
+      <c r="B6" s="113"/>
+      <c r="C6" s="109"/>
+      <c r="D6" s="107"/>
+      <c r="E6" s="109"/>
+      <c r="F6" s="107"/>
+      <c r="G6" s="105"/>
+      <c r="H6" s="105"/>
+      <c r="I6" s="105"/>
     </row>
     <row r="7" spans="1:9" s="48" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="81">
+      <c r="A7" s="114">
         <v>1</v>
       </c>
-      <c r="B7" s="85" t="s">
+      <c r="B7" s="61" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="111"/>
-      <c r="D7" s="82"/>
-      <c r="E7" s="111"/>
-      <c r="F7" s="82"/>
-      <c r="G7" s="96"/>
-      <c r="H7" s="96"/>
-      <c r="I7" s="96"/>
+      <c r="C7" s="83"/>
+      <c r="D7" s="58"/>
+      <c r="E7" s="83"/>
+      <c r="F7" s="58"/>
+      <c r="G7" s="70"/>
+      <c r="H7" s="70"/>
+      <c r="I7" s="70"/>
     </row>
     <row r="8" spans="1:9" ht="75" x14ac:dyDescent="0.25">
-      <c r="A8" s="79"/>
-      <c r="B8" s="86" t="s">
+      <c r="A8" s="115"/>
+      <c r="B8" s="62" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="112">
-        <v>42565</v>
-      </c>
-      <c r="D8" s="113">
-        <v>42565</v>
-      </c>
-      <c r="E8" s="112">
-        <v>42565</v>
-      </c>
-      <c r="F8" s="113">
-        <v>42565</v>
-      </c>
-      <c r="G8" s="100">
+      <c r="C8" s="84">
+        <v>42565</v>
+      </c>
+      <c r="D8" s="85">
+        <v>42565</v>
+      </c>
+      <c r="E8" s="84">
+        <v>42565</v>
+      </c>
+      <c r="F8" s="85">
+        <v>42565</v>
+      </c>
+      <c r="G8" s="74">
         <v>100</v>
       </c>
-      <c r="H8" s="104" t="s">
+      <c r="H8" s="78" t="s">
         <v>48</v>
       </c>
-      <c r="I8" s="97" t="s">
+      <c r="I8" s="71" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="79"/>
-      <c r="B9" s="87" t="s">
+      <c r="A9" s="115"/>
+      <c r="B9" s="63" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="112">
-        <v>42565</v>
-      </c>
-      <c r="D9" s="113">
-        <v>42565</v>
-      </c>
-      <c r="E9" s="112">
-        <v>42565</v>
-      </c>
-      <c r="F9" s="113">
-        <v>42565</v>
-      </c>
-      <c r="G9" s="100">
+      <c r="C9" s="84">
+        <v>42565</v>
+      </c>
+      <c r="D9" s="85">
+        <v>42565</v>
+      </c>
+      <c r="E9" s="84">
+        <v>42565</v>
+      </c>
+      <c r="F9" s="85">
+        <v>42565</v>
+      </c>
+      <c r="G9" s="74">
         <v>100</v>
       </c>
-      <c r="H9" s="104" t="s">
+      <c r="H9" s="78" t="s">
         <v>48</v>
       </c>
-      <c r="I9" s="92"/>
+      <c r="I9" s="68"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="79"/>
-      <c r="B10" s="87" t="s">
+      <c r="A10" s="115"/>
+      <c r="B10" s="63" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="112">
-        <v>42565</v>
-      </c>
-      <c r="D10" s="113">
-        <v>42565</v>
-      </c>
-      <c r="E10" s="112">
-        <v>42565</v>
-      </c>
-      <c r="F10" s="113">
-        <v>42565</v>
-      </c>
-      <c r="G10" s="100">
+      <c r="C10" s="84">
+        <v>42565</v>
+      </c>
+      <c r="D10" s="85">
+        <v>42565</v>
+      </c>
+      <c r="E10" s="84">
+        <v>42565</v>
+      </c>
+      <c r="F10" s="85">
+        <v>42565</v>
+      </c>
+      <c r="G10" s="74">
         <v>100</v>
       </c>
-      <c r="H10" s="104" t="s">
+      <c r="H10" s="78" t="s">
         <v>48</v>
       </c>
-      <c r="I10" s="92"/>
+      <c r="I10" s="68"/>
     </row>
     <row r="11" spans="1:9" s="50" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="79"/>
-      <c r="B11" s="88" t="s">
-        <v>7</v>
-      </c>
-      <c r="C11" s="114"/>
-      <c r="D11" s="115"/>
-      <c r="E11" s="114"/>
-      <c r="F11" s="115"/>
-      <c r="G11" s="101"/>
-      <c r="H11" s="105"/>
-      <c r="I11" s="98"/>
+      <c r="A11" s="115"/>
+      <c r="B11" s="64" t="s">
+        <v>66</v>
+      </c>
+      <c r="C11" s="86"/>
+      <c r="D11" s="87"/>
+      <c r="E11" s="132">
+        <v>42565</v>
+      </c>
+      <c r="F11" s="87"/>
+      <c r="G11" s="75"/>
+      <c r="H11" s="79"/>
+      <c r="I11" s="72"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="79"/>
-      <c r="B12" s="87" t="s">
+      <c r="A12" s="115"/>
+      <c r="B12" s="63" t="s">
         <v>29</v>
       </c>
-      <c r="C12" s="112">
-        <v>42565</v>
-      </c>
-      <c r="D12" s="113">
-        <v>42565</v>
-      </c>
-      <c r="E12" s="112"/>
-      <c r="F12" s="124"/>
-      <c r="G12" s="100"/>
-      <c r="H12" s="100"/>
-      <c r="I12" s="92"/>
+      <c r="C12" s="133"/>
+      <c r="D12" s="134"/>
+      <c r="E12" s="134"/>
+      <c r="F12" s="134"/>
+      <c r="G12" s="134"/>
+      <c r="H12" s="134"/>
+      <c r="I12" s="135"/>
     </row>
     <row r="13" spans="1:9" s="48" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="79"/>
-      <c r="B13" s="108" t="s">
+      <c r="A13" s="115"/>
+      <c r="B13" s="82" t="s">
         <v>30</v>
       </c>
-      <c r="C13" s="112">
-        <v>42565</v>
-      </c>
-      <c r="D13" s="113">
-        <v>42565</v>
-      </c>
-      <c r="E13" s="112"/>
-      <c r="F13" s="124"/>
-      <c r="G13" s="100"/>
-      <c r="H13" s="100"/>
-      <c r="I13" s="92"/>
+      <c r="C13" s="84">
+        <v>42565</v>
+      </c>
+      <c r="D13" s="85">
+        <v>42565</v>
+      </c>
+      <c r="E13" s="84">
+        <v>42565</v>
+      </c>
+      <c r="F13" s="84">
+        <v>42565</v>
+      </c>
+      <c r="G13" s="74">
+        <v>100</v>
+      </c>
+      <c r="H13" s="78" t="s">
+        <v>48</v>
+      </c>
+      <c r="I13" s="68"/>
     </row>
     <row r="14" spans="1:9" s="48" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="79"/>
-      <c r="B14" s="108" t="s">
+      <c r="A14" s="115"/>
+      <c r="B14" s="82" t="s">
         <v>31</v>
       </c>
-      <c r="C14" s="112">
-        <v>42565</v>
-      </c>
-      <c r="D14" s="113">
-        <v>42565</v>
-      </c>
-      <c r="E14" s="112"/>
-      <c r="F14" s="124"/>
-      <c r="G14" s="100"/>
-      <c r="H14" s="100"/>
-      <c r="I14" s="92"/>
+      <c r="C14" s="84">
+        <v>42565</v>
+      </c>
+      <c r="D14" s="85">
+        <v>42565</v>
+      </c>
+      <c r="E14" s="84">
+        <v>42565</v>
+      </c>
+      <c r="F14" s="84">
+        <v>42565</v>
+      </c>
+      <c r="G14" s="74">
+        <v>100</v>
+      </c>
+      <c r="H14" s="78" t="s">
+        <v>48</v>
+      </c>
+      <c r="I14" s="68"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="79"/>
-      <c r="B15" s="108" t="s">
+      <c r="A15" s="115"/>
+      <c r="B15" s="82" t="s">
         <v>35</v>
       </c>
-      <c r="C15" s="112">
-        <v>42565</v>
-      </c>
-      <c r="D15" s="113">
-        <v>42565</v>
-      </c>
-      <c r="E15" s="125"/>
-      <c r="F15" s="124"/>
-      <c r="G15" s="100"/>
-      <c r="H15" s="100"/>
-      <c r="I15" s="92"/>
+      <c r="C15" s="84">
+        <v>42565</v>
+      </c>
+      <c r="D15" s="85">
+        <v>42565</v>
+      </c>
+      <c r="E15" s="84">
+        <v>42565</v>
+      </c>
+      <c r="F15" s="84">
+        <v>42565</v>
+      </c>
+      <c r="G15" s="74">
+        <v>100</v>
+      </c>
+      <c r="H15" s="78" t="s">
+        <v>48</v>
+      </c>
+      <c r="I15" s="68"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="79"/>
-      <c r="B16" s="108" t="s">
+      <c r="A16" s="115"/>
+      <c r="B16" s="82" t="s">
         <v>36</v>
       </c>
-      <c r="C16" s="112">
-        <v>42565</v>
-      </c>
-      <c r="D16" s="113">
-        <v>42565</v>
-      </c>
-      <c r="E16" s="125"/>
-      <c r="F16" s="124"/>
-      <c r="G16" s="100"/>
-      <c r="H16" s="100"/>
-      <c r="I16" s="92"/>
+      <c r="C16" s="84">
+        <v>42565</v>
+      </c>
+      <c r="D16" s="85">
+        <v>42565</v>
+      </c>
+      <c r="E16" s="84">
+        <v>42565</v>
+      </c>
+      <c r="F16" s="84">
+        <v>42565</v>
+      </c>
+      <c r="G16" s="74">
+        <v>100</v>
+      </c>
+      <c r="H16" s="78" t="s">
+        <v>48</v>
+      </c>
+      <c r="I16" s="68"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="79"/>
-      <c r="B17" s="108" t="s">
+      <c r="A17" s="115"/>
+      <c r="B17" s="82" t="s">
         <v>37</v>
       </c>
-      <c r="C17" s="112">
-        <v>42565</v>
-      </c>
-      <c r="D17" s="113">
-        <v>42565</v>
-      </c>
-      <c r="E17" s="125"/>
-      <c r="F17" s="124"/>
-      <c r="G17" s="100"/>
-      <c r="H17" s="100"/>
-      <c r="I17" s="92"/>
+      <c r="C17" s="84">
+        <v>42565</v>
+      </c>
+      <c r="D17" s="85">
+        <v>42565</v>
+      </c>
+      <c r="E17" s="84">
+        <v>42565</v>
+      </c>
+      <c r="F17" s="84">
+        <v>42565</v>
+      </c>
+      <c r="G17" s="74">
+        <v>100</v>
+      </c>
+      <c r="H17" s="78" t="s">
+        <v>48</v>
+      </c>
+      <c r="I17" s="68"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="79"/>
-      <c r="B18" s="87" t="s">
+      <c r="A18" s="115"/>
+      <c r="B18" s="63" t="s">
         <v>26</v>
       </c>
-      <c r="C18" s="112">
-        <v>42565</v>
-      </c>
-      <c r="D18" s="113">
-        <v>42565</v>
-      </c>
-      <c r="E18" s="125"/>
-      <c r="F18" s="124"/>
-      <c r="G18" s="100"/>
-      <c r="H18" s="100"/>
-      <c r="I18" s="92"/>
+      <c r="C18" s="84">
+        <v>42565</v>
+      </c>
+      <c r="D18" s="85">
+        <v>42565</v>
+      </c>
+      <c r="E18" s="84">
+        <v>42565</v>
+      </c>
+      <c r="F18" s="84">
+        <v>42565</v>
+      </c>
+      <c r="G18" s="74">
+        <v>100</v>
+      </c>
+      <c r="H18" s="78" t="s">
+        <v>48</v>
+      </c>
+      <c r="I18" s="68"/>
     </row>
     <row r="19" spans="1:9" s="50" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="79"/>
-      <c r="B19" s="89" t="s">
+      <c r="A19" s="115"/>
+      <c r="B19" s="65" t="s">
         <v>50</v>
       </c>
-      <c r="C19" s="114"/>
-      <c r="D19" s="115"/>
-      <c r="E19" s="126"/>
-      <c r="F19" s="127"/>
-      <c r="G19" s="101"/>
-      <c r="H19" s="101"/>
-      <c r="I19" s="98"/>
+      <c r="C19" s="86"/>
+      <c r="D19" s="87"/>
+      <c r="E19" s="96"/>
+      <c r="F19" s="97"/>
+      <c r="G19" s="75"/>
+      <c r="H19" s="75"/>
+      <c r="I19" s="72"/>
     </row>
     <row r="20" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="80"/>
-      <c r="B20" s="106" t="s">
+      <c r="A20" s="116"/>
+      <c r="B20" s="80" t="s">
         <v>51</v>
       </c>
-      <c r="C20" s="116">
-        <v>42565</v>
-      </c>
-      <c r="D20" s="117">
-        <v>42565</v>
-      </c>
-      <c r="E20" s="128"/>
-      <c r="F20" s="129"/>
-      <c r="G20" s="102"/>
-      <c r="H20" s="102"/>
-      <c r="I20" s="90"/>
+      <c r="C20" s="88">
+        <v>42565</v>
+      </c>
+      <c r="D20" s="89">
+        <v>42573</v>
+      </c>
+      <c r="E20" s="89">
+        <v>42565</v>
+      </c>
+      <c r="F20" s="89"/>
+      <c r="G20" s="76">
+        <v>50</v>
+      </c>
+      <c r="H20" s="76" t="s">
+        <v>67</v>
+      </c>
+      <c r="I20" s="66"/>
     </row>
     <row r="21" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="81">
+      <c r="A21" s="114">
         <v>2</v>
       </c>
-      <c r="B21" s="91" t="s">
+      <c r="B21" s="67" t="s">
         <v>52</v>
       </c>
-      <c r="C21" s="118"/>
-      <c r="D21" s="119"/>
-      <c r="E21" s="118"/>
-      <c r="F21" s="119"/>
-      <c r="G21" s="103"/>
-      <c r="H21" s="103"/>
-      <c r="I21" s="99"/>
+      <c r="C21" s="90"/>
+      <c r="D21" s="91"/>
+      <c r="E21" s="90"/>
+      <c r="F21" s="91"/>
+      <c r="G21" s="77"/>
+      <c r="H21" s="77"/>
+      <c r="I21" s="73"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="79"/>
-      <c r="B22" s="87" t="s">
+      <c r="A22" s="115"/>
+      <c r="B22" s="63" t="s">
         <v>53</v>
       </c>
-      <c r="C22" s="120"/>
-      <c r="D22" s="74"/>
-      <c r="E22" s="120"/>
-      <c r="F22" s="74"/>
-      <c r="G22" s="92"/>
-      <c r="H22" s="92"/>
-      <c r="I22" s="92"/>
+      <c r="C22" s="92"/>
+      <c r="D22" s="56"/>
+      <c r="E22" s="92"/>
+      <c r="F22" s="56"/>
+      <c r="G22" s="68"/>
+      <c r="H22" s="68"/>
+      <c r="I22" s="68"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="79"/>
-      <c r="B23" s="87" t="s">
+      <c r="A23" s="115"/>
+      <c r="B23" s="63" t="s">
         <v>54</v>
       </c>
-      <c r="C23" s="120"/>
-      <c r="D23" s="74"/>
-      <c r="E23" s="120"/>
-      <c r="F23" s="74"/>
-      <c r="G23" s="92"/>
-      <c r="H23" s="92"/>
-      <c r="I23" s="92"/>
+      <c r="C23" s="92"/>
+      <c r="D23" s="56"/>
+      <c r="E23" s="92"/>
+      <c r="F23" s="56"/>
+      <c r="G23" s="68"/>
+      <c r="H23" s="68"/>
+      <c r="I23" s="68"/>
     </row>
     <row r="24" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="80"/>
-      <c r="B24" s="106" t="s">
+      <c r="A24" s="116"/>
+      <c r="B24" s="80" t="s">
         <v>55</v>
       </c>
-      <c r="C24" s="121"/>
-      <c r="D24" s="75"/>
-      <c r="E24" s="121"/>
-      <c r="F24" s="75"/>
-      <c r="G24" s="90"/>
-      <c r="H24" s="90"/>
-      <c r="I24" s="90"/>
+      <c r="C24" s="93"/>
+      <c r="D24" s="57"/>
+      <c r="E24" s="93"/>
+      <c r="F24" s="57"/>
+      <c r="G24" s="66"/>
+      <c r="H24" s="66"/>
+      <c r="I24" s="66"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" s="81">
+      <c r="A25" s="114">
         <v>3</v>
       </c>
-      <c r="B25" s="107" t="s">
+      <c r="B25" s="81" t="s">
         <v>56</v>
       </c>
-      <c r="C25" s="122"/>
-      <c r="D25" s="84"/>
-      <c r="E25" s="122"/>
-      <c r="F25" s="84"/>
-      <c r="G25" s="93"/>
-      <c r="H25" s="93"/>
-      <c r="I25" s="93"/>
+      <c r="C25" s="94"/>
+      <c r="D25" s="60"/>
+      <c r="E25" s="94"/>
+      <c r="F25" s="60"/>
+      <c r="G25" s="69"/>
+      <c r="H25" s="69"/>
+      <c r="I25" s="69"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" s="79"/>
-      <c r="B26" s="87" t="s">
+      <c r="A26" s="115"/>
+      <c r="B26" s="63" t="s">
         <v>57</v>
       </c>
-      <c r="C26" s="120"/>
-      <c r="D26" s="74"/>
-      <c r="E26" s="120"/>
-      <c r="F26" s="74"/>
-      <c r="G26" s="92"/>
-      <c r="H26" s="92"/>
-      <c r="I26" s="92"/>
+      <c r="C26" s="92"/>
+      <c r="D26" s="56"/>
+      <c r="E26" s="92"/>
+      <c r="F26" s="56"/>
+      <c r="G26" s="68"/>
+      <c r="H26" s="68"/>
+      <c r="I26" s="68"/>
     </row>
     <row r="27" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="80"/>
-      <c r="B27" s="106" t="s">
+      <c r="A27" s="116"/>
+      <c r="B27" s="80" t="s">
         <v>58</v>
       </c>
-      <c r="C27" s="121"/>
-      <c r="D27" s="75"/>
-      <c r="E27" s="121"/>
-      <c r="F27" s="75"/>
-      <c r="G27" s="90"/>
-      <c r="H27" s="90"/>
-      <c r="I27" s="90"/>
+      <c r="C27" s="93"/>
+      <c r="D27" s="57"/>
+      <c r="E27" s="93"/>
+      <c r="F27" s="57"/>
+      <c r="G27" s="66"/>
+      <c r="H27" s="66"/>
+      <c r="I27" s="66"/>
     </row>
     <row r="28" spans="1:9" s="48" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A28" s="81">
+      <c r="A28" s="114">
         <v>4</v>
       </c>
-      <c r="B28" s="91" t="s">
+      <c r="B28" s="67" t="s">
         <v>59</v>
       </c>
-      <c r="C28" s="123"/>
-      <c r="D28" s="83"/>
-      <c r="E28" s="123"/>
-      <c r="F28" s="83"/>
-      <c r="G28" s="99"/>
-      <c r="H28" s="99"/>
-      <c r="I28" s="99"/>
+      <c r="C28" s="95"/>
+      <c r="D28" s="59"/>
+      <c r="E28" s="95"/>
+      <c r="F28" s="59"/>
+      <c r="G28" s="73"/>
+      <c r="H28" s="73"/>
+      <c r="I28" s="73"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="79"/>
-      <c r="B29" s="87" t="s">
+      <c r="A29" s="115"/>
+      <c r="B29" s="63" t="s">
         <v>62</v>
       </c>
-      <c r="C29" s="120"/>
-      <c r="D29" s="74"/>
-      <c r="E29" s="120"/>
-      <c r="F29" s="74"/>
-      <c r="G29" s="92"/>
-      <c r="H29" s="92"/>
-      <c r="I29" s="92"/>
+      <c r="C29" s="92"/>
+      <c r="D29" s="56"/>
+      <c r="E29" s="92"/>
+      <c r="F29" s="56"/>
+      <c r="G29" s="68"/>
+      <c r="H29" s="68"/>
+      <c r="I29" s="68"/>
     </row>
     <row r="30" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="80"/>
-      <c r="B30" s="106" t="s">
+      <c r="A30" s="116"/>
+      <c r="B30" s="80" t="s">
         <v>63</v>
       </c>
-      <c r="C30" s="121"/>
-      <c r="D30" s="75"/>
-      <c r="E30" s="121"/>
-      <c r="F30" s="75"/>
-      <c r="G30" s="90"/>
-      <c r="H30" s="90"/>
-      <c r="I30" s="90"/>
+      <c r="C30" s="93"/>
+      <c r="D30" s="57"/>
+      <c r="E30" s="93"/>
+      <c r="F30" s="57"/>
+      <c r="G30" s="66"/>
+      <c r="H30" s="66"/>
+      <c r="I30" s="66"/>
     </row>
     <row r="31" spans="1:9" s="48" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="68"/>
-      <c r="B31" s="69"/>
-      <c r="C31" s="69"/>
-      <c r="D31" s="69"/>
-      <c r="E31" s="69"/>
-      <c r="F31" s="69"/>
-      <c r="G31" s="69"/>
-      <c r="H31" s="69"/>
-      <c r="I31" s="69"/>
+      <c r="A31" s="51"/>
+      <c r="B31" s="52"/>
+      <c r="C31" s="52"/>
+      <c r="D31" s="52"/>
+      <c r="E31" s="52"/>
+      <c r="F31" s="52"/>
+      <c r="G31" s="52"/>
+      <c r="H31" s="52"/>
+      <c r="I31" s="52"/>
     </row>
     <row r="33" spans="2:9" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B33" s="130" t="s">
+      <c r="B33" s="98" t="s">
         <v>46</v>
       </c>
-      <c r="C33" s="71"/>
-      <c r="D33" s="71"/>
-      <c r="E33" s="71"/>
-      <c r="F33" s="71"/>
-      <c r="G33" s="130" t="s">
+      <c r="C33" s="54"/>
+      <c r="D33" s="54"/>
+      <c r="E33" s="54"/>
+      <c r="F33" s="54"/>
+      <c r="G33" s="98" t="s">
         <v>47</v>
       </c>
-      <c r="H33" s="71"/>
-      <c r="I33" s="71"/>
+      <c r="H33" s="54"/>
+      <c r="I33" s="54"/>
     </row>
     <row r="34" spans="2:9" s="48" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B34" s="70"/>
-      <c r="C34" s="71"/>
-      <c r="D34" s="71"/>
-      <c r="E34" s="71"/>
-      <c r="F34" s="71"/>
-      <c r="G34" s="70"/>
-      <c r="H34" s="71"/>
-      <c r="I34" s="71"/>
+      <c r="B34" s="53"/>
+      <c r="C34" s="54"/>
+      <c r="D34" s="54"/>
+      <c r="E34" s="54"/>
+      <c r="F34" s="54"/>
+      <c r="G34" s="53"/>
+      <c r="H34" s="54"/>
+      <c r="I34" s="54"/>
     </row>
     <row r="35" spans="2:9" s="48" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B35" s="70"/>
-      <c r="C35" s="71"/>
-      <c r="D35" s="71"/>
-      <c r="E35" s="71"/>
-      <c r="F35" s="71"/>
-      <c r="G35" s="71"/>
-      <c r="H35" s="71"/>
-      <c r="I35" s="71"/>
+      <c r="B35" s="53"/>
+      <c r="C35" s="54"/>
+      <c r="D35" s="54"/>
+      <c r="E35" s="54"/>
+      <c r="F35" s="54"/>
+      <c r="G35" s="54"/>
+      <c r="H35" s="54"/>
+      <c r="I35" s="54"/>
     </row>
     <row r="36" spans="2:9" s="48" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B36" s="133" t="s">
+      <c r="B36" s="100" t="s">
         <v>12</v>
       </c>
-      <c r="C36" s="134" t="s">
+      <c r="C36" s="103" t="s">
         <v>8</v>
       </c>
-      <c r="D36" s="134"/>
-      <c r="E36" s="134"/>
-      <c r="F36" s="71"/>
-      <c r="G36" s="70"/>
-      <c r="H36" s="135" t="s">
+      <c r="D36" s="103"/>
+      <c r="E36" s="103"/>
+      <c r="F36" s="54"/>
+      <c r="G36" s="53"/>
+      <c r="H36" s="101" t="s">
         <v>10</v>
       </c>
-      <c r="I36" s="71"/>
+      <c r="I36" s="54"/>
     </row>
     <row r="37" spans="2:9" s="48" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B37" s="131" t="s">
+      <c r="B37" s="99" t="s">
         <v>52</v>
       </c>
-      <c r="C37" s="132" t="s">
+      <c r="C37" s="110" t="s">
         <v>61</v>
       </c>
-      <c r="D37" s="132"/>
-      <c r="E37" s="132"/>
-      <c r="F37" s="71"/>
-      <c r="G37" s="71"/>
-      <c r="H37" s="131" t="s">
+      <c r="D37" s="110"/>
+      <c r="E37" s="110"/>
+      <c r="F37" s="54"/>
+      <c r="G37" s="54"/>
+      <c r="H37" s="99" t="s">
         <v>18</v>
       </c>
-      <c r="I37" s="71"/>
+      <c r="I37" s="54"/>
     </row>
     <row r="38" spans="2:9" s="48" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B38" s="72"/>
-      <c r="C38" s="72"/>
-      <c r="D38" s="72"/>
-      <c r="E38" s="72"/>
-      <c r="F38" s="71"/>
-      <c r="G38" s="71"/>
-      <c r="H38" s="72"/>
-      <c r="I38" s="71"/>
+      <c r="B38" s="55"/>
+      <c r="C38" s="55"/>
+      <c r="D38" s="55"/>
+      <c r="E38" s="55"/>
+      <c r="F38" s="54"/>
+      <c r="G38" s="54"/>
+      <c r="H38" s="55"/>
+      <c r="I38" s="54"/>
     </row>
     <row r="39" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B39" s="71"/>
-      <c r="C39" s="71"/>
-      <c r="D39" s="71"/>
-      <c r="E39" s="71"/>
-      <c r="F39" s="71"/>
-      <c r="G39" s="71"/>
-      <c r="H39" s="71"/>
-      <c r="I39" s="71"/>
+      <c r="B39" s="54"/>
+      <c r="C39" s="54"/>
+      <c r="D39" s="54"/>
+      <c r="E39" s="54"/>
+      <c r="F39" s="54"/>
+      <c r="G39" s="54"/>
+      <c r="H39" s="54"/>
+      <c r="I39" s="54"/>
     </row>
     <row r="40" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B40" s="133" t="s">
+      <c r="B40" s="100" t="s">
         <v>9</v>
       </c>
-      <c r="C40" s="134" t="s">
+      <c r="C40" s="103" t="s">
         <v>11</v>
       </c>
-      <c r="D40" s="134"/>
-      <c r="E40" s="134"/>
-      <c r="F40" s="71"/>
-      <c r="G40" s="71"/>
-      <c r="H40" s="71"/>
-      <c r="I40" s="71"/>
+      <c r="D40" s="103"/>
+      <c r="E40" s="103"/>
+      <c r="F40" s="54"/>
+      <c r="G40" s="54"/>
+      <c r="H40" s="54"/>
+      <c r="I40" s="54"/>
     </row>
     <row r="41" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B41" s="131" t="s">
+      <c r="B41" s="99" t="s">
         <v>20</v>
       </c>
-      <c r="C41" s="132" t="s">
+      <c r="C41" s="110" t="s">
         <v>20</v>
       </c>
-      <c r="D41" s="132"/>
-      <c r="E41" s="132"/>
-      <c r="F41" s="71"/>
-      <c r="G41" s="71"/>
-      <c r="H41" s="71"/>
-      <c r="I41" s="71"/>
+      <c r="D41" s="110"/>
+      <c r="E41" s="110"/>
+      <c r="F41" s="54"/>
+      <c r="G41" s="54"/>
+      <c r="H41" s="54"/>
+      <c r="I41" s="54"/>
     </row>
     <row r="42" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B42" s="71"/>
-      <c r="C42" s="71"/>
-      <c r="D42" s="71"/>
-      <c r="E42" s="71"/>
-      <c r="F42" s="71"/>
-      <c r="G42" s="71"/>
-      <c r="H42" s="71"/>
-      <c r="I42" s="71"/>
+      <c r="B42" s="54"/>
+      <c r="C42" s="54"/>
+      <c r="D42" s="54"/>
+      <c r="E42" s="54"/>
+      <c r="F42" s="54"/>
+      <c r="G42" s="54"/>
+      <c r="H42" s="54"/>
+      <c r="I42" s="54"/>
     </row>
     <row r="43" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B43" s="71"/>
-      <c r="C43" s="71"/>
-      <c r="D43" s="71"/>
-      <c r="E43" s="71"/>
-      <c r="F43" s="71"/>
-      <c r="G43" s="71"/>
-      <c r="H43" s="71"/>
-      <c r="I43" s="71"/>
+      <c r="B43" s="54"/>
+      <c r="C43" s="54"/>
+      <c r="D43" s="54"/>
+      <c r="E43" s="54"/>
+      <c r="F43" s="54"/>
+      <c r="G43" s="54"/>
+      <c r="H43" s="54"/>
+      <c r="I43" s="54"/>
     </row>
     <row r="44" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B44" s="71"/>
-      <c r="C44" s="71"/>
-      <c r="D44" s="71"/>
-      <c r="E44" s="71"/>
-      <c r="F44" s="71"/>
-      <c r="G44" s="71"/>
-      <c r="H44" s="71"/>
-      <c r="I44" s="71"/>
+      <c r="B44" s="54"/>
+      <c r="C44" s="54"/>
+      <c r="D44" s="54"/>
+      <c r="E44" s="54"/>
+      <c r="F44" s="54"/>
+      <c r="G44" s="54"/>
+      <c r="H44" s="54"/>
+      <c r="I44" s="54"/>
     </row>
     <row r="45" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B45" s="71"/>
-      <c r="C45" s="71"/>
-      <c r="D45" s="71"/>
-      <c r="E45" s="71"/>
-      <c r="F45" s="71"/>
-      <c r="G45" s="71"/>
-      <c r="H45" s="71"/>
-      <c r="I45" s="71"/>
+      <c r="B45" s="54"/>
+      <c r="C45" s="54"/>
+      <c r="D45" s="54"/>
+      <c r="E45" s="54"/>
+      <c r="F45" s="54"/>
+      <c r="G45" s="54"/>
+      <c r="H45" s="54"/>
+      <c r="I45" s="54"/>
     </row>
   </sheetData>
-  <mergeCells count="19">
+  <mergeCells count="20">
+    <mergeCell ref="C41:E41"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="I5:I6"/>
+    <mergeCell ref="A7:A20"/>
+    <mergeCell ref="A21:A24"/>
+    <mergeCell ref="A25:A27"/>
+    <mergeCell ref="A28:A30"/>
+    <mergeCell ref="C12:I12"/>
     <mergeCell ref="A1:I1"/>
     <mergeCell ref="C40:E40"/>
     <mergeCell ref="H5:H6"/>
@@ -2214,13 +2317,6 @@
     <mergeCell ref="C37:E37"/>
     <mergeCell ref="A2:I2"/>
     <mergeCell ref="A5:A6"/>
-    <mergeCell ref="C41:E41"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="I5:I6"/>
-    <mergeCell ref="A7:A20"/>
-    <mergeCell ref="A21:A24"/>
-    <mergeCell ref="A25:A27"/>
-    <mergeCell ref="A28:A30"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="1" bottom="1" header="0.3" footer="0.3"/>
   <pageSetup paperSize="5" orientation="landscape" r:id="rId1"/>
@@ -2263,7 +2359,7 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="55" t="s">
+      <c r="A2" s="120" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="16" t="s">
@@ -2276,14 +2372,14 @@
         <f>((C2/3)*100)</f>
         <v>33.333333333333329</v>
       </c>
-      <c r="E2" s="58">
+      <c r="E2" s="123">
         <f>(AVERAGE(C2:C4))*100</f>
         <v>66.666666666666657</v>
       </c>
       <c r="F2" s="4"/>
     </row>
     <row r="3" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="56"/>
+      <c r="A3" s="121"/>
       <c r="B3" s="7" t="s">
         <v>5</v>
       </c>
@@ -2294,11 +2390,11 @@
         <f t="shared" ref="D3:D4" si="0">((C3/3)*100)</f>
         <v>33.333333333333329</v>
       </c>
-      <c r="E3" s="59"/>
+      <c r="E3" s="124"/>
       <c r="F3" s="4"/>
     </row>
     <row r="4" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="57"/>
+      <c r="A4" s="122"/>
       <c r="B4" s="18" t="s">
         <v>6</v>
       </c>
@@ -2309,11 +2405,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E4" s="60"/>
+      <c r="E4" s="125"/>
       <c r="F4" s="4"/>
     </row>
     <row r="5" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="61" t="s">
+      <c r="A5" s="126" t="s">
         <v>7</v>
       </c>
       <c r="B5" s="27" t="s">
@@ -2324,14 +2420,14 @@
         <f>(AVERAGE(C6:C13)*100)*0.5</f>
         <v>0</v>
       </c>
-      <c r="E5" s="64">
+      <c r="E5" s="129">
         <f>D5+D14</f>
         <v>0</v>
       </c>
       <c r="F5" s="4"/>
     </row>
     <row r="6" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="62"/>
+      <c r="A6" s="127"/>
       <c r="B6" s="31" t="s">
         <v>30</v>
       </c>
@@ -2342,11 +2438,11 @@
         <f>(C6/8)*100</f>
         <v>0</v>
       </c>
-      <c r="E6" s="65"/>
+      <c r="E6" s="130"/>
       <c r="F6" s="4"/>
     </row>
     <row r="7" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="62"/>
+      <c r="A7" s="127"/>
       <c r="B7" s="31" t="s">
         <v>31</v>
       </c>
@@ -2357,11 +2453,11 @@
         <f t="shared" ref="D7:D13" si="1">(C7/8)*100</f>
         <v>0</v>
       </c>
-      <c r="E7" s="65"/>
+      <c r="E7" s="130"/>
       <c r="F7" s="4"/>
     </row>
     <row r="8" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="62"/>
+      <c r="A8" s="127"/>
       <c r="B8" s="31" t="s">
         <v>32</v>
       </c>
@@ -2372,11 +2468,11 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="E8" s="65"/>
+      <c r="E8" s="130"/>
       <c r="F8" s="4"/>
     </row>
     <row r="9" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="62"/>
+      <c r="A9" s="127"/>
       <c r="B9" s="31" t="s">
         <v>33</v>
       </c>
@@ -2387,11 +2483,11 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="E9" s="65"/>
+      <c r="E9" s="130"/>
       <c r="F9" s="4"/>
     </row>
     <row r="10" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="62"/>
+      <c r="A10" s="127"/>
       <c r="B10" s="31" t="s">
         <v>34</v>
       </c>
@@ -2402,11 +2498,11 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="E10" s="65"/>
+      <c r="E10" s="130"/>
       <c r="F10" s="4"/>
     </row>
     <row r="11" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="62"/>
+      <c r="A11" s="127"/>
       <c r="B11" s="31" t="s">
         <v>35</v>
       </c>
@@ -2417,11 +2513,11 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="E11" s="65"/>
+      <c r="E11" s="130"/>
       <c r="F11" s="4"/>
     </row>
     <row r="12" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="62"/>
+      <c r="A12" s="127"/>
       <c r="B12" s="31" t="s">
         <v>36</v>
       </c>
@@ -2432,11 +2528,11 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="E12" s="65"/>
+      <c r="E12" s="130"/>
       <c r="F12" s="4"/>
     </row>
     <row r="13" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="62"/>
+      <c r="A13" s="127"/>
       <c r="B13" s="31" t="s">
         <v>37</v>
       </c>
@@ -2447,11 +2543,11 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="E13" s="65"/>
+      <c r="E13" s="130"/>
       <c r="F13" s="4"/>
     </row>
     <row r="14" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="63"/>
+      <c r="A14" s="128"/>
       <c r="B14" s="29" t="s">
         <v>26</v>
       </c>
@@ -2462,7 +2558,7 @@
         <f>(C14/2)*100</f>
         <v>0</v>
       </c>
-      <c r="E14" s="66"/>
+      <c r="E14" s="131"/>
       <c r="F14" s="4"/>
     </row>
     <row r="15" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -2674,12 +2770,12 @@
       <c r="F40" s="4"/>
     </row>
     <row r="41" spans="1:6" ht="24" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="52" t="s">
+      <c r="A41" s="117" t="s">
         <v>27</v>
       </c>
-      <c r="B41" s="53"/>
-      <c r="C41" s="53"/>
-      <c r="D41" s="54"/>
+      <c r="B41" s="118"/>
+      <c r="C41" s="118"/>
+      <c r="D41" s="119"/>
       <c r="E41" s="47">
         <f>(AVERAGE(E2,E5))</f>
         <v>33.333333333333329</v>

</xml_diff>

<commit_message>
Sixth commit - Workplan - day 1
</commit_message>
<xml_diff>
--- a/Workplan.xlsx
+++ b/Workplan.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="75" windowWidth="18195" windowHeight="11820"/>
+    <workbookView xWindow="480" yWindow="75" windowWidth="18195" windowHeight="11820" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Work Plan" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="54">
   <si>
     <t>ACTIVITIES</t>
   </si>
@@ -112,15 +112,6 @@
   </si>
   <si>
     <t>Sonarqube</t>
-  </si>
-  <si>
-    <t>ELK</t>
-  </si>
-  <si>
-    <t>Sensu</t>
-  </si>
-  <si>
-    <t>Nexus</t>
   </si>
   <si>
     <t>Ansible</t>
@@ -256,6 +247,21 @@
   <si>
     <t>DAY</t>
   </si>
+  <si>
+    <t>Code Development</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coding the Javascript Calculator App </t>
+  </si>
+  <si>
+    <t>Commit project in the Gitlab Repo</t>
+  </si>
+  <si>
+    <t>Create Cartridges for Stack Spin up</t>
+  </si>
+  <si>
+    <t>CD - CI</t>
+  </si>
 </sst>
 </file>
 
@@ -308,7 +314,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -351,6 +357,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="41">
     <border>
@@ -890,7 +902,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="101">
+  <cellXfs count="106">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -968,9 +980,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1076,13 +1085,36 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1097,6 +1129,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -1142,42 +1192,19 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="8" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="8" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1483,13 +1510,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.42578125" style="49" customWidth="1"/>
+    <col min="1" max="1" width="7.42578125" style="48" customWidth="1"/>
     <col min="2" max="2" width="44" customWidth="1"/>
     <col min="3" max="3" width="10.28515625" customWidth="1"/>
     <col min="4" max="4" width="9.7109375" bestFit="1" customWidth="1"/>
@@ -1500,299 +1527,299 @@
     <col min="9" max="9" width="45.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="49" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B1" s="70" t="s">
+    <row r="1" spans="1:9" s="48" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B1" s="78" t="s">
+        <v>42</v>
+      </c>
+      <c r="C1" s="78"/>
+      <c r="D1" s="78"/>
+      <c r="E1" s="78"/>
+      <c r="F1" s="78"/>
+      <c r="G1" s="78"/>
+      <c r="H1" s="78"/>
+      <c r="I1" s="78"/>
+    </row>
+    <row r="2" spans="1:9" s="48" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="68" t="s">
+        <v>48</v>
+      </c>
+      <c r="B3" s="74" t="s">
+        <v>35</v>
+      </c>
+      <c r="C3" s="84" t="s">
+        <v>37</v>
+      </c>
+      <c r="D3" s="82" t="s">
+        <v>38</v>
+      </c>
+      <c r="E3" s="82" t="s">
+        <v>39</v>
+      </c>
+      <c r="F3" s="82" t="s">
+        <v>40</v>
+      </c>
+      <c r="G3" s="82" t="s">
         <v>45</v>
       </c>
-      <c r="C1" s="70"/>
-      <c r="D1" s="70"/>
-      <c r="E1" s="70"/>
-      <c r="F1" s="70"/>
-      <c r="G1" s="70"/>
-      <c r="H1" s="70"/>
-      <c r="I1" s="70"/>
-    </row>
-    <row r="2" spans="1:9" s="49" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="66" t="s">
-        <v>51</v>
-      </c>
-      <c r="B3" s="93" t="s">
-        <v>38</v>
-      </c>
-      <c r="C3" s="90" t="s">
-        <v>40</v>
-      </c>
-      <c r="D3" s="91" t="s">
+      <c r="H3" s="80" t="s">
         <v>41</v>
       </c>
-      <c r="E3" s="91" t="s">
-        <v>42</v>
-      </c>
-      <c r="F3" s="91" t="s">
-        <v>43</v>
-      </c>
-      <c r="G3" s="91" t="s">
-        <v>48</v>
-      </c>
-      <c r="H3" s="92" t="s">
-        <v>44</v>
-      </c>
-      <c r="I3" s="68" t="s">
-        <v>39</v>
+      <c r="I3" s="76" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="67"/>
-      <c r="B4" s="94"/>
-      <c r="C4" s="89"/>
-      <c r="D4" s="88"/>
-      <c r="E4" s="88"/>
-      <c r="F4" s="88"/>
-      <c r="G4" s="88"/>
-      <c r="H4" s="87"/>
-      <c r="I4" s="69"/>
+      <c r="A4" s="69"/>
+      <c r="B4" s="75"/>
+      <c r="C4" s="85"/>
+      <c r="D4" s="83"/>
+      <c r="E4" s="83"/>
+      <c r="F4" s="83"/>
+      <c r="G4" s="83"/>
+      <c r="H4" s="81"/>
+      <c r="I4" s="77"/>
     </row>
     <row r="5" spans="1:9" ht="83.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="98">
+      <c r="A5" s="70">
         <v>1</v>
       </c>
-      <c r="B5" s="95" t="s">
+      <c r="B5" s="65" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="53">
+      <c r="C5" s="52">
         <v>42565</v>
       </c>
-      <c r="D5" s="53">
+      <c r="D5" s="52">
         <v>42565</v>
       </c>
-      <c r="E5" s="53">
+      <c r="E5" s="52">
         <v>42565</v>
       </c>
-      <c r="F5" s="53">
+      <c r="F5" s="52">
         <v>42565</v>
       </c>
-      <c r="G5" s="52">
+      <c r="G5" s="51">
         <v>100</v>
       </c>
-      <c r="H5" s="59" t="s">
-        <v>49</v>
-      </c>
-      <c r="I5" s="62" t="s">
-        <v>50</v>
+      <c r="H5" s="58" t="s">
+        <v>46</v>
+      </c>
+      <c r="I5" s="61" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="99"/>
-      <c r="B6" s="96" t="s">
+      <c r="A6" s="71"/>
+      <c r="B6" s="66" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="53">
+      <c r="C6" s="52">
         <v>42565</v>
       </c>
-      <c r="D6" s="53">
+      <c r="D6" s="52">
         <v>42565</v>
       </c>
-      <c r="E6" s="53">
+      <c r="E6" s="52">
         <v>42565</v>
       </c>
-      <c r="F6" s="53">
+      <c r="F6" s="52">
         <v>42565</v>
       </c>
       <c r="G6" s="10">
         <v>100</v>
       </c>
-      <c r="H6" s="59" t="s">
-        <v>49</v>
-      </c>
-      <c r="I6" s="57"/>
+      <c r="H6" s="58" t="s">
+        <v>46</v>
+      </c>
+      <c r="I6" s="56"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="100"/>
-      <c r="B7" s="96" t="s">
+      <c r="A7" s="72"/>
+      <c r="B7" s="66" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="53">
+      <c r="C7" s="52">
         <v>42565</v>
       </c>
-      <c r="D7" s="53">
+      <c r="D7" s="52">
         <v>42565</v>
       </c>
-      <c r="E7" s="53">
+      <c r="E7" s="52">
         <v>42565</v>
       </c>
-      <c r="F7" s="53">
+      <c r="F7" s="52">
         <v>42565</v>
       </c>
       <c r="G7" s="10">
         <v>100</v>
       </c>
-      <c r="H7" s="59" t="s">
-        <v>49</v>
-      </c>
-      <c r="I7" s="57"/>
+      <c r="H7" s="58" t="s">
+        <v>46</v>
+      </c>
+      <c r="I7" s="56"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="57"/>
-      <c r="B8" s="96"/>
-      <c r="C8" s="54"/>
-      <c r="D8" s="50"/>
-      <c r="E8" s="50"/>
+      <c r="A8" s="56"/>
+      <c r="B8" s="66"/>
+      <c r="C8" s="53"/>
+      <c r="D8" s="49"/>
+      <c r="E8" s="49"/>
       <c r="F8" s="10"/>
       <c r="G8" s="10"/>
-      <c r="H8" s="60"/>
-      <c r="I8" s="57"/>
-    </row>
-    <row r="9" spans="1:9" s="49" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="57"/>
-      <c r="B9" s="96"/>
-      <c r="C9" s="54"/>
-      <c r="D9" s="50"/>
-      <c r="E9" s="50"/>
+      <c r="H8" s="59"/>
+      <c r="I8" s="56"/>
+    </row>
+    <row r="9" spans="1:9" s="48" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="56"/>
+      <c r="B9" s="66"/>
+      <c r="C9" s="53"/>
+      <c r="D9" s="49"/>
+      <c r="E9" s="49"/>
       <c r="F9" s="10"/>
       <c r="G9" s="10"/>
-      <c r="H9" s="60"/>
-      <c r="I9" s="57"/>
-    </row>
-    <row r="10" spans="1:9" s="49" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="57"/>
-      <c r="B10" s="96"/>
-      <c r="C10" s="54"/>
-      <c r="D10" s="50"/>
-      <c r="E10" s="50"/>
+      <c r="H9" s="59"/>
+      <c r="I9" s="56"/>
+    </row>
+    <row r="10" spans="1:9" s="48" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="56"/>
+      <c r="B10" s="66"/>
+      <c r="C10" s="53"/>
+      <c r="D10" s="49"/>
+      <c r="E10" s="49"/>
       <c r="F10" s="10"/>
       <c r="G10" s="10"/>
-      <c r="H10" s="60"/>
-      <c r="I10" s="57"/>
-    </row>
-    <row r="11" spans="1:9" s="49" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="57"/>
-      <c r="B11" s="96"/>
-      <c r="C11" s="54"/>
-      <c r="D11" s="50"/>
-      <c r="E11" s="50"/>
+      <c r="H10" s="59"/>
+      <c r="I10" s="56"/>
+    </row>
+    <row r="11" spans="1:9" s="48" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="56"/>
+      <c r="B11" s="66"/>
+      <c r="C11" s="53"/>
+      <c r="D11" s="49"/>
+      <c r="E11" s="49"/>
       <c r="F11" s="10"/>
       <c r="G11" s="10"/>
-      <c r="H11" s="60"/>
-      <c r="I11" s="57"/>
-    </row>
-    <row r="12" spans="1:9" s="49" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="57"/>
-      <c r="B12" s="96"/>
-      <c r="C12" s="54"/>
-      <c r="D12" s="50"/>
-      <c r="E12" s="50"/>
+      <c r="H11" s="59"/>
+      <c r="I11" s="56"/>
+    </row>
+    <row r="12" spans="1:9" s="48" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="56"/>
+      <c r="B12" s="66"/>
+      <c r="C12" s="53"/>
+      <c r="D12" s="49"/>
+      <c r="E12" s="49"/>
       <c r="F12" s="10"/>
       <c r="G12" s="10"/>
-      <c r="H12" s="60"/>
-      <c r="I12" s="57"/>
-    </row>
-    <row r="13" spans="1:9" s="49" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="57"/>
-      <c r="B13" s="96"/>
-      <c r="C13" s="54"/>
-      <c r="D13" s="50"/>
-      <c r="E13" s="50"/>
+      <c r="H12" s="59"/>
+      <c r="I12" s="56"/>
+    </row>
+    <row r="13" spans="1:9" s="48" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="56"/>
+      <c r="B13" s="66"/>
+      <c r="C13" s="53"/>
+      <c r="D13" s="49"/>
+      <c r="E13" s="49"/>
       <c r="F13" s="10"/>
       <c r="G13" s="10"/>
-      <c r="H13" s="60"/>
-      <c r="I13" s="57"/>
+      <c r="H13" s="59"/>
+      <c r="I13" s="56"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="57"/>
-      <c r="B14" s="96"/>
-      <c r="C14" s="55"/>
+      <c r="A14" s="56"/>
+      <c r="B14" s="66"/>
+      <c r="C14" s="54"/>
       <c r="D14" s="10"/>
       <c r="E14" s="10"/>
       <c r="F14" s="10"/>
       <c r="G14" s="10"/>
-      <c r="H14" s="60"/>
-      <c r="I14" s="57"/>
+      <c r="H14" s="59"/>
+      <c r="I14" s="56"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="57"/>
-      <c r="B15" s="96"/>
-      <c r="C15" s="55"/>
+      <c r="A15" s="56"/>
+      <c r="B15" s="66"/>
+      <c r="C15" s="54"/>
       <c r="D15" s="10"/>
       <c r="E15" s="10"/>
       <c r="F15" s="10"/>
       <c r="G15" s="10"/>
-      <c r="H15" s="60"/>
-      <c r="I15" s="57"/>
+      <c r="H15" s="59"/>
+      <c r="I15" s="56"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="57"/>
-      <c r="B16" s="96"/>
-      <c r="C16" s="55"/>
+      <c r="A16" s="56"/>
+      <c r="B16" s="66"/>
+      <c r="C16" s="54"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="60"/>
-      <c r="I16" s="57"/>
+      <c r="H16" s="59"/>
+      <c r="I16" s="56"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="57"/>
-      <c r="B17" s="96"/>
-      <c r="C17" s="55"/>
+      <c r="A17" s="56"/>
+      <c r="B17" s="66"/>
+      <c r="C17" s="54"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="60"/>
-      <c r="I17" s="57"/>
+      <c r="H17" s="59"/>
+      <c r="I17" s="56"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="57"/>
-      <c r="B18" s="96"/>
-      <c r="C18" s="55"/>
+      <c r="A18" s="56"/>
+      <c r="B18" s="66"/>
+      <c r="C18" s="54"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="60"/>
-      <c r="I18" s="57"/>
+      <c r="H18" s="59"/>
+      <c r="I18" s="56"/>
     </row>
     <row r="19" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="58"/>
-      <c r="B19" s="97"/>
-      <c r="C19" s="56"/>
-      <c r="D19" s="51"/>
-      <c r="E19" s="51"/>
-      <c r="F19" s="51"/>
-      <c r="G19" s="51"/>
-      <c r="H19" s="61"/>
-      <c r="I19" s="58"/>
+      <c r="A19" s="57"/>
+      <c r="B19" s="67"/>
+      <c r="C19" s="55"/>
+      <c r="D19" s="50"/>
+      <c r="E19" s="50"/>
+      <c r="F19" s="50"/>
+      <c r="G19" s="50"/>
+      <c r="H19" s="60"/>
+      <c r="I19" s="57"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B21" s="64" t="s">
-        <v>46</v>
+      <c r="B21" s="63" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B23" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C23" s="71" t="s">
+      <c r="C23" s="79" t="s">
         <v>11</v>
       </c>
-      <c r="D23" s="71"/>
-      <c r="E23" s="71"/>
+      <c r="D23" s="79"/>
+      <c r="E23" s="79"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B24" s="63" t="s">
+      <c r="B24" s="62" t="s">
         <v>20</v>
       </c>
-      <c r="C24" s="65" t="s">
+      <c r="C24" s="73" t="s">
         <v>20</v>
       </c>
-      <c r="D24" s="65"/>
-      <c r="E24" s="65"/>
-    </row>
-    <row r="26" spans="1:9" s="49" customFormat="1" x14ac:dyDescent="0.25"/>
+      <c r="D24" s="73"/>
+      <c r="E24" s="73"/>
+    </row>
+    <row r="26" spans="1:9" s="48" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B27" s="64" t="s">
-        <v>47</v>
+      <c r="B27" s="63" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
@@ -1801,17 +1828,12 @@
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B30" s="63" t="s">
+      <c r="B30" s="62" t="s">
         <v>18</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="A5:A7"/>
-    <mergeCell ref="C24:E24"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="I3:I4"/>
     <mergeCell ref="B1:I1"/>
     <mergeCell ref="C23:E23"/>
     <mergeCell ref="H3:H4"/>
@@ -1820,6 +1842,11 @@
     <mergeCell ref="E3:E4"/>
     <mergeCell ref="D3:D4"/>
     <mergeCell ref="C3:C4"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="A5:A7"/>
+    <mergeCell ref="C24:E24"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="I3:I4"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="5" orientation="landscape" r:id="rId1"/>
@@ -1828,10 +1855,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F49"/>
+  <dimension ref="A1:F47"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1854,15 +1881,15 @@
       <c r="C1" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="34" t="s">
+      <c r="D1" s="33" t="s">
         <v>28</v>
       </c>
-      <c r="E1" s="44" t="s">
+      <c r="E1" s="43" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="75" t="s">
+      <c r="A2" s="89" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="17" t="s">
@@ -1871,203 +1898,198 @@
       <c r="C2" s="18">
         <v>1</v>
       </c>
-      <c r="D2" s="35">
+      <c r="D2" s="34">
         <f>((C2/3)*100)</f>
         <v>33.333333333333329</v>
       </c>
-      <c r="E2" s="78">
+      <c r="E2" s="92">
         <f>(AVERAGE(C2:C4))*100</f>
-        <v>66.666666666666657</v>
+        <v>100</v>
       </c>
       <c r="F2" s="5"/>
     </row>
     <row r="3" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="76"/>
+      <c r="A3" s="90"/>
       <c r="B3" s="8" t="s">
         <v>5</v>
       </c>
       <c r="C3" s="9">
         <v>1</v>
       </c>
-      <c r="D3" s="36">
+      <c r="D3" s="35">
         <f t="shared" ref="D3:D4" si="0">((C3/3)*100)</f>
         <v>33.333333333333329</v>
       </c>
-      <c r="E3" s="79"/>
+      <c r="E3" s="93"/>
       <c r="F3" s="5"/>
     </row>
     <row r="4" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="77"/>
+      <c r="A4" s="91"/>
       <c r="B4" s="19" t="s">
         <v>6</v>
       </c>
       <c r="C4" s="20">
+        <v>1</v>
+      </c>
+      <c r="D4" s="36">
+        <f t="shared" si="0"/>
+        <v>33.333333333333329</v>
+      </c>
+      <c r="E4" s="94"/>
+      <c r="F4" s="5"/>
+    </row>
+    <row r="5" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="95" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="27" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5" s="28"/>
+      <c r="D5" s="37">
+        <f>(AVERAGE(C6:C10)*100)*0.5</f>
         <v>0</v>
       </c>
-      <c r="D4" s="37">
-        <f t="shared" si="0"/>
+      <c r="E5" s="98">
+        <f>D5+D11</f>
         <v>0</v>
       </c>
-      <c r="E4" s="80"/>
-      <c r="F4" s="5"/>
-    </row>
-    <row r="5" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="81" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="28" t="s">
-        <v>29</v>
-      </c>
-      <c r="C5" s="29"/>
-      <c r="D5" s="38">
-        <f>(AVERAGE(C6:C13)*100)*0.5</f>
+      <c r="F5" s="5"/>
+    </row>
+    <row r="6" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="96"/>
+      <c r="B6" s="31" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6" s="32">
         <v>0</v>
       </c>
-      <c r="E5" s="84">
-        <f>D5+D14</f>
-        <v>0</v>
-      </c>
-      <c r="F5" s="5"/>
-    </row>
-    <row r="6" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="82"/>
-      <c r="B6" s="32" t="s">
-        <v>30</v>
-      </c>
-      <c r="C6" s="33">
-        <v>0</v>
-      </c>
-      <c r="D6" s="39">
+      <c r="D6" s="38">
         <f>(C6/8)*100</f>
         <v>0</v>
       </c>
-      <c r="E6" s="85"/>
+      <c r="E6" s="99"/>
       <c r="F6" s="5"/>
     </row>
     <row r="7" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="82"/>
-      <c r="B7" s="32" t="s">
+      <c r="A7" s="96"/>
+      <c r="B7" s="31" t="s">
         <v>31</v>
       </c>
-      <c r="C7" s="33">
+      <c r="C7" s="32">
         <v>0</v>
       </c>
-      <c r="D7" s="39">
-        <f t="shared" ref="D7:D13" si="1">(C7/8)*100</f>
+      <c r="D7" s="38">
+        <f t="shared" ref="D7:D10" si="1">(C7/8)*100</f>
         <v>0</v>
       </c>
-      <c r="E7" s="85"/>
+      <c r="E7" s="99"/>
       <c r="F7" s="5"/>
     </row>
     <row r="8" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="82"/>
-      <c r="B8" s="32" t="s">
+      <c r="A8" s="96"/>
+      <c r="B8" s="31" t="s">
         <v>32</v>
       </c>
-      <c r="C8" s="33">
+      <c r="C8" s="32">
         <v>0</v>
       </c>
-      <c r="D8" s="39">
+      <c r="D8" s="38">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="E8" s="85"/>
+      <c r="E8" s="99"/>
       <c r="F8" s="5"/>
     </row>
     <row r="9" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="82"/>
-      <c r="B9" s="32" t="s">
+      <c r="A9" s="96"/>
+      <c r="B9" s="31" t="s">
         <v>33</v>
       </c>
-      <c r="C9" s="33">
+      <c r="C9" s="32">
         <v>0</v>
       </c>
-      <c r="D9" s="39">
+      <c r="D9" s="38">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="E9" s="85"/>
+      <c r="E9" s="99"/>
       <c r="F9" s="5"/>
     </row>
     <row r="10" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="82"/>
-      <c r="B10" s="32" t="s">
+      <c r="A10" s="96"/>
+      <c r="B10" s="31" t="s">
         <v>34</v>
       </c>
-      <c r="C10" s="33">
+      <c r="C10" s="32">
         <v>0</v>
       </c>
-      <c r="D10" s="39">
+      <c r="D10" s="38">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="E10" s="85"/>
+      <c r="E10" s="99"/>
       <c r="F10" s="5"/>
     </row>
-    <row r="11" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="82"/>
-      <c r="B11" s="32" t="s">
-        <v>35</v>
-      </c>
-      <c r="C11" s="33">
+    <row r="11" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="97"/>
+      <c r="B11" s="29" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11" s="30">
         <v>0</v>
       </c>
       <c r="D11" s="39">
-        <f t="shared" si="1"/>
+        <f>(C11/2)*100</f>
         <v>0</v>
       </c>
-      <c r="E11" s="85"/>
+      <c r="E11" s="100"/>
       <c r="F11" s="5"/>
     </row>
-    <row r="12" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="82"/>
-      <c r="B12" s="32" t="s">
-        <v>36</v>
-      </c>
-      <c r="C12" s="33">
+    <row r="12" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="101" t="s">
+        <v>49</v>
+      </c>
+      <c r="B12" s="102" t="s">
+        <v>50</v>
+      </c>
+      <c r="C12" s="103"/>
+      <c r="D12" s="104">
+        <f>C12*100</f>
         <v>0</v>
       </c>
-      <c r="D12" s="39">
-        <f t="shared" si="1"/>
+      <c r="E12" s="105">
+        <f>D12</f>
         <v>0</v>
       </c>
-      <c r="E12" s="85"/>
       <c r="F12" s="5"/>
     </row>
     <row r="13" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="82"/>
-      <c r="B13" s="32" t="s">
-        <v>37</v>
-      </c>
-      <c r="C13" s="33">
-        <v>0</v>
-      </c>
-      <c r="D13" s="39">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="E13" s="85"/>
+      <c r="A13" s="25" t="s">
+        <v>53</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C13" s="26"/>
+      <c r="D13" s="40"/>
+      <c r="E13" s="44"/>
       <c r="F13" s="5"/>
     </row>
-    <row r="14" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="83"/>
-      <c r="B14" s="30" t="s">
-        <v>26</v>
-      </c>
-      <c r="C14" s="31">
-        <v>0</v>
-      </c>
-      <c r="D14" s="40">
-        <f>(C14/2)*100</f>
-        <v>0</v>
-      </c>
-      <c r="E14" s="86"/>
+    <row r="14" spans="1:6" s="64" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="25"/>
+      <c r="B14" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="C14" s="26"/>
+      <c r="D14" s="40"/>
+      <c r="E14" s="44"/>
       <c r="F14" s="5"/>
     </row>
     <row r="15" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="25"/>
-      <c r="B15" s="26"/>
-      <c r="C15" s="27"/>
+      <c r="A15" s="23"/>
+      <c r="B15" s="6"/>
+      <c r="C15" s="7"/>
       <c r="D15" s="41"/>
       <c r="E15" s="45"/>
       <c r="F15" s="5"/>
@@ -2076,213 +2098,213 @@
       <c r="A16" s="23"/>
       <c r="B16" s="6"/>
       <c r="C16" s="7"/>
-      <c r="D16" s="42"/>
-      <c r="E16" s="46"/>
+      <c r="D16" s="41"/>
+      <c r="E16" s="45"/>
       <c r="F16" s="5"/>
     </row>
     <row r="17" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="23"/>
       <c r="B17" s="6"/>
       <c r="C17" s="7"/>
-      <c r="D17" s="42"/>
-      <c r="E17" s="46"/>
+      <c r="D17" s="41"/>
+      <c r="E17" s="45"/>
       <c r="F17" s="5"/>
     </row>
     <row r="18" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="23"/>
       <c r="B18" s="6"/>
       <c r="C18" s="7"/>
-      <c r="D18" s="42"/>
-      <c r="E18" s="46"/>
+      <c r="D18" s="41"/>
+      <c r="E18" s="45"/>
       <c r="F18" s="5"/>
     </row>
     <row r="19" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="23"/>
       <c r="B19" s="6"/>
       <c r="C19" s="7"/>
-      <c r="D19" s="42"/>
-      <c r="E19" s="46"/>
+      <c r="D19" s="41"/>
+      <c r="E19" s="45"/>
       <c r="F19" s="5"/>
     </row>
     <row r="20" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="23"/>
       <c r="B20" s="6"/>
       <c r="C20" s="7"/>
-      <c r="D20" s="42"/>
-      <c r="E20" s="46"/>
+      <c r="D20" s="41"/>
+      <c r="E20" s="45"/>
       <c r="F20" s="5"/>
     </row>
     <row r="21" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="23"/>
       <c r="B21" s="6"/>
       <c r="C21" s="7"/>
-      <c r="D21" s="42"/>
-      <c r="E21" s="46"/>
+      <c r="D21" s="41"/>
+      <c r="E21" s="45"/>
       <c r="F21" s="5"/>
     </row>
     <row r="22" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="23"/>
       <c r="B22" s="6"/>
       <c r="C22" s="7"/>
-      <c r="D22" s="42"/>
-      <c r="E22" s="46"/>
+      <c r="D22" s="41"/>
+      <c r="E22" s="45"/>
       <c r="F22" s="5"/>
     </row>
     <row r="23" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="23"/>
       <c r="B23" s="6"/>
       <c r="C23" s="7"/>
-      <c r="D23" s="42"/>
-      <c r="E23" s="46"/>
+      <c r="D23" s="41"/>
+      <c r="E23" s="45"/>
       <c r="F23" s="5"/>
     </row>
     <row r="24" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="23"/>
       <c r="B24" s="6"/>
       <c r="C24" s="7"/>
-      <c r="D24" s="42"/>
-      <c r="E24" s="46"/>
+      <c r="D24" s="41"/>
+      <c r="E24" s="45"/>
       <c r="F24" s="5"/>
     </row>
     <row r="25" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="23"/>
       <c r="B25" s="6"/>
       <c r="C25" s="7"/>
-      <c r="D25" s="42"/>
-      <c r="E25" s="46"/>
+      <c r="D25" s="41"/>
+      <c r="E25" s="45"/>
       <c r="F25" s="5"/>
     </row>
     <row r="26" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" s="23"/>
       <c r="B26" s="6"/>
       <c r="C26" s="7"/>
-      <c r="D26" s="42"/>
-      <c r="E26" s="46"/>
+      <c r="D26" s="41"/>
+      <c r="E26" s="45"/>
       <c r="F26" s="5"/>
     </row>
     <row r="27" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" s="23"/>
       <c r="B27" s="6"/>
       <c r="C27" s="7"/>
-      <c r="D27" s="42"/>
-      <c r="E27" s="46"/>
+      <c r="D27" s="41"/>
+      <c r="E27" s="45"/>
       <c r="F27" s="5"/>
     </row>
     <row r="28" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" s="23"/>
       <c r="B28" s="6"/>
       <c r="C28" s="7"/>
-      <c r="D28" s="42"/>
-      <c r="E28" s="46"/>
+      <c r="D28" s="41"/>
+      <c r="E28" s="45"/>
       <c r="F28" s="5"/>
     </row>
     <row r="29" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" s="23"/>
       <c r="B29" s="6"/>
       <c r="C29" s="7"/>
-      <c r="D29" s="42"/>
-      <c r="E29" s="46"/>
+      <c r="D29" s="41"/>
+      <c r="E29" s="45"/>
       <c r="F29" s="5"/>
     </row>
     <row r="30" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30" s="23"/>
       <c r="B30" s="6"/>
       <c r="C30" s="7"/>
-      <c r="D30" s="42"/>
-      <c r="E30" s="46"/>
+      <c r="D30" s="41"/>
+      <c r="E30" s="45"/>
       <c r="F30" s="5"/>
     </row>
     <row r="31" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A31" s="23"/>
       <c r="B31" s="6"/>
       <c r="C31" s="7"/>
-      <c r="D31" s="42"/>
-      <c r="E31" s="46"/>
+      <c r="D31" s="41"/>
+      <c r="E31" s="45"/>
       <c r="F31" s="5"/>
     </row>
     <row r="32" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A32" s="23"/>
       <c r="B32" s="6"/>
       <c r="C32" s="7"/>
-      <c r="D32" s="42"/>
-      <c r="E32" s="46"/>
+      <c r="D32" s="41"/>
+      <c r="E32" s="45"/>
       <c r="F32" s="5"/>
     </row>
     <row r="33" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A33" s="23"/>
       <c r="B33" s="6"/>
       <c r="C33" s="7"/>
-      <c r="D33" s="42"/>
-      <c r="E33" s="46"/>
+      <c r="D33" s="41"/>
+      <c r="E33" s="45"/>
       <c r="F33" s="5"/>
     </row>
     <row r="34" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A34" s="23"/>
       <c r="B34" s="6"/>
       <c r="C34" s="7"/>
-      <c r="D34" s="42"/>
-      <c r="E34" s="46"/>
+      <c r="D34" s="41"/>
+      <c r="E34" s="45"/>
       <c r="F34" s="5"/>
     </row>
     <row r="35" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A35" s="23"/>
       <c r="B35" s="6"/>
       <c r="C35" s="7"/>
-      <c r="D35" s="42"/>
-      <c r="E35" s="46"/>
+      <c r="D35" s="41"/>
+      <c r="E35" s="45"/>
       <c r="F35" s="5"/>
     </row>
     <row r="36" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A36" s="23"/>
       <c r="B36" s="6"/>
       <c r="C36" s="7"/>
-      <c r="D36" s="42"/>
-      <c r="E36" s="46"/>
+      <c r="D36" s="41"/>
+      <c r="E36" s="45"/>
       <c r="F36" s="5"/>
     </row>
     <row r="37" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A37" s="23"/>
       <c r="B37" s="6"/>
       <c r="C37" s="7"/>
-      <c r="D37" s="42"/>
-      <c r="E37" s="46"/>
+      <c r="D37" s="41"/>
+      <c r="E37" s="45"/>
       <c r="F37" s="5"/>
     </row>
-    <row r="38" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A38" s="23"/>
-      <c r="B38" s="6"/>
-      <c r="C38" s="7"/>
+    <row r="38" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="24"/>
+      <c r="B38" s="16"/>
+      <c r="C38" s="15"/>
       <c r="D38" s="42"/>
       <c r="E38" s="46"/>
       <c r="F38" s="5"/>
     </row>
-    <row r="39" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A39" s="23"/>
-      <c r="B39" s="6"/>
-      <c r="C39" s="7"/>
-      <c r="D39" s="42"/>
-      <c r="E39" s="46"/>
+    <row r="39" spans="1:6" ht="24" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="86" t="s">
+        <v>27</v>
+      </c>
+      <c r="B39" s="87"/>
+      <c r="C39" s="87"/>
+      <c r="D39" s="88"/>
+      <c r="E39" s="47">
+        <f>(AVERAGE(E2,E5))</f>
+        <v>50</v>
+      </c>
       <c r="F39" s="5"/>
     </row>
-    <row r="40" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="24"/>
-      <c r="B40" s="16"/>
-      <c r="C40" s="15"/>
-      <c r="D40" s="43"/>
-      <c r="E40" s="47"/>
+    <row r="40" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A40" s="5"/>
+      <c r="B40" s="4"/>
+      <c r="C40" s="5"/>
+      <c r="D40" s="5"/>
+      <c r="E40" s="5"/>
       <c r="F40" s="5"/>
     </row>
-    <row r="41" spans="1:6" ht="24" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="72" t="s">
-        <v>27</v>
-      </c>
-      <c r="B41" s="73"/>
-      <c r="C41" s="73"/>
-      <c r="D41" s="74"/>
-      <c r="E41" s="48">
-        <f>(AVERAGE(E2,E5))</f>
-        <v>33.333333333333329</v>
-      </c>
+    <row r="41" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A41" s="5"/>
+      <c r="B41" s="4"/>
+      <c r="C41" s="5"/>
+      <c r="D41" s="5"/>
+      <c r="E41" s="5"/>
       <c r="F41" s="5"/>
     </row>
     <row r="42" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -2333,29 +2355,13 @@
       <c r="E47" s="5"/>
       <c r="F47" s="5"/>
     </row>
-    <row r="48" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A48" s="5"/>
-      <c r="B48" s="4"/>
-      <c r="C48" s="5"/>
-      <c r="D48" s="5"/>
-      <c r="E48" s="5"/>
-      <c r="F48" s="5"/>
-    </row>
-    <row r="49" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A49" s="5"/>
-      <c r="B49" s="4"/>
-      <c r="C49" s="5"/>
-      <c r="D49" s="5"/>
-      <c r="E49" s="5"/>
-      <c r="F49" s="5"/>
-    </row>
   </sheetData>
   <mergeCells count="5">
-    <mergeCell ref="A41:D41"/>
+    <mergeCell ref="A39:D39"/>
     <mergeCell ref="A2:A4"/>
     <mergeCell ref="E2:E4"/>
-    <mergeCell ref="A5:A14"/>
-    <mergeCell ref="E5:E14"/>
+    <mergeCell ref="A5:A11"/>
+    <mergeCell ref="E5:E11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Initial commit - Workplan - Second Day
</commit_message>
<xml_diff>
--- a/Workplan.xlsx
+++ b/Workplan.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="75" windowWidth="18195" windowHeight="11820" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="75" windowWidth="18195" windowHeight="11820"/>
   </bookViews>
   <sheets>
     <sheet name="Work Plan" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="68">
   <si>
     <t>ACTIVITIES</t>
   </si>
@@ -114,6 +114,15 @@
     <t>Sonarqube</t>
   </si>
   <si>
+    <t>ELK</t>
+  </si>
+  <si>
+    <t>Sensu</t>
+  </si>
+  <si>
+    <t>Nexus</t>
+  </si>
+  <si>
     <t>Ansible</t>
   </si>
   <si>
@@ -153,10 +162,55 @@
     <t>Reviewed by:</t>
   </si>
   <si>
-    <t>Percentage</t>
-  </si>
-  <si>
     <t>Completed</t>
+  </si>
+  <si>
+    <t>DAY</t>
+  </si>
+  <si>
+    <t>Code Development</t>
+  </si>
+  <si>
+    <t>Javascript Calculator</t>
+  </si>
+  <si>
+    <t>CI-CD</t>
+  </si>
+  <si>
+    <t>Developer Check-in code to Repository</t>
+  </si>
+  <si>
+    <t>Configure GitLab and Jenkins</t>
+  </si>
+  <si>
+    <t>Configure Jenkins and Maven</t>
+  </si>
+  <si>
+    <t>Configure Jenkins and Sonarqube</t>
+  </si>
+  <si>
+    <t>Deploy App from Ansible to Tomcat</t>
+  </si>
+  <si>
+    <t>Test app using Selenium</t>
+  </si>
+  <si>
+    <t>Debugging</t>
+  </si>
+  <si>
+    <t>Percent Complete</t>
+  </si>
+  <si>
+    <t>Developer</t>
+  </si>
+  <si>
+    <t>Debug Project Pipeline</t>
+  </si>
+  <si>
+    <t>Finalize Documents</t>
+  </si>
+  <si>
+    <t>DEVOPS BOOTCAMP</t>
   </si>
   <si>
     <r>
@@ -178,7 +232,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">Angelo Q. De Rivera     </t>
+      <t xml:space="preserve">Angelo Q. De Rivera                                          </t>
     </r>
     <r>
       <rPr>
@@ -210,7 +264,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">   Dev/CI-CD:</t>
+      <t xml:space="preserve">                                                  Dev/CI-CD:</t>
     </r>
     <r>
       <rPr>
@@ -220,7 +274,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> Rhodenel  S. Omaña   </t>
+      <t xml:space="preserve"> Rhodenel  S. Omaña                                       </t>
     </r>
     <r>
       <rPr>
@@ -245,29 +299,17 @@
     </r>
   </si>
   <si>
-    <t>DAY</t>
-  </si>
-  <si>
-    <t>Code Development</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Coding the Javascript Calculator App </t>
-  </si>
-  <si>
-    <t>Commit project in the Gitlab Repo</t>
-  </si>
-  <si>
-    <t>Create Cartridges for Stack Spin up</t>
-  </si>
-  <si>
-    <t>CD - CI</t>
+    <t>Environment Setup (Cloud Formation)</t>
+  </si>
+  <si>
+    <t>In Progress</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -307,14 +349,52 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="9"/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -359,12 +439,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.79998168889431442"/>
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="41">
+  <borders count="35">
     <border>
       <left/>
       <right/>
@@ -427,19 +513,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
@@ -771,11 +844,13 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="thin">
+      <right style="medium">
         <color indexed="64"/>
       </right>
-      <top/>
-      <bottom style="medium">
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -784,44 +859,52 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
+      <right style="medium">
         <color indexed="64"/>
       </right>
       <top style="thin">
         <color indexed="64"/>
       </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
       <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -831,83 +914,21 @@
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="medium">
+      <top style="thin">
         <color indexed="64"/>
       </top>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="106">
+  <cellXfs count="136">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -952,46 +973,49 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1000,211 +1024,271 @@
     <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="2" fontId="3" fillId="3" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="2" fontId="3" fillId="3" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="3" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="3" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="5" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="3" fillId="5" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="3" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="3" fillId="5" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="3" fillId="5" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="6" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="3" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="8" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="6"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="8" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="8" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="8" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="3" fillId="3" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="3" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="3" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="3" fillId="3" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="3" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="3" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="5" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="3" fillId="5" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="8" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="8" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1508,10 +1592,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I30"/>
+  <dimension ref="A1:I45"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1519,7 +1603,7 @@
     <col min="1" max="1" width="7.42578125" style="48" customWidth="1"/>
     <col min="2" max="2" width="44" customWidth="1"/>
     <col min="3" max="3" width="10.28515625" customWidth="1"/>
-    <col min="4" max="4" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.7109375" customWidth="1"/>
     <col min="5" max="5" width="11.140625" customWidth="1"/>
     <col min="6" max="6" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.42578125" customWidth="1"/>
@@ -1527,358 +1611,744 @@
     <col min="9" max="9" width="45.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="48" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B1" s="78" t="s">
+    <row r="1" spans="1:9" s="48" customFormat="1" ht="21" x14ac:dyDescent="0.35">
+      <c r="A1" s="114" t="s">
+        <v>64</v>
+      </c>
+      <c r="B1" s="114"/>
+      <c r="C1" s="114"/>
+      <c r="D1" s="114"/>
+      <c r="E1" s="114"/>
+      <c r="F1" s="114"/>
+      <c r="G1" s="114"/>
+      <c r="H1" s="114"/>
+      <c r="I1" s="114"/>
+    </row>
+    <row r="2" spans="1:9" s="48" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A2" s="120" t="s">
+        <v>45</v>
+      </c>
+      <c r="B2" s="120"/>
+      <c r="C2" s="120"/>
+      <c r="D2" s="120"/>
+      <c r="E2" s="120"/>
+      <c r="F2" s="120"/>
+      <c r="G2" s="120"/>
+      <c r="H2" s="120"/>
+      <c r="I2" s="120"/>
+    </row>
+    <row r="3" spans="1:9" s="48" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="49"/>
+      <c r="C3" s="49"/>
+      <c r="D3" s="49"/>
+      <c r="E3" s="49"/>
+      <c r="F3" s="49"/>
+      <c r="G3" s="49"/>
+      <c r="H3" s="49"/>
+      <c r="I3" s="49"/>
+    </row>
+    <row r="4" spans="1:9" s="48" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="104" t="s">
+        <v>49</v>
+      </c>
+      <c r="B5" s="104" t="s">
+        <v>38</v>
+      </c>
+      <c r="C5" s="118" t="s">
+        <v>40</v>
+      </c>
+      <c r="D5" s="116" t="s">
+        <v>41</v>
+      </c>
+      <c r="E5" s="118" t="s">
         <v>42</v>
       </c>
-      <c r="C1" s="78"/>
-      <c r="D1" s="78"/>
-      <c r="E1" s="78"/>
-      <c r="F1" s="78"/>
-      <c r="G1" s="78"/>
-      <c r="H1" s="78"/>
-      <c r="I1" s="78"/>
-    </row>
-    <row r="2" spans="1:9" s="48" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="68" t="s">
+      <c r="F5" s="116" t="s">
+        <v>43</v>
+      </c>
+      <c r="G5" s="106" t="s">
+        <v>60</v>
+      </c>
+      <c r="H5" s="106" t="s">
+        <v>44</v>
+      </c>
+      <c r="I5" s="106" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="105"/>
+      <c r="B6" s="105"/>
+      <c r="C6" s="119"/>
+      <c r="D6" s="117"/>
+      <c r="E6" s="119"/>
+      <c r="F6" s="117"/>
+      <c r="G6" s="107"/>
+      <c r="H6" s="107"/>
+      <c r="I6" s="107"/>
+    </row>
+    <row r="7" spans="1:9" s="48" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="108">
+        <v>1</v>
+      </c>
+      <c r="B7" s="61" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="83"/>
+      <c r="D7" s="58"/>
+      <c r="E7" s="83"/>
+      <c r="F7" s="58"/>
+      <c r="G7" s="70"/>
+      <c r="H7" s="70"/>
+      <c r="I7" s="70"/>
+    </row>
+    <row r="8" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+      <c r="A8" s="109"/>
+      <c r="B8" s="62" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="84">
+        <v>42565</v>
+      </c>
+      <c r="D8" s="85">
+        <v>42565</v>
+      </c>
+      <c r="E8" s="84">
+        <v>42565</v>
+      </c>
+      <c r="F8" s="85">
+        <v>42565</v>
+      </c>
+      <c r="G8" s="74">
+        <v>100</v>
+      </c>
+      <c r="H8" s="78" t="s">
         <v>48</v>
       </c>
-      <c r="B3" s="74" t="s">
+      <c r="I8" s="71" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="109"/>
+      <c r="B9" s="63" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="84">
+        <v>42565</v>
+      </c>
+      <c r="D9" s="85">
+        <v>42565</v>
+      </c>
+      <c r="E9" s="84">
+        <v>42565</v>
+      </c>
+      <c r="F9" s="85">
+        <v>42565</v>
+      </c>
+      <c r="G9" s="74">
+        <v>100</v>
+      </c>
+      <c r="H9" s="78" t="s">
+        <v>48</v>
+      </c>
+      <c r="I9" s="68"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="109"/>
+      <c r="B10" s="63" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" s="84">
+        <v>42565</v>
+      </c>
+      <c r="D10" s="85">
+        <v>42565</v>
+      </c>
+      <c r="E10" s="84">
+        <v>42565</v>
+      </c>
+      <c r="F10" s="85">
+        <v>42565</v>
+      </c>
+      <c r="G10" s="74">
+        <v>100</v>
+      </c>
+      <c r="H10" s="78" t="s">
+        <v>48</v>
+      </c>
+      <c r="I10" s="68"/>
+    </row>
+    <row r="11" spans="1:9" s="50" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="109"/>
+      <c r="B11" s="64" t="s">
+        <v>66</v>
+      </c>
+      <c r="C11" s="86"/>
+      <c r="D11" s="87"/>
+      <c r="E11" s="102">
+        <v>42565</v>
+      </c>
+      <c r="F11" s="87"/>
+      <c r="G11" s="75"/>
+      <c r="H11" s="79"/>
+      <c r="I11" s="72"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="109"/>
+      <c r="B12" s="63" t="s">
+        <v>29</v>
+      </c>
+      <c r="C12" s="111"/>
+      <c r="D12" s="112"/>
+      <c r="E12" s="112"/>
+      <c r="F12" s="112"/>
+      <c r="G12" s="112"/>
+      <c r="H12" s="112"/>
+      <c r="I12" s="113"/>
+    </row>
+    <row r="13" spans="1:9" s="48" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="109"/>
+      <c r="B13" s="82" t="s">
+        <v>30</v>
+      </c>
+      <c r="C13" s="84">
+        <v>42565</v>
+      </c>
+      <c r="D13" s="85">
+        <v>42565</v>
+      </c>
+      <c r="E13" s="84">
+        <v>42565</v>
+      </c>
+      <c r="F13" s="84">
+        <v>42565</v>
+      </c>
+      <c r="G13" s="74">
+        <v>100</v>
+      </c>
+      <c r="H13" s="78" t="s">
+        <v>48</v>
+      </c>
+      <c r="I13" s="68"/>
+    </row>
+    <row r="14" spans="1:9" s="48" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="109"/>
+      <c r="B14" s="82" t="s">
+        <v>31</v>
+      </c>
+      <c r="C14" s="84">
+        <v>42565</v>
+      </c>
+      <c r="D14" s="85">
+        <v>42565</v>
+      </c>
+      <c r="E14" s="84">
+        <v>42565</v>
+      </c>
+      <c r="F14" s="84">
+        <v>42565</v>
+      </c>
+      <c r="G14" s="74">
+        <v>100</v>
+      </c>
+      <c r="H14" s="78" t="s">
+        <v>48</v>
+      </c>
+      <c r="I14" s="68"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="109"/>
+      <c r="B15" s="82" t="s">
         <v>35</v>
       </c>
-      <c r="C3" s="84" t="s">
+      <c r="C15" s="84">
+        <v>42565</v>
+      </c>
+      <c r="D15" s="85">
+        <v>42565</v>
+      </c>
+      <c r="E15" s="84">
+        <v>42565</v>
+      </c>
+      <c r="F15" s="84">
+        <v>42565</v>
+      </c>
+      <c r="G15" s="74">
+        <v>100</v>
+      </c>
+      <c r="H15" s="78" t="s">
+        <v>48</v>
+      </c>
+      <c r="I15" s="68"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="109"/>
+      <c r="B16" s="82" t="s">
+        <v>36</v>
+      </c>
+      <c r="C16" s="84">
+        <v>42565</v>
+      </c>
+      <c r="D16" s="85">
+        <v>42565</v>
+      </c>
+      <c r="E16" s="84">
+        <v>42565</v>
+      </c>
+      <c r="F16" s="84">
+        <v>42565</v>
+      </c>
+      <c r="G16" s="74">
+        <v>100</v>
+      </c>
+      <c r="H16" s="78" t="s">
+        <v>48</v>
+      </c>
+      <c r="I16" s="68"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="109"/>
+      <c r="B17" s="82" t="s">
         <v>37</v>
       </c>
-      <c r="D3" s="82" t="s">
-        <v>38</v>
-      </c>
-      <c r="E3" s="82" t="s">
-        <v>39</v>
-      </c>
-      <c r="F3" s="82" t="s">
-        <v>40</v>
-      </c>
-      <c r="G3" s="82" t="s">
-        <v>45</v>
-      </c>
-      <c r="H3" s="80" t="s">
-        <v>41</v>
-      </c>
-      <c r="I3" s="76" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="69"/>
-      <c r="B4" s="75"/>
-      <c r="C4" s="85"/>
-      <c r="D4" s="83"/>
-      <c r="E4" s="83"/>
-      <c r="F4" s="83"/>
-      <c r="G4" s="83"/>
-      <c r="H4" s="81"/>
-      <c r="I4" s="77"/>
-    </row>
-    <row r="5" spans="1:9" ht="83.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="70">
-        <v>1</v>
-      </c>
-      <c r="B5" s="65" t="s">
+      <c r="C17" s="84">
+        <v>42565</v>
+      </c>
+      <c r="D17" s="85">
+        <v>42565</v>
+      </c>
+      <c r="E17" s="84">
+        <v>42565</v>
+      </c>
+      <c r="F17" s="84">
+        <v>42565</v>
+      </c>
+      <c r="G17" s="74">
+        <v>100</v>
+      </c>
+      <c r="H17" s="78" t="s">
+        <v>48</v>
+      </c>
+      <c r="I17" s="68"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="109"/>
+      <c r="B18" s="63" t="s">
+        <v>26</v>
+      </c>
+      <c r="C18" s="84">
+        <v>42565</v>
+      </c>
+      <c r="D18" s="85">
+        <v>42565</v>
+      </c>
+      <c r="E18" s="84">
+        <v>42565</v>
+      </c>
+      <c r="F18" s="84">
+        <v>42565</v>
+      </c>
+      <c r="G18" s="74">
+        <v>100</v>
+      </c>
+      <c r="H18" s="78" t="s">
+        <v>48</v>
+      </c>
+      <c r="I18" s="68"/>
+    </row>
+    <row r="19" spans="1:9" s="50" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A19" s="109"/>
+      <c r="B19" s="65" t="s">
+        <v>50</v>
+      </c>
+      <c r="C19" s="86"/>
+      <c r="D19" s="87"/>
+      <c r="E19" s="96"/>
+      <c r="F19" s="97"/>
+      <c r="G19" s="75"/>
+      <c r="H19" s="75"/>
+      <c r="I19" s="72"/>
+    </row>
+    <row r="20" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="110"/>
+      <c r="B20" s="80" t="s">
+        <v>51</v>
+      </c>
+      <c r="C20" s="88">
+        <v>42565</v>
+      </c>
+      <c r="D20" s="89">
+        <v>42573</v>
+      </c>
+      <c r="E20" s="89">
+        <v>42565</v>
+      </c>
+      <c r="F20" s="89"/>
+      <c r="G20" s="76">
+        <v>50</v>
+      </c>
+      <c r="H20" s="76" t="s">
+        <v>67</v>
+      </c>
+      <c r="I20" s="66"/>
+    </row>
+    <row r="21" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A21" s="108">
+        <v>2</v>
+      </c>
+      <c r="B21" s="67" t="s">
+        <v>52</v>
+      </c>
+      <c r="C21" s="90"/>
+      <c r="D21" s="91"/>
+      <c r="E21" s="90"/>
+      <c r="F21" s="91"/>
+      <c r="G21" s="77"/>
+      <c r="H21" s="77"/>
+      <c r="I21" s="73"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" s="109"/>
+      <c r="B22" s="63" t="s">
+        <v>53</v>
+      </c>
+      <c r="C22" s="92"/>
+      <c r="D22" s="56"/>
+      <c r="E22" s="92"/>
+      <c r="F22" s="56"/>
+      <c r="G22" s="68"/>
+      <c r="H22" s="68"/>
+      <c r="I22" s="68"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" s="109"/>
+      <c r="B23" s="63" t="s">
+        <v>54</v>
+      </c>
+      <c r="C23" s="92"/>
+      <c r="D23" s="56"/>
+      <c r="E23" s="92"/>
+      <c r="F23" s="56"/>
+      <c r="G23" s="68"/>
+      <c r="H23" s="68"/>
+      <c r="I23" s="68"/>
+    </row>
+    <row r="24" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="110"/>
+      <c r="B24" s="80" t="s">
+        <v>55</v>
+      </c>
+      <c r="C24" s="93"/>
+      <c r="D24" s="57"/>
+      <c r="E24" s="93"/>
+      <c r="F24" s="57"/>
+      <c r="G24" s="66"/>
+      <c r="H24" s="66"/>
+      <c r="I24" s="66"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" s="108">
         <v>3</v>
       </c>
-      <c r="C5" s="52">
-        <v>42565</v>
-      </c>
-      <c r="D5" s="52">
-        <v>42565</v>
-      </c>
-      <c r="E5" s="52">
-        <v>42565</v>
-      </c>
-      <c r="F5" s="52">
-        <v>42565</v>
-      </c>
-      <c r="G5" s="51">
-        <v>100</v>
-      </c>
-      <c r="H5" s="58" t="s">
+      <c r="B25" s="81" t="s">
+        <v>56</v>
+      </c>
+      <c r="C25" s="94"/>
+      <c r="D25" s="60"/>
+      <c r="E25" s="94"/>
+      <c r="F25" s="60"/>
+      <c r="G25" s="69"/>
+      <c r="H25" s="69"/>
+      <c r="I25" s="69"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" s="109"/>
+      <c r="B26" s="63" t="s">
+        <v>57</v>
+      </c>
+      <c r="C26" s="92"/>
+      <c r="D26" s="56"/>
+      <c r="E26" s="92"/>
+      <c r="F26" s="56"/>
+      <c r="G26" s="68"/>
+      <c r="H26" s="68"/>
+      <c r="I26" s="68"/>
+    </row>
+    <row r="27" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="110"/>
+      <c r="B27" s="80" t="s">
+        <v>58</v>
+      </c>
+      <c r="C27" s="93"/>
+      <c r="D27" s="57"/>
+      <c r="E27" s="93"/>
+      <c r="F27" s="57"/>
+      <c r="G27" s="66"/>
+      <c r="H27" s="66"/>
+      <c r="I27" s="66"/>
+    </row>
+    <row r="28" spans="1:9" s="48" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A28" s="108">
+        <v>4</v>
+      </c>
+      <c r="B28" s="67" t="s">
+        <v>59</v>
+      </c>
+      <c r="C28" s="95"/>
+      <c r="D28" s="59"/>
+      <c r="E28" s="95"/>
+      <c r="F28" s="59"/>
+      <c r="G28" s="73"/>
+      <c r="H28" s="73"/>
+      <c r="I28" s="73"/>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" s="109"/>
+      <c r="B29" s="63" t="s">
+        <v>62</v>
+      </c>
+      <c r="C29" s="92"/>
+      <c r="D29" s="56"/>
+      <c r="E29" s="92"/>
+      <c r="F29" s="56"/>
+      <c r="G29" s="68"/>
+      <c r="H29" s="68"/>
+      <c r="I29" s="68"/>
+    </row>
+    <row r="30" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="110"/>
+      <c r="B30" s="80" t="s">
+        <v>63</v>
+      </c>
+      <c r="C30" s="93"/>
+      <c r="D30" s="57"/>
+      <c r="E30" s="93"/>
+      <c r="F30" s="57"/>
+      <c r="G30" s="66"/>
+      <c r="H30" s="66"/>
+      <c r="I30" s="66"/>
+    </row>
+    <row r="31" spans="1:9" s="48" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="51"/>
+      <c r="B31" s="52"/>
+      <c r="C31" s="52"/>
+      <c r="D31" s="52"/>
+      <c r="E31" s="52"/>
+      <c r="F31" s="52"/>
+      <c r="G31" s="52"/>
+      <c r="H31" s="52"/>
+      <c r="I31" s="52"/>
+    </row>
+    <row r="33" spans="2:9" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B33" s="98" t="s">
         <v>46</v>
       </c>
-      <c r="I5" s="61" t="s">
+      <c r="C33" s="54"/>
+      <c r="D33" s="54"/>
+      <c r="E33" s="54"/>
+      <c r="F33" s="54"/>
+      <c r="G33" s="98" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="71"/>
-      <c r="B6" s="66" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" s="52">
-        <v>42565</v>
-      </c>
-      <c r="D6" s="52">
-        <v>42565</v>
-      </c>
-      <c r="E6" s="52">
-        <v>42565</v>
-      </c>
-      <c r="F6" s="52">
-        <v>42565</v>
-      </c>
-      <c r="G6" s="10">
-        <v>100</v>
-      </c>
-      <c r="H6" s="58" t="s">
-        <v>46</v>
-      </c>
-      <c r="I6" s="56"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="72"/>
-      <c r="B7" s="66" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" s="52">
-        <v>42565</v>
-      </c>
-      <c r="D7" s="52">
-        <v>42565</v>
-      </c>
-      <c r="E7" s="52">
-        <v>42565</v>
-      </c>
-      <c r="F7" s="52">
-        <v>42565</v>
-      </c>
-      <c r="G7" s="10">
-        <v>100</v>
-      </c>
-      <c r="H7" s="58" t="s">
-        <v>46</v>
-      </c>
-      <c r="I7" s="56"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="56"/>
-      <c r="B8" s="66"/>
-      <c r="C8" s="53"/>
-      <c r="D8" s="49"/>
-      <c r="E8" s="49"/>
-      <c r="F8" s="10"/>
-      <c r="G8" s="10"/>
-      <c r="H8" s="59"/>
-      <c r="I8" s="56"/>
-    </row>
-    <row r="9" spans="1:9" s="48" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="56"/>
-      <c r="B9" s="66"/>
-      <c r="C9" s="53"/>
-      <c r="D9" s="49"/>
-      <c r="E9" s="49"/>
-      <c r="F9" s="10"/>
-      <c r="G9" s="10"/>
-      <c r="H9" s="59"/>
-      <c r="I9" s="56"/>
-    </row>
-    <row r="10" spans="1:9" s="48" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="56"/>
-      <c r="B10" s="66"/>
-      <c r="C10" s="53"/>
-      <c r="D10" s="49"/>
-      <c r="E10" s="49"/>
-      <c r="F10" s="10"/>
-      <c r="G10" s="10"/>
-      <c r="H10" s="59"/>
-      <c r="I10" s="56"/>
-    </row>
-    <row r="11" spans="1:9" s="48" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="56"/>
-      <c r="B11" s="66"/>
-      <c r="C11" s="53"/>
-      <c r="D11" s="49"/>
-      <c r="E11" s="49"/>
-      <c r="F11" s="10"/>
-      <c r="G11" s="10"/>
-      <c r="H11" s="59"/>
-      <c r="I11" s="56"/>
-    </row>
-    <row r="12" spans="1:9" s="48" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="56"/>
-      <c r="B12" s="66"/>
-      <c r="C12" s="53"/>
-      <c r="D12" s="49"/>
-      <c r="E12" s="49"/>
-      <c r="F12" s="10"/>
-      <c r="G12" s="10"/>
-      <c r="H12" s="59"/>
-      <c r="I12" s="56"/>
-    </row>
-    <row r="13" spans="1:9" s="48" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="56"/>
-      <c r="B13" s="66"/>
-      <c r="C13" s="53"/>
-      <c r="D13" s="49"/>
-      <c r="E13" s="49"/>
-      <c r="F13" s="10"/>
-      <c r="G13" s="10"/>
-      <c r="H13" s="59"/>
-      <c r="I13" s="56"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="56"/>
-      <c r="B14" s="66"/>
-      <c r="C14" s="54"/>
-      <c r="D14" s="10"/>
-      <c r="E14" s="10"/>
-      <c r="F14" s="10"/>
-      <c r="G14" s="10"/>
-      <c r="H14" s="59"/>
-      <c r="I14" s="56"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="56"/>
-      <c r="B15" s="66"/>
-      <c r="C15" s="54"/>
-      <c r="D15" s="10"/>
-      <c r="E15" s="10"/>
-      <c r="F15" s="10"/>
-      <c r="G15" s="10"/>
-      <c r="H15" s="59"/>
-      <c r="I15" s="56"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="56"/>
-      <c r="B16" s="66"/>
-      <c r="C16" s="54"/>
-      <c r="D16" s="10"/>
-      <c r="E16" s="10"/>
-      <c r="F16" s="10"/>
-      <c r="G16" s="10"/>
-      <c r="H16" s="59"/>
-      <c r="I16" s="56"/>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="56"/>
-      <c r="B17" s="66"/>
-      <c r="C17" s="54"/>
-      <c r="D17" s="10"/>
-      <c r="E17" s="10"/>
-      <c r="F17" s="10"/>
-      <c r="G17" s="10"/>
-      <c r="H17" s="59"/>
-      <c r="I17" s="56"/>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="56"/>
-      <c r="B18" s="66"/>
-      <c r="C18" s="54"/>
-      <c r="D18" s="10"/>
-      <c r="E18" s="10"/>
-      <c r="F18" s="10"/>
-      <c r="G18" s="10"/>
-      <c r="H18" s="59"/>
-      <c r="I18" s="56"/>
-    </row>
-    <row r="19" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="57"/>
-      <c r="B19" s="67"/>
-      <c r="C19" s="55"/>
-      <c r="D19" s="50"/>
-      <c r="E19" s="50"/>
-      <c r="F19" s="50"/>
-      <c r="G19" s="50"/>
-      <c r="H19" s="60"/>
-      <c r="I19" s="57"/>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B21" s="63" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B23" s="2" t="s">
+      <c r="H33" s="54"/>
+      <c r="I33" s="54"/>
+    </row>
+    <row r="34" spans="2:9" s="48" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B34" s="53"/>
+      <c r="C34" s="54"/>
+      <c r="D34" s="54"/>
+      <c r="E34" s="54"/>
+      <c r="F34" s="54"/>
+      <c r="G34" s="53"/>
+      <c r="H34" s="54"/>
+      <c r="I34" s="54"/>
+    </row>
+    <row r="35" spans="2:9" s="48" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B35" s="53"/>
+      <c r="C35" s="54"/>
+      <c r="D35" s="54"/>
+      <c r="E35" s="54"/>
+      <c r="F35" s="54"/>
+      <c r="G35" s="54"/>
+      <c r="H35" s="54"/>
+      <c r="I35" s="54"/>
+    </row>
+    <row r="36" spans="2:9" s="48" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B36" s="100" t="s">
+        <v>12</v>
+      </c>
+      <c r="C36" s="115" t="s">
+        <v>8</v>
+      </c>
+      <c r="D36" s="115"/>
+      <c r="E36" s="115"/>
+      <c r="F36" s="54"/>
+      <c r="G36" s="53"/>
+      <c r="H36" s="101" t="s">
+        <v>10</v>
+      </c>
+      <c r="I36" s="54"/>
+    </row>
+    <row r="37" spans="2:9" s="48" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B37" s="99" t="s">
+        <v>52</v>
+      </c>
+      <c r="C37" s="103" t="s">
+        <v>61</v>
+      </c>
+      <c r="D37" s="103"/>
+      <c r="E37" s="103"/>
+      <c r="F37" s="54"/>
+      <c r="G37" s="54"/>
+      <c r="H37" s="99" t="s">
+        <v>18</v>
+      </c>
+      <c r="I37" s="54"/>
+    </row>
+    <row r="38" spans="2:9" s="48" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B38" s="55"/>
+      <c r="C38" s="55"/>
+      <c r="D38" s="55"/>
+      <c r="E38" s="55"/>
+      <c r="F38" s="54"/>
+      <c r="G38" s="54"/>
+      <c r="H38" s="55"/>
+      <c r="I38" s="54"/>
+    </row>
+    <row r="39" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B39" s="54"/>
+      <c r="C39" s="54"/>
+      <c r="D39" s="54"/>
+      <c r="E39" s="54"/>
+      <c r="F39" s="54"/>
+      <c r="G39" s="54"/>
+      <c r="H39" s="54"/>
+      <c r="I39" s="54"/>
+    </row>
+    <row r="40" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B40" s="100" t="s">
         <v>9</v>
       </c>
-      <c r="C23" s="79" t="s">
+      <c r="C40" s="115" t="s">
         <v>11</v>
       </c>
-      <c r="D23" s="79"/>
-      <c r="E23" s="79"/>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B24" s="62" t="s">
+      <c r="D40" s="115"/>
+      <c r="E40" s="115"/>
+      <c r="F40" s="54"/>
+      <c r="G40" s="54"/>
+      <c r="H40" s="54"/>
+      <c r="I40" s="54"/>
+    </row>
+    <row r="41" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B41" s="99" t="s">
         <v>20</v>
       </c>
-      <c r="C24" s="73" t="s">
+      <c r="C41" s="103" t="s">
         <v>20</v>
       </c>
-      <c r="D24" s="73"/>
-      <c r="E24" s="73"/>
-    </row>
-    <row r="26" spans="1:9" s="48" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B27" s="63" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B29" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B30" s="62" t="s">
-        <v>18</v>
-      </c>
+      <c r="D41" s="103"/>
+      <c r="E41" s="103"/>
+      <c r="F41" s="54"/>
+      <c r="G41" s="54"/>
+      <c r="H41" s="54"/>
+      <c r="I41" s="54"/>
+    </row>
+    <row r="42" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B42" s="54"/>
+      <c r="C42" s="54"/>
+      <c r="D42" s="54"/>
+      <c r="E42" s="54"/>
+      <c r="F42" s="54"/>
+      <c r="G42" s="54"/>
+      <c r="H42" s="54"/>
+      <c r="I42" s="54"/>
+    </row>
+    <row r="43" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B43" s="54"/>
+      <c r="C43" s="54"/>
+      <c r="D43" s="54"/>
+      <c r="E43" s="54"/>
+      <c r="F43" s="54"/>
+      <c r="G43" s="54"/>
+      <c r="H43" s="54"/>
+      <c r="I43" s="54"/>
+    </row>
+    <row r="44" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B44" s="54"/>
+      <c r="C44" s="54"/>
+      <c r="D44" s="54"/>
+      <c r="E44" s="54"/>
+      <c r="F44" s="54"/>
+      <c r="G44" s="54"/>
+      <c r="H44" s="54"/>
+      <c r="I44" s="54"/>
+    </row>
+    <row r="45" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B45" s="54"/>
+      <c r="C45" s="54"/>
+      <c r="D45" s="54"/>
+      <c r="E45" s="54"/>
+      <c r="F45" s="54"/>
+      <c r="G45" s="54"/>
+      <c r="H45" s="54"/>
+      <c r="I45" s="54"/>
     </row>
   </sheetData>
-  <mergeCells count="13">
-    <mergeCell ref="B1:I1"/>
-    <mergeCell ref="C23:E23"/>
-    <mergeCell ref="H3:H4"/>
-    <mergeCell ref="G3:G4"/>
-    <mergeCell ref="F3:F4"/>
-    <mergeCell ref="E3:E4"/>
-    <mergeCell ref="D3:D4"/>
-    <mergeCell ref="C3:C4"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="A5:A7"/>
-    <mergeCell ref="C24:E24"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="I3:I4"/>
+  <mergeCells count="20">
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="C40:E40"/>
+    <mergeCell ref="H5:H6"/>
+    <mergeCell ref="G5:G6"/>
+    <mergeCell ref="F5:F6"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="C36:E36"/>
+    <mergeCell ref="C37:E37"/>
+    <mergeCell ref="A2:I2"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="C41:E41"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="I5:I6"/>
+    <mergeCell ref="A7:A20"/>
+    <mergeCell ref="A21:A24"/>
+    <mergeCell ref="A25:A27"/>
+    <mergeCell ref="A28:A30"/>
+    <mergeCell ref="C12:I12"/>
   </mergeCells>
-  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.25" right="0.25" top="1" bottom="1" header="0.3" footer="0.3"/>
   <pageSetup paperSize="5" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F47"/>
+  <dimension ref="A1:F49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.7109375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="66.140625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="16.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.85546875" style="2" customWidth="1"/>
-    <col min="5" max="5" width="27.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="1" width="22.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="66.140625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="16.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.85546875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="22" t="s">
+      <c r="B1" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="22" t="s">
+      <c r="C1" s="21" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="33" t="s">
@@ -1889,57 +2359,57 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="89" t="s">
+      <c r="A2" s="124" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="18">
+      <c r="C2" s="17">
         <v>1</v>
       </c>
       <c r="D2" s="34">
         <f>((C2/3)*100)</f>
         <v>33.333333333333329</v>
       </c>
-      <c r="E2" s="92">
+      <c r="E2" s="127">
         <f>(AVERAGE(C2:C4))*100</f>
-        <v>100</v>
-      </c>
-      <c r="F2" s="5"/>
+        <v>66.666666666666657</v>
+      </c>
+      <c r="F2" s="4"/>
     </row>
     <row r="3" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="90"/>
-      <c r="B3" s="8" t="s">
+      <c r="A3" s="125"/>
+      <c r="B3" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="9">
+      <c r="C3" s="8">
         <v>1</v>
       </c>
       <c r="D3" s="35">
         <f t="shared" ref="D3:D4" si="0">((C3/3)*100)</f>
         <v>33.333333333333329</v>
       </c>
-      <c r="E3" s="93"/>
-      <c r="F3" s="5"/>
+      <c r="E3" s="128"/>
+      <c r="F3" s="4"/>
     </row>
     <row r="4" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="91"/>
-      <c r="B4" s="19" t="s">
+      <c r="A4" s="126"/>
+      <c r="B4" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="20">
-        <v>1</v>
+      <c r="C4" s="19">
+        <v>0</v>
       </c>
       <c r="D4" s="36">
         <f t="shared" si="0"/>
-        <v>33.333333333333329</v>
-      </c>
-      <c r="E4" s="94"/>
-      <c r="F4" s="5"/>
+        <v>0</v>
+      </c>
+      <c r="E4" s="129"/>
+      <c r="F4" s="4"/>
     </row>
     <row r="5" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="95" t="s">
+      <c r="A5" s="130" t="s">
         <v>7</v>
       </c>
       <c r="B5" s="27" t="s">
@@ -1947,17 +2417,17 @@
       </c>
       <c r="C5" s="28"/>
       <c r="D5" s="37">
-        <f>(AVERAGE(C6:C10)*100)*0.5</f>
+        <f>(AVERAGE(C6:C13)*100)*0.5</f>
         <v>0</v>
       </c>
-      <c r="E5" s="98">
-        <f>D5+D11</f>
+      <c r="E5" s="133">
+        <f>D5+D14</f>
         <v>0</v>
       </c>
-      <c r="F5" s="5"/>
+      <c r="F5" s="4"/>
     </row>
     <row r="6" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="96"/>
+      <c r="A6" s="131"/>
       <c r="B6" s="31" t="s">
         <v>30</v>
       </c>
@@ -1968,11 +2438,11 @@
         <f>(C6/8)*100</f>
         <v>0</v>
       </c>
-      <c r="E6" s="99"/>
-      <c r="F6" s="5"/>
+      <c r="E6" s="134"/>
+      <c r="F6" s="4"/>
     </row>
     <row r="7" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="96"/>
+      <c r="A7" s="131"/>
       <c r="B7" s="31" t="s">
         <v>31</v>
       </c>
@@ -1980,14 +2450,14 @@
         <v>0</v>
       </c>
       <c r="D7" s="38">
-        <f t="shared" ref="D7:D10" si="1">(C7/8)*100</f>
+        <f t="shared" ref="D7:D13" si="1">(C7/8)*100</f>
         <v>0</v>
       </c>
-      <c r="E7" s="99"/>
-      <c r="F7" s="5"/>
+      <c r="E7" s="134"/>
+      <c r="F7" s="4"/>
     </row>
     <row r="8" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="96"/>
+      <c r="A8" s="131"/>
       <c r="B8" s="31" t="s">
         <v>32</v>
       </c>
@@ -1998,11 +2468,11 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="E8" s="99"/>
-      <c r="F8" s="5"/>
+      <c r="E8" s="134"/>
+      <c r="F8" s="4"/>
     </row>
     <row r="9" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="96"/>
+      <c r="A9" s="131"/>
       <c r="B9" s="31" t="s">
         <v>33</v>
       </c>
@@ -2013,11 +2483,11 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="E9" s="99"/>
-      <c r="F9" s="5"/>
+      <c r="E9" s="134"/>
+      <c r="F9" s="4"/>
     </row>
     <row r="10" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="96"/>
+      <c r="A10" s="131"/>
       <c r="B10" s="31" t="s">
         <v>34</v>
       </c>
@@ -2028,340 +2498,361 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="E10" s="99"/>
-      <c r="F10" s="5"/>
-    </row>
-    <row r="11" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="97"/>
-      <c r="B11" s="29" t="s">
+      <c r="E10" s="134"/>
+      <c r="F10" s="4"/>
+    </row>
+    <row r="11" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="131"/>
+      <c r="B11" s="31" t="s">
+        <v>35</v>
+      </c>
+      <c r="C11" s="32">
+        <v>0</v>
+      </c>
+      <c r="D11" s="38">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E11" s="134"/>
+      <c r="F11" s="4"/>
+    </row>
+    <row r="12" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="131"/>
+      <c r="B12" s="31" t="s">
+        <v>36</v>
+      </c>
+      <c r="C12" s="32">
+        <v>0</v>
+      </c>
+      <c r="D12" s="38">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E12" s="134"/>
+      <c r="F12" s="4"/>
+    </row>
+    <row r="13" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="131"/>
+      <c r="B13" s="31" t="s">
+        <v>37</v>
+      </c>
+      <c r="C13" s="32">
+        <v>0</v>
+      </c>
+      <c r="D13" s="38">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E13" s="134"/>
+      <c r="F13" s="4"/>
+    </row>
+    <row r="14" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="132"/>
+      <c r="B14" s="29" t="s">
         <v>26</v>
       </c>
-      <c r="C11" s="30">
+      <c r="C14" s="30">
         <v>0</v>
       </c>
-      <c r="D11" s="39">
-        <f>(C11/2)*100</f>
+      <c r="D14" s="39">
+        <f>(C14/2)*100</f>
         <v>0</v>
       </c>
-      <c r="E11" s="100"/>
-      <c r="F11" s="5"/>
-    </row>
-    <row r="12" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="101" t="s">
-        <v>49</v>
-      </c>
-      <c r="B12" s="102" t="s">
-        <v>50</v>
-      </c>
-      <c r="C12" s="103"/>
-      <c r="D12" s="104">
-        <f>C12*100</f>
-        <v>0</v>
-      </c>
-      <c r="E12" s="105">
-        <f>D12</f>
-        <v>0</v>
-      </c>
-      <c r="F12" s="5"/>
-    </row>
-    <row r="13" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="25" t="s">
-        <v>53</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="C13" s="26"/>
-      <c r="D13" s="40"/>
-      <c r="E13" s="44"/>
-      <c r="F13" s="5"/>
-    </row>
-    <row r="14" spans="1:6" s="64" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="25"/>
-      <c r="B14" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="C14" s="26"/>
-      <c r="D14" s="40"/>
-      <c r="E14" s="44"/>
-      <c r="F14" s="5"/>
+      <c r="E14" s="135"/>
+      <c r="F14" s="4"/>
     </row>
     <row r="15" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="23"/>
-      <c r="B15" s="6"/>
-      <c r="C15" s="7"/>
-      <c r="D15" s="41"/>
-      <c r="E15" s="45"/>
-      <c r="F15" s="5"/>
+      <c r="A15" s="24"/>
+      <c r="B15" s="25"/>
+      <c r="C15" s="26"/>
+      <c r="D15" s="40"/>
+      <c r="E15" s="44"/>
+      <c r="F15" s="4"/>
     </row>
     <row r="16" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="23"/>
-      <c r="B16" s="6"/>
-      <c r="C16" s="7"/>
+      <c r="A16" s="22"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="6"/>
       <c r="D16" s="41"/>
       <c r="E16" s="45"/>
-      <c r="F16" s="5"/>
+      <c r="F16" s="4"/>
     </row>
     <row r="17" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="23"/>
-      <c r="B17" s="6"/>
-      <c r="C17" s="7"/>
+      <c r="A17" s="22"/>
+      <c r="B17" s="5"/>
+      <c r="C17" s="6"/>
       <c r="D17" s="41"/>
       <c r="E17" s="45"/>
-      <c r="F17" s="5"/>
+      <c r="F17" s="4"/>
     </row>
     <row r="18" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="23"/>
-      <c r="B18" s="6"/>
-      <c r="C18" s="7"/>
+      <c r="A18" s="22"/>
+      <c r="B18" s="5"/>
+      <c r="C18" s="6"/>
       <c r="D18" s="41"/>
       <c r="E18" s="45"/>
-      <c r="F18" s="5"/>
+      <c r="F18" s="4"/>
     </row>
     <row r="19" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="23"/>
-      <c r="B19" s="6"/>
-      <c r="C19" s="7"/>
+      <c r="A19" s="22"/>
+      <c r="B19" s="5"/>
+      <c r="C19" s="6"/>
       <c r="D19" s="41"/>
       <c r="E19" s="45"/>
-      <c r="F19" s="5"/>
+      <c r="F19" s="4"/>
     </row>
     <row r="20" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="23"/>
-      <c r="B20" s="6"/>
-      <c r="C20" s="7"/>
+      <c r="A20" s="22"/>
+      <c r="B20" s="5"/>
+      <c r="C20" s="6"/>
       <c r="D20" s="41"/>
       <c r="E20" s="45"/>
-      <c r="F20" s="5"/>
+      <c r="F20" s="4"/>
     </row>
     <row r="21" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="23"/>
-      <c r="B21" s="6"/>
-      <c r="C21" s="7"/>
+      <c r="A21" s="22"/>
+      <c r="B21" s="5"/>
+      <c r="C21" s="6"/>
       <c r="D21" s="41"/>
       <c r="E21" s="45"/>
-      <c r="F21" s="5"/>
+      <c r="F21" s="4"/>
     </row>
     <row r="22" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A22" s="23"/>
-      <c r="B22" s="6"/>
-      <c r="C22" s="7"/>
+      <c r="A22" s="22"/>
+      <c r="B22" s="5"/>
+      <c r="C22" s="6"/>
       <c r="D22" s="41"/>
       <c r="E22" s="45"/>
-      <c r="F22" s="5"/>
+      <c r="F22" s="4"/>
     </row>
     <row r="23" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A23" s="23"/>
-      <c r="B23" s="6"/>
-      <c r="C23" s="7"/>
+      <c r="A23" s="22"/>
+      <c r="B23" s="5"/>
+      <c r="C23" s="6"/>
       <c r="D23" s="41"/>
       <c r="E23" s="45"/>
-      <c r="F23" s="5"/>
+      <c r="F23" s="4"/>
     </row>
     <row r="24" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A24" s="23"/>
-      <c r="B24" s="6"/>
-      <c r="C24" s="7"/>
+      <c r="A24" s="22"/>
+      <c r="B24" s="5"/>
+      <c r="C24" s="6"/>
       <c r="D24" s="41"/>
       <c r="E24" s="45"/>
-      <c r="F24" s="5"/>
+      <c r="F24" s="4"/>
     </row>
     <row r="25" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A25" s="23"/>
-      <c r="B25" s="6"/>
-      <c r="C25" s="7"/>
+      <c r="A25" s="22"/>
+      <c r="B25" s="5"/>
+      <c r="C25" s="6"/>
       <c r="D25" s="41"/>
       <c r="E25" s="45"/>
-      <c r="F25" s="5"/>
+      <c r="F25" s="4"/>
     </row>
     <row r="26" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A26" s="23"/>
-      <c r="B26" s="6"/>
-      <c r="C26" s="7"/>
+      <c r="A26" s="22"/>
+      <c r="B26" s="5"/>
+      <c r="C26" s="6"/>
       <c r="D26" s="41"/>
       <c r="E26" s="45"/>
-      <c r="F26" s="5"/>
+      <c r="F26" s="4"/>
     </row>
     <row r="27" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A27" s="23"/>
-      <c r="B27" s="6"/>
-      <c r="C27" s="7"/>
+      <c r="A27" s="22"/>
+      <c r="B27" s="5"/>
+      <c r="C27" s="6"/>
       <c r="D27" s="41"/>
       <c r="E27" s="45"/>
-      <c r="F27" s="5"/>
+      <c r="F27" s="4"/>
     </row>
     <row r="28" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A28" s="23"/>
-      <c r="B28" s="6"/>
-      <c r="C28" s="7"/>
+      <c r="A28" s="22"/>
+      <c r="B28" s="5"/>
+      <c r="C28" s="6"/>
       <c r="D28" s="41"/>
       <c r="E28" s="45"/>
-      <c r="F28" s="5"/>
+      <c r="F28" s="4"/>
     </row>
     <row r="29" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A29" s="23"/>
-      <c r="B29" s="6"/>
-      <c r="C29" s="7"/>
+      <c r="A29" s="22"/>
+      <c r="B29" s="5"/>
+      <c r="C29" s="6"/>
       <c r="D29" s="41"/>
       <c r="E29" s="45"/>
-      <c r="F29" s="5"/>
+      <c r="F29" s="4"/>
     </row>
     <row r="30" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A30" s="23"/>
-      <c r="B30" s="6"/>
-      <c r="C30" s="7"/>
+      <c r="A30" s="22"/>
+      <c r="B30" s="5"/>
+      <c r="C30" s="6"/>
       <c r="D30" s="41"/>
       <c r="E30" s="45"/>
-      <c r="F30" s="5"/>
+      <c r="F30" s="4"/>
     </row>
     <row r="31" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A31" s="23"/>
-      <c r="B31" s="6"/>
-      <c r="C31" s="7"/>
+      <c r="A31" s="22"/>
+      <c r="B31" s="5"/>
+      <c r="C31" s="6"/>
       <c r="D31" s="41"/>
       <c r="E31" s="45"/>
-      <c r="F31" s="5"/>
+      <c r="F31" s="4"/>
     </row>
     <row r="32" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A32" s="23"/>
-      <c r="B32" s="6"/>
-      <c r="C32" s="7"/>
+      <c r="A32" s="22"/>
+      <c r="B32" s="5"/>
+      <c r="C32" s="6"/>
       <c r="D32" s="41"/>
       <c r="E32" s="45"/>
-      <c r="F32" s="5"/>
+      <c r="F32" s="4"/>
     </row>
     <row r="33" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A33" s="23"/>
-      <c r="B33" s="6"/>
-      <c r="C33" s="7"/>
+      <c r="A33" s="22"/>
+      <c r="B33" s="5"/>
+      <c r="C33" s="6"/>
       <c r="D33" s="41"/>
       <c r="E33" s="45"/>
-      <c r="F33" s="5"/>
+      <c r="F33" s="4"/>
     </row>
     <row r="34" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A34" s="23"/>
-      <c r="B34" s="6"/>
-      <c r="C34" s="7"/>
+      <c r="A34" s="22"/>
+      <c r="B34" s="5"/>
+      <c r="C34" s="6"/>
       <c r="D34" s="41"/>
       <c r="E34" s="45"/>
-      <c r="F34" s="5"/>
+      <c r="F34" s="4"/>
     </row>
     <row r="35" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A35" s="23"/>
-      <c r="B35" s="6"/>
-      <c r="C35" s="7"/>
+      <c r="A35" s="22"/>
+      <c r="B35" s="5"/>
+      <c r="C35" s="6"/>
       <c r="D35" s="41"/>
       <c r="E35" s="45"/>
-      <c r="F35" s="5"/>
+      <c r="F35" s="4"/>
     </row>
     <row r="36" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A36" s="23"/>
-      <c r="B36" s="6"/>
-      <c r="C36" s="7"/>
+      <c r="A36" s="22"/>
+      <c r="B36" s="5"/>
+      <c r="C36" s="6"/>
       <c r="D36" s="41"/>
       <c r="E36" s="45"/>
-      <c r="F36" s="5"/>
+      <c r="F36" s="4"/>
     </row>
     <row r="37" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A37" s="23"/>
-      <c r="B37" s="6"/>
-      <c r="C37" s="7"/>
+      <c r="A37" s="22"/>
+      <c r="B37" s="5"/>
+      <c r="C37" s="6"/>
       <c r="D37" s="41"/>
       <c r="E37" s="45"/>
-      <c r="F37" s="5"/>
-    </row>
-    <row r="38" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="24"/>
-      <c r="B38" s="16"/>
-      <c r="C38" s="15"/>
-      <c r="D38" s="42"/>
-      <c r="E38" s="46"/>
-      <c r="F38" s="5"/>
-    </row>
-    <row r="39" spans="1:6" ht="24" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="86" t="s">
+      <c r="F37" s="4"/>
+    </row>
+    <row r="38" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A38" s="22"/>
+      <c r="B38" s="5"/>
+      <c r="C38" s="6"/>
+      <c r="D38" s="41"/>
+      <c r="E38" s="45"/>
+      <c r="F38" s="4"/>
+    </row>
+    <row r="39" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A39" s="22"/>
+      <c r="B39" s="5"/>
+      <c r="C39" s="6"/>
+      <c r="D39" s="41"/>
+      <c r="E39" s="45"/>
+      <c r="F39" s="4"/>
+    </row>
+    <row r="40" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="23"/>
+      <c r="B40" s="15"/>
+      <c r="C40" s="14"/>
+      <c r="D40" s="42"/>
+      <c r="E40" s="46"/>
+      <c r="F40" s="4"/>
+    </row>
+    <row r="41" spans="1:6" ht="24" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="121" t="s">
         <v>27</v>
       </c>
-      <c r="B39" s="87"/>
-      <c r="C39" s="87"/>
-      <c r="D39" s="88"/>
-      <c r="E39" s="47">
+      <c r="B41" s="122"/>
+      <c r="C41" s="122"/>
+      <c r="D41" s="123"/>
+      <c r="E41" s="47">
         <f>(AVERAGE(E2,E5))</f>
-        <v>50</v>
-      </c>
-      <c r="F39" s="5"/>
-    </row>
-    <row r="40" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A40" s="5"/>
-      <c r="B40" s="4"/>
-      <c r="C40" s="5"/>
-      <c r="D40" s="5"/>
-      <c r="E40" s="5"/>
-      <c r="F40" s="5"/>
-    </row>
-    <row r="41" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A41" s="5"/>
-      <c r="B41" s="4"/>
-      <c r="C41" s="5"/>
-      <c r="D41" s="5"/>
-      <c r="E41" s="5"/>
-      <c r="F41" s="5"/>
+        <v>33.333333333333329</v>
+      </c>
+      <c r="F41" s="4"/>
     </row>
     <row r="42" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A42" s="5"/>
-      <c r="B42" s="4"/>
-      <c r="C42" s="5"/>
-      <c r="D42" s="5"/>
-      <c r="E42" s="5"/>
-      <c r="F42" s="5"/>
+      <c r="A42" s="4"/>
+      <c r="B42" s="3"/>
+      <c r="C42" s="4"/>
+      <c r="D42" s="4"/>
+      <c r="E42" s="4"/>
+      <c r="F42" s="4"/>
     </row>
     <row r="43" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A43" s="5"/>
-      <c r="B43" s="4"/>
-      <c r="C43" s="5"/>
-      <c r="D43" s="5"/>
-      <c r="E43" s="5"/>
-      <c r="F43" s="5"/>
+      <c r="A43" s="4"/>
+      <c r="B43" s="3"/>
+      <c r="C43" s="4"/>
+      <c r="D43" s="4"/>
+      <c r="E43" s="4"/>
+      <c r="F43" s="4"/>
     </row>
     <row r="44" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A44" s="5"/>
-      <c r="B44" s="4"/>
-      <c r="C44" s="5"/>
-      <c r="D44" s="5"/>
-      <c r="E44" s="5"/>
-      <c r="F44" s="5"/>
+      <c r="A44" s="4"/>
+      <c r="B44" s="3"/>
+      <c r="C44" s="4"/>
+      <c r="D44" s="4"/>
+      <c r="E44" s="4"/>
+      <c r="F44" s="4"/>
     </row>
     <row r="45" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A45" s="5"/>
-      <c r="B45" s="4"/>
-      <c r="C45" s="5"/>
-      <c r="D45" s="5"/>
-      <c r="E45" s="5"/>
-      <c r="F45" s="5"/>
+      <c r="A45" s="4"/>
+      <c r="B45" s="3"/>
+      <c r="C45" s="4"/>
+      <c r="D45" s="4"/>
+      <c r="E45" s="4"/>
+      <c r="F45" s="4"/>
     </row>
     <row r="46" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A46" s="5"/>
-      <c r="B46" s="4"/>
-      <c r="C46" s="5"/>
-      <c r="D46" s="5"/>
-      <c r="E46" s="5"/>
-      <c r="F46" s="5"/>
+      <c r="A46" s="4"/>
+      <c r="B46" s="3"/>
+      <c r="C46" s="4"/>
+      <c r="D46" s="4"/>
+      <c r="E46" s="4"/>
+      <c r="F46" s="4"/>
     </row>
     <row r="47" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A47" s="5"/>
-      <c r="B47" s="4"/>
-      <c r="C47" s="5"/>
-      <c r="D47" s="5"/>
-      <c r="E47" s="5"/>
-      <c r="F47" s="5"/>
+      <c r="A47" s="4"/>
+      <c r="B47" s="3"/>
+      <c r="C47" s="4"/>
+      <c r="D47" s="4"/>
+      <c r="E47" s="4"/>
+      <c r="F47" s="4"/>
+    </row>
+    <row r="48" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A48" s="4"/>
+      <c r="B48" s="3"/>
+      <c r="C48" s="4"/>
+      <c r="D48" s="4"/>
+      <c r="E48" s="4"/>
+      <c r="F48" s="4"/>
+    </row>
+    <row r="49" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A49" s="4"/>
+      <c r="B49" s="3"/>
+      <c r="C49" s="4"/>
+      <c r="D49" s="4"/>
+      <c r="E49" s="4"/>
+      <c r="F49" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="5">
-    <mergeCell ref="A39:D39"/>
+    <mergeCell ref="A41:D41"/>
     <mergeCell ref="A2:A4"/>
     <mergeCell ref="E2:E4"/>
-    <mergeCell ref="A5:A11"/>
-    <mergeCell ref="E5:E11"/>
+    <mergeCell ref="A5:A14"/>
+    <mergeCell ref="E5:E14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2384,68 +2875,68 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:4" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="C2" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="D2" s="12" t="s">
+      <c r="D2" s="11" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B3" s="13" t="s">
+      <c r="B3" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="C3" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="14" t="s">
+      <c r="D3" s="13" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="11" t="s">
+      <c r="C4" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="10" t="s">
+      <c r="D4" s="9" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B5" s="13" t="s">
+      <c r="B5" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="13" t="s">
+      <c r="C5" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="14" t="s">
+      <c r="D5" s="13" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B6" s="11" t="s">
+      <c r="B6" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="11" t="s">
+      <c r="C6" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="10" t="s">
+      <c r="D6" s="9" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B7" s="13" t="s">
+      <c r="B7" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="13" t="s">
+      <c r="C7" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="D7" s="14" t="s">
+      <c r="D7" s="13" t="s">
         <v>20</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Day 2 - Workplan
</commit_message>
<xml_diff>
--- a/Workplan.xlsx
+++ b/Workplan.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="69">
   <si>
     <t>ACTIVITIES</t>
   </si>
@@ -303,6 +303,9 @@
   </si>
   <si>
     <t>In Progress</t>
+  </si>
+  <si>
+    <t>Second actual commit will be done on the presentation day</t>
   </si>
 </sst>
 </file>
@@ -450,7 +453,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="35">
+  <borders count="41">
     <border>
       <left/>
       <right/>
@@ -922,11 +925,87 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="136">
+  <cellXfs count="173">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1085,11 +1164,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="8" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="8" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1106,7 +1181,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="8" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="8" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1115,9 +1189,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="8" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="8" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="8" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1136,9 +1207,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="2"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="6"/>
     </xf>
@@ -1154,9 +1222,6 @@
     <xf numFmtId="14" fontId="5" fillId="8" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="5" fillId="8" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1171,14 +1236,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -1189,63 +1247,60 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="8" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -1289,6 +1344,117 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="8" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="8" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="8" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1594,8 +1760,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I45"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1612,30 +1778,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="48" customFormat="1" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="114" t="s">
+      <c r="A1" s="93" t="s">
         <v>64</v>
       </c>
-      <c r="B1" s="114"/>
-      <c r="C1" s="114"/>
-      <c r="D1" s="114"/>
-      <c r="E1" s="114"/>
-      <c r="F1" s="114"/>
-      <c r="G1" s="114"/>
-      <c r="H1" s="114"/>
-      <c r="I1" s="114"/>
+      <c r="B1" s="93"/>
+      <c r="C1" s="93"/>
+      <c r="D1" s="93"/>
+      <c r="E1" s="93"/>
+      <c r="F1" s="93"/>
+      <c r="G1" s="93"/>
+      <c r="H1" s="93"/>
+      <c r="I1" s="93"/>
     </row>
     <row r="2" spans="1:9" s="48" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A2" s="120" t="s">
+      <c r="A2" s="102" t="s">
         <v>45</v>
       </c>
-      <c r="B2" s="120"/>
-      <c r="C2" s="120"/>
-      <c r="D2" s="120"/>
-      <c r="E2" s="120"/>
-      <c r="F2" s="120"/>
-      <c r="G2" s="120"/>
-      <c r="H2" s="120"/>
-      <c r="I2" s="120"/>
+      <c r="B2" s="102"/>
+      <c r="C2" s="102"/>
+      <c r="D2" s="102"/>
+      <c r="E2" s="102"/>
+      <c r="F2" s="102"/>
+      <c r="G2" s="102"/>
+      <c r="H2" s="102"/>
+      <c r="I2" s="102"/>
     </row>
     <row r="3" spans="1:9" s="48" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="49"/>
@@ -1649,486 +1815,552 @@
     </row>
     <row r="4" spans="1:9" s="48" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="104" t="s">
+      <c r="A5" s="103" t="s">
         <v>49</v>
       </c>
-      <c r="B5" s="104" t="s">
+      <c r="B5" s="103" t="s">
         <v>38</v>
       </c>
-      <c r="C5" s="118" t="s">
+      <c r="C5" s="99" t="s">
         <v>40</v>
       </c>
-      <c r="D5" s="116" t="s">
+      <c r="D5" s="152" t="s">
         <v>41</v>
       </c>
-      <c r="E5" s="118" t="s">
+      <c r="E5" s="99" t="s">
         <v>42</v>
       </c>
-      <c r="F5" s="116" t="s">
+      <c r="F5" s="97" t="s">
         <v>43</v>
       </c>
-      <c r="G5" s="106" t="s">
+      <c r="G5" s="162" t="s">
         <v>60</v>
       </c>
-      <c r="H5" s="106" t="s">
+      <c r="H5" s="95" t="s">
         <v>44</v>
       </c>
-      <c r="I5" s="106" t="s">
+      <c r="I5" s="95" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="105"/>
-      <c r="B6" s="105"/>
-      <c r="C6" s="119"/>
-      <c r="D6" s="117"/>
-      <c r="E6" s="119"/>
-      <c r="F6" s="117"/>
-      <c r="G6" s="107"/>
-      <c r="H6" s="107"/>
-      <c r="I6" s="107"/>
-    </row>
-    <row r="7" spans="1:9" s="48" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="108">
+      <c r="A6" s="104"/>
+      <c r="B6" s="104"/>
+      <c r="C6" s="100"/>
+      <c r="D6" s="153"/>
+      <c r="E6" s="100"/>
+      <c r="F6" s="98"/>
+      <c r="G6" s="163"/>
+      <c r="H6" s="96"/>
+      <c r="I6" s="96"/>
+    </row>
+    <row r="7" spans="1:9" s="48" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="105">
         <v>1</v>
       </c>
-      <c r="B7" s="61" t="s">
+      <c r="B7" s="59" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="83"/>
-      <c r="D7" s="58"/>
-      <c r="E7" s="83"/>
-      <c r="F7" s="58"/>
-      <c r="G7" s="70"/>
-      <c r="H7" s="70"/>
-      <c r="I7" s="70"/>
+      <c r="C7" s="78"/>
+      <c r="D7" s="154"/>
+      <c r="E7" s="141"/>
+      <c r="F7" s="142"/>
+      <c r="G7" s="164"/>
+      <c r="H7" s="67"/>
+      <c r="I7" s="67"/>
     </row>
     <row r="8" spans="1:9" ht="75" x14ac:dyDescent="0.25">
-      <c r="A8" s="109"/>
-      <c r="B8" s="62" t="s">
+      <c r="A8" s="106"/>
+      <c r="B8" s="60" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="84">
-        <v>42565</v>
-      </c>
-      <c r="D8" s="85">
-        <v>42565</v>
-      </c>
-      <c r="E8" s="84">
-        <v>42565</v>
-      </c>
-      <c r="F8" s="85">
-        <v>42565</v>
-      </c>
-      <c r="G8" s="74">
+      <c r="C8" s="79">
+        <v>42565</v>
+      </c>
+      <c r="D8" s="150">
+        <v>42565</v>
+      </c>
+      <c r="E8" s="145">
+        <v>42565</v>
+      </c>
+      <c r="F8" s="146">
+        <v>42565</v>
+      </c>
+      <c r="G8" s="151">
         <v>100</v>
       </c>
-      <c r="H8" s="78" t="s">
+      <c r="H8" s="74" t="s">
         <v>48</v>
       </c>
-      <c r="I8" s="71" t="s">
+      <c r="I8" s="68" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="109"/>
-      <c r="B9" s="63" t="s">
+      <c r="A9" s="106"/>
+      <c r="B9" s="61" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="84">
-        <v>42565</v>
-      </c>
-      <c r="D9" s="85">
-        <v>42565</v>
-      </c>
-      <c r="E9" s="84">
-        <v>42565</v>
-      </c>
-      <c r="F9" s="85">
-        <v>42565</v>
-      </c>
-      <c r="G9" s="74">
+      <c r="C9" s="79">
+        <v>42565</v>
+      </c>
+      <c r="D9" s="150">
+        <v>42565</v>
+      </c>
+      <c r="E9" s="79">
+        <v>42565</v>
+      </c>
+      <c r="F9" s="80">
+        <v>42565</v>
+      </c>
+      <c r="G9" s="151">
         <v>100</v>
       </c>
-      <c r="H9" s="78" t="s">
+      <c r="H9" s="74" t="s">
         <v>48</v>
       </c>
-      <c r="I9" s="68"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="109"/>
-      <c r="B10" s="63" t="s">
+      <c r="I9" s="66"/>
+    </row>
+    <row r="10" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="106"/>
+      <c r="B10" s="61" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="84">
-        <v>42565</v>
-      </c>
-      <c r="D10" s="85">
-        <v>42565</v>
-      </c>
-      <c r="E10" s="84">
-        <v>42565</v>
-      </c>
-      <c r="F10" s="85">
-        <v>42565</v>
-      </c>
-      <c r="G10" s="74">
+      <c r="C10" s="79">
+        <v>42565</v>
+      </c>
+      <c r="D10" s="150">
+        <v>42565</v>
+      </c>
+      <c r="E10" s="82">
+        <v>42565</v>
+      </c>
+      <c r="F10" s="83">
+        <v>42565</v>
+      </c>
+      <c r="G10" s="151">
         <v>100</v>
       </c>
-      <c r="H10" s="78" t="s">
+      <c r="H10" s="74" t="s">
         <v>48</v>
       </c>
-      <c r="I10" s="68"/>
+      <c r="I10" s="66"/>
     </row>
     <row r="11" spans="1:9" s="50" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="109"/>
-      <c r="B11" s="64" t="s">
+      <c r="A11" s="106"/>
+      <c r="B11" s="62" t="s">
         <v>66</v>
       </c>
-      <c r="C11" s="86"/>
-      <c r="D11" s="87"/>
-      <c r="E11" s="102">
-        <v>42565</v>
-      </c>
-      <c r="F11" s="87"/>
-      <c r="G11" s="75"/>
-      <c r="H11" s="79"/>
-      <c r="I11" s="72"/>
+      <c r="C11" s="81"/>
+      <c r="D11" s="155"/>
+      <c r="E11" s="143">
+        <v>42565</v>
+      </c>
+      <c r="F11" s="144"/>
+      <c r="G11" s="165"/>
+      <c r="H11" s="75"/>
+      <c r="I11" s="69"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="109"/>
-      <c r="B12" s="63" t="s">
+      <c r="A12" s="106"/>
+      <c r="B12" s="61" t="s">
         <v>29</v>
       </c>
-      <c r="C12" s="111"/>
-      <c r="D12" s="112"/>
-      <c r="E12" s="112"/>
-      <c r="F12" s="112"/>
-      <c r="G12" s="112"/>
-      <c r="H12" s="112"/>
-      <c r="I12" s="113"/>
+      <c r="C12" s="108"/>
+      <c r="D12" s="109"/>
+      <c r="E12" s="109"/>
+      <c r="F12" s="109"/>
+      <c r="G12" s="109"/>
+      <c r="H12" s="109"/>
+      <c r="I12" s="110"/>
     </row>
     <row r="13" spans="1:9" s="48" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="109"/>
-      <c r="B13" s="82" t="s">
+      <c r="A13" s="106"/>
+      <c r="B13" s="77" t="s">
         <v>30</v>
       </c>
-      <c r="C13" s="84">
-        <v>42565</v>
-      </c>
-      <c r="D13" s="85">
-        <v>42565</v>
-      </c>
-      <c r="E13" s="84">
-        <v>42565</v>
-      </c>
-      <c r="F13" s="84">
-        <v>42565</v>
-      </c>
-      <c r="G13" s="74">
+      <c r="C13" s="79">
+        <v>42565</v>
+      </c>
+      <c r="D13" s="150">
+        <v>42565</v>
+      </c>
+      <c r="E13" s="79">
+        <v>42565</v>
+      </c>
+      <c r="F13" s="80">
+        <v>42565</v>
+      </c>
+      <c r="G13" s="151">
         <v>100</v>
       </c>
-      <c r="H13" s="78" t="s">
+      <c r="H13" s="74" t="s">
         <v>48</v>
       </c>
-      <c r="I13" s="68"/>
+      <c r="I13" s="66"/>
     </row>
     <row r="14" spans="1:9" s="48" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="109"/>
-      <c r="B14" s="82" t="s">
+      <c r="A14" s="106"/>
+      <c r="B14" s="77" t="s">
         <v>31</v>
       </c>
-      <c r="C14" s="84">
-        <v>42565</v>
-      </c>
-      <c r="D14" s="85">
-        <v>42565</v>
-      </c>
-      <c r="E14" s="84">
-        <v>42565</v>
-      </c>
-      <c r="F14" s="84">
-        <v>42565</v>
-      </c>
-      <c r="G14" s="74">
+      <c r="C14" s="79">
+        <v>42565</v>
+      </c>
+      <c r="D14" s="150">
+        <v>42565</v>
+      </c>
+      <c r="E14" s="79">
+        <v>42565</v>
+      </c>
+      <c r="F14" s="80">
+        <v>42565</v>
+      </c>
+      <c r="G14" s="151">
         <v>100</v>
       </c>
-      <c r="H14" s="78" t="s">
+      <c r="H14" s="74" t="s">
         <v>48</v>
       </c>
-      <c r="I14" s="68"/>
+      <c r="I14" s="66"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="109"/>
-      <c r="B15" s="82" t="s">
+      <c r="A15" s="106"/>
+      <c r="B15" s="77" t="s">
         <v>35</v>
       </c>
-      <c r="C15" s="84">
-        <v>42565</v>
-      </c>
-      <c r="D15" s="85">
-        <v>42565</v>
-      </c>
-      <c r="E15" s="84">
-        <v>42565</v>
-      </c>
-      <c r="F15" s="84">
-        <v>42565</v>
-      </c>
-      <c r="G15" s="74">
+      <c r="C15" s="79">
+        <v>42565</v>
+      </c>
+      <c r="D15" s="150">
+        <v>42565</v>
+      </c>
+      <c r="E15" s="79">
+        <v>42565</v>
+      </c>
+      <c r="F15" s="80">
+        <v>42565</v>
+      </c>
+      <c r="G15" s="151">
         <v>100</v>
       </c>
-      <c r="H15" s="78" t="s">
+      <c r="H15" s="74" t="s">
         <v>48</v>
       </c>
-      <c r="I15" s="68"/>
+      <c r="I15" s="66"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="109"/>
-      <c r="B16" s="82" t="s">
+      <c r="A16" s="106"/>
+      <c r="B16" s="77" t="s">
         <v>36</v>
       </c>
-      <c r="C16" s="84">
-        <v>42565</v>
-      </c>
-      <c r="D16" s="85">
-        <v>42565</v>
-      </c>
-      <c r="E16" s="84">
-        <v>42565</v>
-      </c>
-      <c r="F16" s="84">
-        <v>42565</v>
-      </c>
-      <c r="G16" s="74">
+      <c r="C16" s="79">
+        <v>42565</v>
+      </c>
+      <c r="D16" s="150">
+        <v>42565</v>
+      </c>
+      <c r="E16" s="79">
+        <v>42565</v>
+      </c>
+      <c r="F16" s="80">
+        <v>42565</v>
+      </c>
+      <c r="G16" s="151">
         <v>100</v>
       </c>
-      <c r="H16" s="78" t="s">
+      <c r="H16" s="74" t="s">
         <v>48</v>
       </c>
-      <c r="I16" s="68"/>
+      <c r="I16" s="66"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="109"/>
-      <c r="B17" s="82" t="s">
+      <c r="A17" s="106"/>
+      <c r="B17" s="77" t="s">
         <v>37</v>
       </c>
-      <c r="C17" s="84">
-        <v>42565</v>
-      </c>
-      <c r="D17" s="85">
-        <v>42565</v>
-      </c>
-      <c r="E17" s="84">
-        <v>42565</v>
-      </c>
-      <c r="F17" s="84">
-        <v>42565</v>
-      </c>
-      <c r="G17" s="74">
+      <c r="C17" s="79">
+        <v>42565</v>
+      </c>
+      <c r="D17" s="150">
+        <v>42565</v>
+      </c>
+      <c r="E17" s="79">
+        <v>42565</v>
+      </c>
+      <c r="F17" s="80">
+        <v>42565</v>
+      </c>
+      <c r="G17" s="151">
         <v>100</v>
       </c>
-      <c r="H17" s="78" t="s">
+      <c r="H17" s="74" t="s">
         <v>48</v>
       </c>
-      <c r="I17" s="68"/>
+      <c r="I17" s="66"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="109"/>
-      <c r="B18" s="63" t="s">
+      <c r="A18" s="106"/>
+      <c r="B18" s="61" t="s">
         <v>26</v>
       </c>
-      <c r="C18" s="84">
-        <v>42565</v>
-      </c>
-      <c r="D18" s="85">
-        <v>42565</v>
-      </c>
-      <c r="E18" s="84">
-        <v>42565</v>
-      </c>
-      <c r="F18" s="84">
-        <v>42565</v>
-      </c>
-      <c r="G18" s="74">
+      <c r="C18" s="79">
+        <v>42565</v>
+      </c>
+      <c r="D18" s="150">
+        <v>42565</v>
+      </c>
+      <c r="E18" s="79">
+        <v>42565</v>
+      </c>
+      <c r="F18" s="80">
+        <v>42565</v>
+      </c>
+      <c r="G18" s="151">
         <v>100</v>
       </c>
-      <c r="H18" s="78" t="s">
+      <c r="H18" s="74" t="s">
         <v>48</v>
       </c>
-      <c r="I18" s="68"/>
+      <c r="I18" s="66"/>
     </row>
     <row r="19" spans="1:9" s="50" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="109"/>
-      <c r="B19" s="65" t="s">
+      <c r="A19" s="106"/>
+      <c r="B19" s="63" t="s">
         <v>50</v>
       </c>
-      <c r="C19" s="86"/>
-      <c r="D19" s="87"/>
-      <c r="E19" s="96"/>
-      <c r="F19" s="97"/>
-      <c r="G19" s="75"/>
-      <c r="H19" s="75"/>
-      <c r="I19" s="72"/>
-    </row>
-    <row r="20" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="110"/>
-      <c r="B20" s="80" t="s">
+      <c r="C19" s="81"/>
+      <c r="D19" s="155"/>
+      <c r="E19" s="147"/>
+      <c r="F19" s="148"/>
+      <c r="G19" s="165"/>
+      <c r="H19" s="71"/>
+      <c r="I19" s="69"/>
+    </row>
+    <row r="20" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="107"/>
+      <c r="B20" s="128" t="s">
         <v>51</v>
       </c>
-      <c r="C20" s="88">
-        <v>42565</v>
-      </c>
-      <c r="D20" s="89">
+      <c r="C20" s="82">
+        <v>42565</v>
+      </c>
+      <c r="D20" s="156">
         <v>42573</v>
       </c>
-      <c r="E20" s="89">
-        <v>42565</v>
-      </c>
-      <c r="F20" s="89"/>
-      <c r="G20" s="76">
-        <v>50</v>
-      </c>
-      <c r="H20" s="76" t="s">
+      <c r="E20" s="149">
+        <v>42565</v>
+      </c>
+      <c r="F20" s="83">
+        <v>42566</v>
+      </c>
+      <c r="G20" s="166">
+        <v>100</v>
+      </c>
+      <c r="H20" s="72" t="s">
+        <v>48</v>
+      </c>
+      <c r="I20" s="127" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A21" s="105">
+        <v>2</v>
+      </c>
+      <c r="B21" s="65" t="s">
+        <v>52</v>
+      </c>
+      <c r="C21" s="84"/>
+      <c r="D21" s="157"/>
+      <c r="E21" s="84"/>
+      <c r="F21" s="85"/>
+      <c r="G21" s="167"/>
+      <c r="H21" s="73"/>
+      <c r="I21" s="70"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" s="106"/>
+      <c r="B22" s="61" t="s">
+        <v>53</v>
+      </c>
+      <c r="C22" s="134">
+        <v>42566</v>
+      </c>
+      <c r="D22" s="158">
+        <v>42566</v>
+      </c>
+      <c r="E22" s="126">
+        <v>42566</v>
+      </c>
+      <c r="F22" s="129">
+        <v>42566</v>
+      </c>
+      <c r="G22" s="140">
+        <v>100</v>
+      </c>
+      <c r="H22" s="130" t="s">
+        <v>48</v>
+      </c>
+      <c r="I22" s="66"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" s="106"/>
+      <c r="B23" s="61" t="s">
+        <v>54</v>
+      </c>
+      <c r="C23" s="134">
+        <v>42566</v>
+      </c>
+      <c r="D23" s="158">
+        <v>42566</v>
+      </c>
+      <c r="E23" s="126">
+        <v>42566</v>
+      </c>
+      <c r="F23" s="129">
+        <v>42566</v>
+      </c>
+      <c r="G23" s="140">
+        <v>100</v>
+      </c>
+      <c r="H23" s="130" t="s">
+        <v>48</v>
+      </c>
+      <c r="I23" s="66"/>
+    </row>
+    <row r="24" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="107"/>
+      <c r="B24" s="76" t="s">
+        <v>55</v>
+      </c>
+      <c r="C24" s="139">
+        <v>42566</v>
+      </c>
+      <c r="D24" s="159">
+        <v>42566</v>
+      </c>
+      <c r="E24" s="126">
+        <v>42566</v>
+      </c>
+      <c r="F24" s="129">
+        <v>42566</v>
+      </c>
+      <c r="G24" s="140">
+        <v>100</v>
+      </c>
+      <c r="H24" s="131" t="s">
+        <v>48</v>
+      </c>
+      <c r="I24" s="64"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" s="132">
+        <v>3</v>
+      </c>
+      <c r="B25" s="135" t="s">
+        <v>56</v>
+      </c>
+      <c r="C25" s="136">
+        <v>42569</v>
+      </c>
+      <c r="D25" s="160">
+        <v>42569</v>
+      </c>
+      <c r="E25" s="126">
+        <v>42566</v>
+      </c>
+      <c r="F25" s="137"/>
+      <c r="G25" s="171">
+        <v>10</v>
+      </c>
+      <c r="H25" s="172" t="s">
         <v>67</v>
       </c>
-      <c r="I20" s="66"/>
-    </row>
-    <row r="21" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="108">
-        <v>2</v>
-      </c>
-      <c r="B21" s="67" t="s">
-        <v>52</v>
-      </c>
-      <c r="C21" s="90"/>
-      <c r="D21" s="91"/>
-      <c r="E21" s="90"/>
-      <c r="F21" s="91"/>
-      <c r="G21" s="77"/>
-      <c r="H21" s="77"/>
-      <c r="I21" s="73"/>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="109"/>
-      <c r="B22" s="63" t="s">
-        <v>53</v>
-      </c>
-      <c r="C22" s="92"/>
-      <c r="D22" s="56"/>
-      <c r="E22" s="92"/>
-      <c r="F22" s="56"/>
-      <c r="G22" s="68"/>
-      <c r="H22" s="68"/>
-      <c r="I22" s="68"/>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="109"/>
-      <c r="B23" s="63" t="s">
-        <v>54</v>
-      </c>
-      <c r="C23" s="92"/>
-      <c r="D23" s="56"/>
-      <c r="E23" s="92"/>
-      <c r="F23" s="56"/>
-      <c r="G23" s="68"/>
-      <c r="H23" s="68"/>
-      <c r="I23" s="68"/>
-    </row>
-    <row r="24" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="110"/>
-      <c r="B24" s="80" t="s">
-        <v>55</v>
-      </c>
-      <c r="C24" s="93"/>
-      <c r="D24" s="57"/>
-      <c r="E24" s="93"/>
-      <c r="F24" s="57"/>
-      <c r="G24" s="66"/>
-      <c r="H24" s="66"/>
-      <c r="I24" s="66"/>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" s="108">
-        <v>3</v>
-      </c>
-      <c r="B25" s="81" t="s">
-        <v>56</v>
-      </c>
-      <c r="C25" s="94"/>
-      <c r="D25" s="60"/>
-      <c r="E25" s="94"/>
-      <c r="F25" s="60"/>
-      <c r="G25" s="69"/>
-      <c r="H25" s="69"/>
-      <c r="I25" s="69"/>
+      <c r="I25" s="138"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" s="109"/>
-      <c r="B26" s="63" t="s">
+      <c r="A26" s="106"/>
+      <c r="B26" s="61" t="s">
         <v>57</v>
       </c>
-      <c r="C26" s="92"/>
-      <c r="D26" s="56"/>
-      <c r="E26" s="92"/>
+      <c r="C26" s="126">
+        <v>42569</v>
+      </c>
+      <c r="D26" s="158">
+        <v>42569</v>
+      </c>
+      <c r="E26" s="86"/>
       <c r="F26" s="56"/>
-      <c r="G26" s="68"/>
-      <c r="H26" s="68"/>
-      <c r="I26" s="68"/>
+      <c r="G26" s="168"/>
+      <c r="H26" s="66"/>
+      <c r="I26" s="66"/>
     </row>
     <row r="27" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="110"/>
-      <c r="B27" s="80" t="s">
+      <c r="A27" s="107"/>
+      <c r="B27" s="76" t="s">
         <v>58</v>
       </c>
-      <c r="C27" s="93"/>
-      <c r="D27" s="57"/>
-      <c r="E27" s="93"/>
+      <c r="C27" s="133">
+        <v>42569</v>
+      </c>
+      <c r="D27" s="159">
+        <v>42569</v>
+      </c>
+      <c r="E27" s="87"/>
       <c r="F27" s="57"/>
-      <c r="G27" s="66"/>
-      <c r="H27" s="66"/>
-      <c r="I27" s="66"/>
+      <c r="G27" s="169"/>
+      <c r="H27" s="64"/>
+      <c r="I27" s="64"/>
     </row>
     <row r="28" spans="1:9" s="48" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A28" s="108">
+      <c r="A28" s="105">
         <v>4</v>
       </c>
-      <c r="B28" s="67" t="s">
+      <c r="B28" s="65" t="s">
         <v>59</v>
       </c>
-      <c r="C28" s="95"/>
-      <c r="D28" s="59"/>
-      <c r="E28" s="95"/>
-      <c r="F28" s="59"/>
-      <c r="G28" s="73"/>
-      <c r="H28" s="73"/>
-      <c r="I28" s="73"/>
+      <c r="C28" s="88"/>
+      <c r="D28" s="161"/>
+      <c r="E28" s="88"/>
+      <c r="F28" s="58"/>
+      <c r="G28" s="170"/>
+      <c r="H28" s="70"/>
+      <c r="I28" s="70"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="109"/>
-      <c r="B29" s="63" t="s">
+      <c r="A29" s="106"/>
+      <c r="B29" s="61" t="s">
         <v>62</v>
       </c>
-      <c r="C29" s="92"/>
-      <c r="D29" s="56"/>
-      <c r="E29" s="92"/>
+      <c r="C29" s="126">
+        <v>42570</v>
+      </c>
+      <c r="D29" s="158">
+        <v>42570</v>
+      </c>
+      <c r="E29" s="86"/>
       <c r="F29" s="56"/>
-      <c r="G29" s="68"/>
-      <c r="H29" s="68"/>
-      <c r="I29" s="68"/>
+      <c r="G29" s="168"/>
+      <c r="H29" s="66"/>
+      <c r="I29" s="66"/>
     </row>
     <row r="30" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="110"/>
-      <c r="B30" s="80" t="s">
+      <c r="A30" s="107"/>
+      <c r="B30" s="76" t="s">
         <v>63</v>
       </c>
-      <c r="C30" s="93"/>
-      <c r="D30" s="57"/>
-      <c r="E30" s="93"/>
+      <c r="C30" s="133">
+        <v>42570</v>
+      </c>
+      <c r="D30" s="159">
+        <v>42570</v>
+      </c>
+      <c r="E30" s="87"/>
       <c r="F30" s="57"/>
-      <c r="G30" s="66"/>
-      <c r="H30" s="66"/>
-      <c r="I30" s="66"/>
+      <c r="G30" s="169"/>
+      <c r="H30" s="64"/>
+      <c r="I30" s="64"/>
     </row>
     <row r="31" spans="1:9" s="48" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="51"/>
@@ -2142,14 +2374,14 @@
       <c r="I31" s="52"/>
     </row>
     <row r="33" spans="2:9" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B33" s="98" t="s">
+      <c r="B33" s="89" t="s">
         <v>46</v>
       </c>
       <c r="C33" s="54"/>
       <c r="D33" s="54"/>
       <c r="E33" s="54"/>
       <c r="F33" s="54"/>
-      <c r="G33" s="98" t="s">
+      <c r="G33" s="89" t="s">
         <v>47</v>
       </c>
       <c r="H33" s="54"/>
@@ -2176,33 +2408,33 @@
       <c r="I35" s="54"/>
     </row>
     <row r="36" spans="2:9" s="48" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B36" s="100" t="s">
+      <c r="B36" s="91" t="s">
         <v>12</v>
       </c>
-      <c r="C36" s="115" t="s">
+      <c r="C36" s="94" t="s">
         <v>8</v>
       </c>
-      <c r="D36" s="115"/>
-      <c r="E36" s="115"/>
+      <c r="D36" s="94"/>
+      <c r="E36" s="94"/>
       <c r="F36" s="54"/>
       <c r="G36" s="53"/>
-      <c r="H36" s="101" t="s">
+      <c r="H36" s="92" t="s">
         <v>10</v>
       </c>
       <c r="I36" s="54"/>
     </row>
     <row r="37" spans="2:9" s="48" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B37" s="99" t="s">
+      <c r="B37" s="90" t="s">
         <v>52</v>
       </c>
-      <c r="C37" s="103" t="s">
+      <c r="C37" s="101" t="s">
         <v>61</v>
       </c>
-      <c r="D37" s="103"/>
-      <c r="E37" s="103"/>
+      <c r="D37" s="101"/>
+      <c r="E37" s="101"/>
       <c r="F37" s="54"/>
       <c r="G37" s="54"/>
-      <c r="H37" s="99" t="s">
+      <c r="H37" s="90" t="s">
         <v>18</v>
       </c>
       <c r="I37" s="54"/>
@@ -2228,28 +2460,28 @@
       <c r="I39" s="54"/>
     </row>
     <row r="40" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B40" s="100" t="s">
+      <c r="B40" s="91" t="s">
         <v>9</v>
       </c>
-      <c r="C40" s="115" t="s">
+      <c r="C40" s="94" t="s">
         <v>11</v>
       </c>
-      <c r="D40" s="115"/>
-      <c r="E40" s="115"/>
+      <c r="D40" s="94"/>
+      <c r="E40" s="94"/>
       <c r="F40" s="54"/>
       <c r="G40" s="54"/>
       <c r="H40" s="54"/>
       <c r="I40" s="54"/>
     </row>
     <row r="41" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B41" s="99" t="s">
+      <c r="B41" s="90" t="s">
         <v>20</v>
       </c>
-      <c r="C41" s="103" t="s">
+      <c r="C41" s="101" t="s">
         <v>20</v>
       </c>
-      <c r="D41" s="103"/>
-      <c r="E41" s="103"/>
+      <c r="D41" s="101"/>
+      <c r="E41" s="101"/>
       <c r="F41" s="54"/>
       <c r="G41" s="54"/>
       <c r="H41" s="54"/>
@@ -2297,6 +2529,14 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="C41:E41"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="I5:I6"/>
+    <mergeCell ref="A7:A20"/>
+    <mergeCell ref="A21:A24"/>
+    <mergeCell ref="A25:A27"/>
+    <mergeCell ref="A28:A30"/>
+    <mergeCell ref="C12:I12"/>
     <mergeCell ref="A1:I1"/>
     <mergeCell ref="C40:E40"/>
     <mergeCell ref="H5:H6"/>
@@ -2309,14 +2549,6 @@
     <mergeCell ref="C37:E37"/>
     <mergeCell ref="A2:I2"/>
     <mergeCell ref="A5:A6"/>
-    <mergeCell ref="C41:E41"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="I5:I6"/>
-    <mergeCell ref="A7:A20"/>
-    <mergeCell ref="A21:A24"/>
-    <mergeCell ref="A25:A27"/>
-    <mergeCell ref="A28:A30"/>
-    <mergeCell ref="C12:I12"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="1" bottom="1" header="0.3" footer="0.3"/>
   <pageSetup paperSize="5" orientation="landscape" r:id="rId1"/>
@@ -2359,7 +2591,7 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="124" t="s">
+      <c r="A2" s="114" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="16" t="s">
@@ -2372,14 +2604,14 @@
         <f>((C2/3)*100)</f>
         <v>33.333333333333329</v>
       </c>
-      <c r="E2" s="127">
+      <c r="E2" s="117">
         <f>(AVERAGE(C2:C4))*100</f>
         <v>66.666666666666657</v>
       </c>
       <c r="F2" s="4"/>
     </row>
     <row r="3" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="125"/>
+      <c r="A3" s="115"/>
       <c r="B3" s="7" t="s">
         <v>5</v>
       </c>
@@ -2390,11 +2622,11 @@
         <f t="shared" ref="D3:D4" si="0">((C3/3)*100)</f>
         <v>33.333333333333329</v>
       </c>
-      <c r="E3" s="128"/>
+      <c r="E3" s="118"/>
       <c r="F3" s="4"/>
     </row>
     <row r="4" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="126"/>
+      <c r="A4" s="116"/>
       <c r="B4" s="18" t="s">
         <v>6</v>
       </c>
@@ -2405,11 +2637,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E4" s="129"/>
+      <c r="E4" s="119"/>
       <c r="F4" s="4"/>
     </row>
     <row r="5" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="130" t="s">
+      <c r="A5" s="120" t="s">
         <v>7</v>
       </c>
       <c r="B5" s="27" t="s">
@@ -2420,14 +2652,14 @@
         <f>(AVERAGE(C6:C13)*100)*0.5</f>
         <v>0</v>
       </c>
-      <c r="E5" s="133">
+      <c r="E5" s="123">
         <f>D5+D14</f>
         <v>0</v>
       </c>
       <c r="F5" s="4"/>
     </row>
     <row r="6" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="131"/>
+      <c r="A6" s="121"/>
       <c r="B6" s="31" t="s">
         <v>30</v>
       </c>
@@ -2438,11 +2670,11 @@
         <f>(C6/8)*100</f>
         <v>0</v>
       </c>
-      <c r="E6" s="134"/>
+      <c r="E6" s="124"/>
       <c r="F6" s="4"/>
     </row>
     <row r="7" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="131"/>
+      <c r="A7" s="121"/>
       <c r="B7" s="31" t="s">
         <v>31</v>
       </c>
@@ -2453,11 +2685,11 @@
         <f t="shared" ref="D7:D13" si="1">(C7/8)*100</f>
         <v>0</v>
       </c>
-      <c r="E7" s="134"/>
+      <c r="E7" s="124"/>
       <c r="F7" s="4"/>
     </row>
     <row r="8" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="131"/>
+      <c r="A8" s="121"/>
       <c r="B8" s="31" t="s">
         <v>32</v>
       </c>
@@ -2468,11 +2700,11 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="E8" s="134"/>
+      <c r="E8" s="124"/>
       <c r="F8" s="4"/>
     </row>
     <row r="9" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="131"/>
+      <c r="A9" s="121"/>
       <c r="B9" s="31" t="s">
         <v>33</v>
       </c>
@@ -2483,11 +2715,11 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="E9" s="134"/>
+      <c r="E9" s="124"/>
       <c r="F9" s="4"/>
     </row>
     <row r="10" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="131"/>
+      <c r="A10" s="121"/>
       <c r="B10" s="31" t="s">
         <v>34</v>
       </c>
@@ -2498,11 +2730,11 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="E10" s="134"/>
+      <c r="E10" s="124"/>
       <c r="F10" s="4"/>
     </row>
     <row r="11" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="131"/>
+      <c r="A11" s="121"/>
       <c r="B11" s="31" t="s">
         <v>35</v>
       </c>
@@ -2513,11 +2745,11 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="E11" s="134"/>
+      <c r="E11" s="124"/>
       <c r="F11" s="4"/>
     </row>
     <row r="12" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="131"/>
+      <c r="A12" s="121"/>
       <c r="B12" s="31" t="s">
         <v>36</v>
       </c>
@@ -2528,11 +2760,11 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="E12" s="134"/>
+      <c r="E12" s="124"/>
       <c r="F12" s="4"/>
     </row>
     <row r="13" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="131"/>
+      <c r="A13" s="121"/>
       <c r="B13" s="31" t="s">
         <v>37</v>
       </c>
@@ -2543,11 +2775,11 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="E13" s="134"/>
+      <c r="E13" s="124"/>
       <c r="F13" s="4"/>
     </row>
     <row r="14" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="132"/>
+      <c r="A14" s="122"/>
       <c r="B14" s="29" t="s">
         <v>26</v>
       </c>
@@ -2558,7 +2790,7 @@
         <f>(C14/2)*100</f>
         <v>0</v>
       </c>
-      <c r="E14" s="135"/>
+      <c r="E14" s="125"/>
       <c r="F14" s="4"/>
     </row>
     <row r="15" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -2770,12 +3002,12 @@
       <c r="F40" s="4"/>
     </row>
     <row r="41" spans="1:6" ht="24" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="121" t="s">
+      <c r="A41" s="111" t="s">
         <v>27</v>
       </c>
-      <c r="B41" s="122"/>
-      <c r="C41" s="122"/>
-      <c r="D41" s="123"/>
+      <c r="B41" s="112"/>
+      <c r="C41" s="112"/>
+      <c r="D41" s="113"/>
       <c r="E41" s="47">
         <f>(AVERAGE(E2,E5))</f>
         <v>33.333333333333329</v>

</xml_diff>

<commit_message>
Edited workplan - Day 3
</commit_message>
<xml_diff>
--- a/Workplan.xlsx
+++ b/Workplan.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="68">
   <si>
     <t>ACTIVITIES</t>
   </si>
@@ -300,9 +300,6 @@
   </si>
   <si>
     <t>Environment Setup (Cloud Formation)</t>
-  </si>
-  <si>
-    <t>In Progress</t>
   </si>
   <si>
     <t>Second actual commit will be done on the presentation day</t>
@@ -1005,7 +1002,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="173">
+  <cellXfs count="176">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1247,103 +1244,10 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="3" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="3" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="3" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="5" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -1359,9 +1263,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -1369,7 +1270,6 @@
       <alignment horizontal="left" indent="2"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1408,12 +1308,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1430,12 +1324,6 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="8" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1457,6 +1345,122 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="3" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="3" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="3" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="5" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1761,7 +1765,7 @@
   <dimension ref="A1:I45"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1778,30 +1782,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="48" customFormat="1" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="93" t="s">
+      <c r="A1" s="148" t="s">
         <v>64</v>
       </c>
-      <c r="B1" s="93"/>
-      <c r="C1" s="93"/>
-      <c r="D1" s="93"/>
-      <c r="E1" s="93"/>
-      <c r="F1" s="93"/>
-      <c r="G1" s="93"/>
-      <c r="H1" s="93"/>
-      <c r="I1" s="93"/>
+      <c r="B1" s="148"/>
+      <c r="C1" s="148"/>
+      <c r="D1" s="148"/>
+      <c r="E1" s="148"/>
+      <c r="F1" s="148"/>
+      <c r="G1" s="148"/>
+      <c r="H1" s="148"/>
+      <c r="I1" s="148"/>
     </row>
     <row r="2" spans="1:9" s="48" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A2" s="102" t="s">
+      <c r="A2" s="158" t="s">
         <v>45</v>
       </c>
-      <c r="B2" s="102"/>
-      <c r="C2" s="102"/>
-      <c r="D2" s="102"/>
-      <c r="E2" s="102"/>
-      <c r="F2" s="102"/>
-      <c r="G2" s="102"/>
-      <c r="H2" s="102"/>
-      <c r="I2" s="102"/>
+      <c r="B2" s="158"/>
+      <c r="C2" s="158"/>
+      <c r="D2" s="158"/>
+      <c r="E2" s="158"/>
+      <c r="F2" s="158"/>
+      <c r="G2" s="158"/>
+      <c r="H2" s="158"/>
+      <c r="I2" s="158"/>
     </row>
     <row r="3" spans="1:9" s="48" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="49"/>
@@ -1815,78 +1819,78 @@
     </row>
     <row r="4" spans="1:9" s="48" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="103" t="s">
+      <c r="A5" s="137" t="s">
         <v>49</v>
       </c>
-      <c r="B5" s="103" t="s">
+      <c r="B5" s="137" t="s">
         <v>38</v>
       </c>
-      <c r="C5" s="99" t="s">
+      <c r="C5" s="154" t="s">
         <v>40</v>
       </c>
-      <c r="D5" s="152" t="s">
+      <c r="D5" s="156" t="s">
         <v>41</v>
       </c>
-      <c r="E5" s="99" t="s">
+      <c r="E5" s="154" t="s">
         <v>42</v>
       </c>
-      <c r="F5" s="97" t="s">
+      <c r="F5" s="152" t="s">
         <v>43</v>
       </c>
-      <c r="G5" s="162" t="s">
+      <c r="G5" s="150" t="s">
         <v>60</v>
       </c>
-      <c r="H5" s="95" t="s">
+      <c r="H5" s="139" t="s">
         <v>44</v>
       </c>
-      <c r="I5" s="95" t="s">
+      <c r="I5" s="139" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="104"/>
-      <c r="B6" s="104"/>
-      <c r="C6" s="100"/>
-      <c r="D6" s="153"/>
-      <c r="E6" s="100"/>
-      <c r="F6" s="98"/>
-      <c r="G6" s="163"/>
-      <c r="H6" s="96"/>
-      <c r="I6" s="96"/>
+      <c r="A6" s="138"/>
+      <c r="B6" s="138"/>
+      <c r="C6" s="155"/>
+      <c r="D6" s="157"/>
+      <c r="E6" s="155"/>
+      <c r="F6" s="153"/>
+      <c r="G6" s="151"/>
+      <c r="H6" s="140"/>
+      <c r="I6" s="140"/>
     </row>
     <row r="7" spans="1:9" s="48" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="105">
+      <c r="A7" s="141">
         <v>1</v>
       </c>
       <c r="B7" s="59" t="s">
         <v>4</v>
       </c>
       <c r="C7" s="78"/>
-      <c r="D7" s="154"/>
-      <c r="E7" s="141"/>
-      <c r="F7" s="142"/>
-      <c r="G7" s="164"/>
+      <c r="D7" s="119"/>
+      <c r="E7" s="108"/>
+      <c r="F7" s="109"/>
+      <c r="G7" s="127"/>
       <c r="H7" s="67"/>
       <c r="I7" s="67"/>
     </row>
     <row r="8" spans="1:9" ht="75" x14ac:dyDescent="0.25">
-      <c r="A8" s="106"/>
+      <c r="A8" s="142"/>
       <c r="B8" s="60" t="s">
         <v>3</v>
       </c>
       <c r="C8" s="79">
         <v>42565</v>
       </c>
-      <c r="D8" s="150">
-        <v>42565</v>
-      </c>
-      <c r="E8" s="145">
-        <v>42565</v>
-      </c>
-      <c r="F8" s="146">
-        <v>42565</v>
-      </c>
-      <c r="G8" s="151">
+      <c r="D8" s="117">
+        <v>42565</v>
+      </c>
+      <c r="E8" s="112">
+        <v>42565</v>
+      </c>
+      <c r="F8" s="113">
+        <v>42565</v>
+      </c>
+      <c r="G8" s="118">
         <v>100</v>
       </c>
       <c r="H8" s="74" t="s">
@@ -1897,14 +1901,14 @@
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="106"/>
+      <c r="A9" s="142"/>
       <c r="B9" s="61" t="s">
         <v>5</v>
       </c>
       <c r="C9" s="79">
         <v>42565</v>
       </c>
-      <c r="D9" s="150">
+      <c r="D9" s="117">
         <v>42565</v>
       </c>
       <c r="E9" s="79">
@@ -1913,7 +1917,7 @@
       <c r="F9" s="80">
         <v>42565</v>
       </c>
-      <c r="G9" s="151">
+      <c r="G9" s="118">
         <v>100</v>
       </c>
       <c r="H9" s="74" t="s">
@@ -1922,14 +1926,14 @@
       <c r="I9" s="66"/>
     </row>
     <row r="10" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="106"/>
+      <c r="A10" s="142"/>
       <c r="B10" s="61" t="s">
         <v>6</v>
       </c>
       <c r="C10" s="79">
         <v>42565</v>
       </c>
-      <c r="D10" s="150">
+      <c r="D10" s="117">
         <v>42565</v>
       </c>
       <c r="E10" s="82">
@@ -1938,7 +1942,7 @@
       <c r="F10" s="83">
         <v>42565</v>
       </c>
-      <c r="G10" s="151">
+      <c r="G10" s="118">
         <v>100</v>
       </c>
       <c r="H10" s="74" t="s">
@@ -1947,42 +1951,42 @@
       <c r="I10" s="66"/>
     </row>
     <row r="11" spans="1:9" s="50" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="106"/>
+      <c r="A11" s="142"/>
       <c r="B11" s="62" t="s">
         <v>66</v>
       </c>
       <c r="C11" s="81"/>
-      <c r="D11" s="155"/>
-      <c r="E11" s="143">
-        <v>42565</v>
-      </c>
-      <c r="F11" s="144"/>
-      <c r="G11" s="165"/>
+      <c r="D11" s="120"/>
+      <c r="E11" s="110">
+        <v>42565</v>
+      </c>
+      <c r="F11" s="111"/>
+      <c r="G11" s="128"/>
       <c r="H11" s="75"/>
       <c r="I11" s="69"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="106"/>
+      <c r="A12" s="142"/>
       <c r="B12" s="61" t="s">
         <v>29</v>
       </c>
-      <c r="C12" s="108"/>
-      <c r="D12" s="109"/>
-      <c r="E12" s="109"/>
-      <c r="F12" s="109"/>
-      <c r="G12" s="109"/>
-      <c r="H12" s="109"/>
-      <c r="I12" s="110"/>
+      <c r="C12" s="145"/>
+      <c r="D12" s="146"/>
+      <c r="E12" s="146"/>
+      <c r="F12" s="146"/>
+      <c r="G12" s="146"/>
+      <c r="H12" s="146"/>
+      <c r="I12" s="147"/>
     </row>
     <row r="13" spans="1:9" s="48" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="106"/>
+      <c r="A13" s="142"/>
       <c r="B13" s="77" t="s">
         <v>30</v>
       </c>
       <c r="C13" s="79">
         <v>42565</v>
       </c>
-      <c r="D13" s="150">
+      <c r="D13" s="117">
         <v>42565</v>
       </c>
       <c r="E13" s="79">
@@ -1991,7 +1995,7 @@
       <c r="F13" s="80">
         <v>42565</v>
       </c>
-      <c r="G13" s="151">
+      <c r="G13" s="118">
         <v>100</v>
       </c>
       <c r="H13" s="74" t="s">
@@ -2000,14 +2004,14 @@
       <c r="I13" s="66"/>
     </row>
     <row r="14" spans="1:9" s="48" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="106"/>
+      <c r="A14" s="142"/>
       <c r="B14" s="77" t="s">
         <v>31</v>
       </c>
       <c r="C14" s="79">
         <v>42565</v>
       </c>
-      <c r="D14" s="150">
+      <c r="D14" s="117">
         <v>42565</v>
       </c>
       <c r="E14" s="79">
@@ -2016,7 +2020,7 @@
       <c r="F14" s="80">
         <v>42565</v>
       </c>
-      <c r="G14" s="151">
+      <c r="G14" s="118">
         <v>100</v>
       </c>
       <c r="H14" s="74" t="s">
@@ -2025,14 +2029,14 @@
       <c r="I14" s="66"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="106"/>
+      <c r="A15" s="142"/>
       <c r="B15" s="77" t="s">
         <v>35</v>
       </c>
       <c r="C15" s="79">
         <v>42565</v>
       </c>
-      <c r="D15" s="150">
+      <c r="D15" s="117">
         <v>42565</v>
       </c>
       <c r="E15" s="79">
@@ -2041,7 +2045,7 @@
       <c r="F15" s="80">
         <v>42565</v>
       </c>
-      <c r="G15" s="151">
+      <c r="G15" s="118">
         <v>100</v>
       </c>
       <c r="H15" s="74" t="s">
@@ -2050,14 +2054,14 @@
       <c r="I15" s="66"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="106"/>
+      <c r="A16" s="142"/>
       <c r="B16" s="77" t="s">
         <v>36</v>
       </c>
       <c r="C16" s="79">
         <v>42565</v>
       </c>
-      <c r="D16" s="150">
+      <c r="D16" s="117">
         <v>42565</v>
       </c>
       <c r="E16" s="79">
@@ -2066,7 +2070,7 @@
       <c r="F16" s="80">
         <v>42565</v>
       </c>
-      <c r="G16" s="151">
+      <c r="G16" s="118">
         <v>100</v>
       </c>
       <c r="H16" s="74" t="s">
@@ -2075,14 +2079,14 @@
       <c r="I16" s="66"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="106"/>
+      <c r="A17" s="142"/>
       <c r="B17" s="77" t="s">
         <v>37</v>
       </c>
       <c r="C17" s="79">
         <v>42565</v>
       </c>
-      <c r="D17" s="150">
+      <c r="D17" s="117">
         <v>42565</v>
       </c>
       <c r="E17" s="79">
@@ -2091,7 +2095,7 @@
       <c r="F17" s="80">
         <v>42565</v>
       </c>
-      <c r="G17" s="151">
+      <c r="G17" s="118">
         <v>100</v>
       </c>
       <c r="H17" s="74" t="s">
@@ -2100,14 +2104,14 @@
       <c r="I17" s="66"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="106"/>
+      <c r="A18" s="142"/>
       <c r="B18" s="61" t="s">
         <v>26</v>
       </c>
       <c r="C18" s="79">
         <v>42565</v>
       </c>
-      <c r="D18" s="150">
+      <c r="D18" s="117">
         <v>42565</v>
       </c>
       <c r="E18" s="79">
@@ -2116,7 +2120,7 @@
       <c r="F18" s="80">
         <v>42565</v>
       </c>
-      <c r="G18" s="151">
+      <c r="G18" s="118">
         <v>100</v>
       </c>
       <c r="H18" s="74" t="s">
@@ -2125,240 +2129,250 @@
       <c r="I18" s="66"/>
     </row>
     <row r="19" spans="1:9" s="50" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="106"/>
+      <c r="A19" s="142"/>
       <c r="B19" s="63" t="s">
         <v>50</v>
       </c>
       <c r="C19" s="81"/>
-      <c r="D19" s="155"/>
-      <c r="E19" s="147"/>
-      <c r="F19" s="148"/>
-      <c r="G19" s="165"/>
+      <c r="D19" s="120"/>
+      <c r="E19" s="114"/>
+      <c r="F19" s="115"/>
+      <c r="G19" s="128"/>
       <c r="H19" s="71"/>
       <c r="I19" s="69"/>
     </row>
     <row r="20" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="107"/>
-      <c r="B20" s="128" t="s">
+      <c r="A20" s="143"/>
+      <c r="B20" s="97" t="s">
         <v>51</v>
       </c>
       <c r="C20" s="82">
         <v>42565</v>
       </c>
-      <c r="D20" s="156">
+      <c r="D20" s="121">
         <v>42573</v>
       </c>
-      <c r="E20" s="149">
+      <c r="E20" s="116">
         <v>42565</v>
       </c>
       <c r="F20" s="83">
         <v>42566</v>
       </c>
-      <c r="G20" s="166">
+      <c r="G20" s="129">
         <v>100</v>
       </c>
       <c r="H20" s="72" t="s">
         <v>48</v>
       </c>
-      <c r="I20" s="127" t="s">
-        <v>68</v>
+      <c r="I20" s="96" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="105">
+      <c r="A21" s="141">
         <v>2</v>
       </c>
       <c r="B21" s="65" t="s">
         <v>52</v>
       </c>
       <c r="C21" s="84"/>
-      <c r="D21" s="157"/>
+      <c r="D21" s="122"/>
       <c r="E21" s="84"/>
       <c r="F21" s="85"/>
-      <c r="G21" s="167"/>
+      <c r="G21" s="130"/>
       <c r="H21" s="73"/>
       <c r="I21" s="70"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="106"/>
+      <c r="A22" s="142"/>
       <c r="B22" s="61" t="s">
         <v>53</v>
       </c>
-      <c r="C22" s="134">
+      <c r="C22" s="102">
         <v>42566</v>
       </c>
-      <c r="D22" s="158">
+      <c r="D22" s="123">
         <v>42566</v>
       </c>
-      <c r="E22" s="126">
+      <c r="E22" s="95">
         <v>42566</v>
       </c>
-      <c r="F22" s="129">
+      <c r="F22" s="98">
         <v>42566</v>
       </c>
-      <c r="G22" s="140">
+      <c r="G22" s="107">
         <v>100</v>
       </c>
-      <c r="H22" s="130" t="s">
+      <c r="H22" s="99" t="s">
         <v>48</v>
       </c>
       <c r="I22" s="66"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="106"/>
+      <c r="A23" s="142"/>
       <c r="B23" s="61" t="s">
         <v>54</v>
       </c>
-      <c r="C23" s="134">
+      <c r="C23" s="102">
         <v>42566</v>
       </c>
-      <c r="D23" s="158">
+      <c r="D23" s="123">
         <v>42566</v>
       </c>
-      <c r="E23" s="126">
+      <c r="E23" s="95">
         <v>42566</v>
       </c>
-      <c r="F23" s="129">
+      <c r="F23" s="98">
         <v>42566</v>
       </c>
-      <c r="G23" s="140">
+      <c r="G23" s="107">
         <v>100</v>
       </c>
-      <c r="H23" s="130" t="s">
+      <c r="H23" s="99" t="s">
         <v>48</v>
       </c>
       <c r="I23" s="66"/>
     </row>
     <row r="24" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="107"/>
+      <c r="A24" s="143"/>
       <c r="B24" s="76" t="s">
         <v>55</v>
       </c>
-      <c r="C24" s="139">
+      <c r="C24" s="106">
         <v>42566</v>
       </c>
-      <c r="D24" s="159">
+      <c r="D24" s="124">
         <v>42566</v>
       </c>
-      <c r="E24" s="126">
+      <c r="E24" s="95">
         <v>42566</v>
       </c>
-      <c r="F24" s="129">
+      <c r="F24" s="98">
         <v>42566</v>
       </c>
-      <c r="G24" s="140">
+      <c r="G24" s="107">
         <v>100</v>
       </c>
-      <c r="H24" s="131" t="s">
+      <c r="H24" s="100" t="s">
         <v>48</v>
       </c>
       <c r="I24" s="64"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" s="132">
+      <c r="A25" s="144">
         <v>3</v>
       </c>
-      <c r="B25" s="135" t="s">
+      <c r="B25" s="103" t="s">
         <v>56</v>
       </c>
-      <c r="C25" s="136">
+      <c r="C25" s="104">
         <v>42569</v>
       </c>
-      <c r="D25" s="160">
+      <c r="D25" s="125">
         <v>42569</v>
       </c>
-      <c r="E25" s="126">
+      <c r="E25" s="95">
         <v>42566</v>
       </c>
-      <c r="F25" s="137"/>
-      <c r="G25" s="171">
-        <v>10</v>
-      </c>
-      <c r="H25" s="172" t="s">
-        <v>67</v>
-      </c>
-      <c r="I25" s="138"/>
+      <c r="F25" s="174">
+        <v>42569</v>
+      </c>
+      <c r="G25" s="134">
+        <v>100</v>
+      </c>
+      <c r="H25" s="135" t="s">
+        <v>48</v>
+      </c>
+      <c r="I25" s="105"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" s="106"/>
+      <c r="A26" s="142"/>
       <c r="B26" s="61" t="s">
         <v>57</v>
       </c>
-      <c r="C26" s="126">
+      <c r="C26" s="95">
         <v>42569</v>
       </c>
-      <c r="D26" s="158">
+      <c r="D26" s="123">
         <v>42569</v>
       </c>
-      <c r="E26" s="86"/>
-      <c r="F26" s="56"/>
-      <c r="G26" s="168"/>
-      <c r="H26" s="66"/>
+      <c r="E26" s="95">
+        <v>42569</v>
+      </c>
+      <c r="F26" s="98">
+        <v>42569</v>
+      </c>
+      <c r="G26" s="118">
+        <v>100</v>
+      </c>
+      <c r="H26" s="93" t="s">
+        <v>48</v>
+      </c>
       <c r="I26" s="66"/>
     </row>
     <row r="27" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="107"/>
+      <c r="A27" s="143"/>
       <c r="B27" s="76" t="s">
         <v>58</v>
       </c>
-      <c r="C27" s="133">
+      <c r="C27" s="101">
         <v>42569</v>
       </c>
-      <c r="D27" s="159">
+      <c r="D27" s="124">
         <v>42569</v>
       </c>
-      <c r="E27" s="87"/>
-      <c r="F27" s="57"/>
-      <c r="G27" s="169"/>
-      <c r="H27" s="64"/>
+      <c r="E27" s="101"/>
+      <c r="F27" s="175"/>
+      <c r="G27" s="129"/>
+      <c r="H27" s="94"/>
       <c r="I27" s="64"/>
     </row>
     <row r="28" spans="1:9" s="48" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A28" s="105">
+      <c r="A28" s="141">
         <v>4</v>
       </c>
       <c r="B28" s="65" t="s">
         <v>59</v>
       </c>
       <c r="C28" s="88"/>
-      <c r="D28" s="161"/>
+      <c r="D28" s="126"/>
       <c r="E28" s="88"/>
       <c r="F28" s="58"/>
-      <c r="G28" s="170"/>
+      <c r="G28" s="133"/>
       <c r="H28" s="70"/>
       <c r="I28" s="70"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="106"/>
+      <c r="A29" s="142"/>
       <c r="B29" s="61" t="s">
         <v>62</v>
       </c>
-      <c r="C29" s="126">
+      <c r="C29" s="95">
         <v>42570</v>
       </c>
-      <c r="D29" s="158">
+      <c r="D29" s="123">
         <v>42570</v>
       </c>
       <c r="E29" s="86"/>
       <c r="F29" s="56"/>
-      <c r="G29" s="168"/>
+      <c r="G29" s="131"/>
       <c r="H29" s="66"/>
       <c r="I29" s="66"/>
     </row>
     <row r="30" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="107"/>
+      <c r="A30" s="143"/>
       <c r="B30" s="76" t="s">
         <v>63</v>
       </c>
-      <c r="C30" s="133">
+      <c r="C30" s="101">
         <v>42570</v>
       </c>
-      <c r="D30" s="159">
+      <c r="D30" s="124">
         <v>42570</v>
       </c>
       <c r="E30" s="87"/>
       <c r="F30" s="57"/>
-      <c r="G30" s="169"/>
+      <c r="G30" s="132"/>
       <c r="H30" s="64"/>
       <c r="I30" s="64"/>
     </row>
@@ -2411,11 +2425,11 @@
       <c r="B36" s="91" t="s">
         <v>12</v>
       </c>
-      <c r="C36" s="94" t="s">
+      <c r="C36" s="149" t="s">
         <v>8</v>
       </c>
-      <c r="D36" s="94"/>
-      <c r="E36" s="94"/>
+      <c r="D36" s="149"/>
+      <c r="E36" s="149"/>
       <c r="F36" s="54"/>
       <c r="G36" s="53"/>
       <c r="H36" s="92" t="s">
@@ -2427,11 +2441,11 @@
       <c r="B37" s="90" t="s">
         <v>52</v>
       </c>
-      <c r="C37" s="101" t="s">
+      <c r="C37" s="136" t="s">
         <v>61</v>
       </c>
-      <c r="D37" s="101"/>
-      <c r="E37" s="101"/>
+      <c r="D37" s="136"/>
+      <c r="E37" s="136"/>
       <c r="F37" s="54"/>
       <c r="G37" s="54"/>
       <c r="H37" s="90" t="s">
@@ -2463,11 +2477,11 @@
       <c r="B40" s="91" t="s">
         <v>9</v>
       </c>
-      <c r="C40" s="94" t="s">
+      <c r="C40" s="149" t="s">
         <v>11</v>
       </c>
-      <c r="D40" s="94"/>
-      <c r="E40" s="94"/>
+      <c r="D40" s="149"/>
+      <c r="E40" s="149"/>
       <c r="F40" s="54"/>
       <c r="G40" s="54"/>
       <c r="H40" s="54"/>
@@ -2477,11 +2491,11 @@
       <c r="B41" s="90" t="s">
         <v>20</v>
       </c>
-      <c r="C41" s="101" t="s">
+      <c r="C41" s="136" t="s">
         <v>20</v>
       </c>
-      <c r="D41" s="101"/>
-      <c r="E41" s="101"/>
+      <c r="D41" s="136"/>
+      <c r="E41" s="136"/>
       <c r="F41" s="54"/>
       <c r="G41" s="54"/>
       <c r="H41" s="54"/>
@@ -2529,14 +2543,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="C41:E41"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="I5:I6"/>
-    <mergeCell ref="A7:A20"/>
-    <mergeCell ref="A21:A24"/>
-    <mergeCell ref="A25:A27"/>
-    <mergeCell ref="A28:A30"/>
-    <mergeCell ref="C12:I12"/>
     <mergeCell ref="A1:I1"/>
     <mergeCell ref="C40:E40"/>
     <mergeCell ref="H5:H6"/>
@@ -2549,6 +2555,14 @@
     <mergeCell ref="C37:E37"/>
     <mergeCell ref="A2:I2"/>
     <mergeCell ref="A5:A6"/>
+    <mergeCell ref="C41:E41"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="I5:I6"/>
+    <mergeCell ref="A7:A20"/>
+    <mergeCell ref="A21:A24"/>
+    <mergeCell ref="A25:A27"/>
+    <mergeCell ref="A28:A30"/>
+    <mergeCell ref="C12:I12"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="1" bottom="1" header="0.3" footer="0.3"/>
   <pageSetup paperSize="5" orientation="landscape" r:id="rId1"/>
@@ -2591,7 +2605,7 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="114" t="s">
+      <c r="A2" s="162" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="16" t="s">
@@ -2604,14 +2618,14 @@
         <f>((C2/3)*100)</f>
         <v>33.333333333333329</v>
       </c>
-      <c r="E2" s="117">
+      <c r="E2" s="165">
         <f>(AVERAGE(C2:C4))*100</f>
         <v>66.666666666666657</v>
       </c>
       <c r="F2" s="4"/>
     </row>
     <row r="3" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="115"/>
+      <c r="A3" s="163"/>
       <c r="B3" s="7" t="s">
         <v>5</v>
       </c>
@@ -2622,11 +2636,11 @@
         <f t="shared" ref="D3:D4" si="0">((C3/3)*100)</f>
         <v>33.333333333333329</v>
       </c>
-      <c r="E3" s="118"/>
+      <c r="E3" s="166"/>
       <c r="F3" s="4"/>
     </row>
     <row r="4" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="116"/>
+      <c r="A4" s="164"/>
       <c r="B4" s="18" t="s">
         <v>6</v>
       </c>
@@ -2637,11 +2651,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E4" s="119"/>
+      <c r="E4" s="167"/>
       <c r="F4" s="4"/>
     </row>
     <row r="5" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="120" t="s">
+      <c r="A5" s="168" t="s">
         <v>7</v>
       </c>
       <c r="B5" s="27" t="s">
@@ -2652,14 +2666,14 @@
         <f>(AVERAGE(C6:C13)*100)*0.5</f>
         <v>0</v>
       </c>
-      <c r="E5" s="123">
+      <c r="E5" s="171">
         <f>D5+D14</f>
         <v>0</v>
       </c>
       <c r="F5" s="4"/>
     </row>
     <row r="6" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="121"/>
+      <c r="A6" s="169"/>
       <c r="B6" s="31" t="s">
         <v>30</v>
       </c>
@@ -2670,11 +2684,11 @@
         <f>(C6/8)*100</f>
         <v>0</v>
       </c>
-      <c r="E6" s="124"/>
+      <c r="E6" s="172"/>
       <c r="F6" s="4"/>
     </row>
     <row r="7" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="121"/>
+      <c r="A7" s="169"/>
       <c r="B7" s="31" t="s">
         <v>31</v>
       </c>
@@ -2685,11 +2699,11 @@
         <f t="shared" ref="D7:D13" si="1">(C7/8)*100</f>
         <v>0</v>
       </c>
-      <c r="E7" s="124"/>
+      <c r="E7" s="172"/>
       <c r="F7" s="4"/>
     </row>
     <row r="8" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="121"/>
+      <c r="A8" s="169"/>
       <c r="B8" s="31" t="s">
         <v>32</v>
       </c>
@@ -2700,11 +2714,11 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="E8" s="124"/>
+      <c r="E8" s="172"/>
       <c r="F8" s="4"/>
     </row>
     <row r="9" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="121"/>
+      <c r="A9" s="169"/>
       <c r="B9" s="31" t="s">
         <v>33</v>
       </c>
@@ -2715,11 +2729,11 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="E9" s="124"/>
+      <c r="E9" s="172"/>
       <c r="F9" s="4"/>
     </row>
     <row r="10" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="121"/>
+      <c r="A10" s="169"/>
       <c r="B10" s="31" t="s">
         <v>34</v>
       </c>
@@ -2730,11 +2744,11 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="E10" s="124"/>
+      <c r="E10" s="172"/>
       <c r="F10" s="4"/>
     </row>
     <row r="11" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="121"/>
+      <c r="A11" s="169"/>
       <c r="B11" s="31" t="s">
         <v>35</v>
       </c>
@@ -2745,11 +2759,11 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="E11" s="124"/>
+      <c r="E11" s="172"/>
       <c r="F11" s="4"/>
     </row>
     <row r="12" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="121"/>
+      <c r="A12" s="169"/>
       <c r="B12" s="31" t="s">
         <v>36</v>
       </c>
@@ -2760,11 +2774,11 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="E12" s="124"/>
+      <c r="E12" s="172"/>
       <c r="F12" s="4"/>
     </row>
     <row r="13" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="121"/>
+      <c r="A13" s="169"/>
       <c r="B13" s="31" t="s">
         <v>37</v>
       </c>
@@ -2775,11 +2789,11 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="E13" s="124"/>
+      <c r="E13" s="172"/>
       <c r="F13" s="4"/>
     </row>
     <row r="14" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="122"/>
+      <c r="A14" s="170"/>
       <c r="B14" s="29" t="s">
         <v>26</v>
       </c>
@@ -2790,7 +2804,7 @@
         <f>(C14/2)*100</f>
         <v>0</v>
       </c>
-      <c r="E14" s="125"/>
+      <c r="E14" s="173"/>
       <c r="F14" s="4"/>
     </row>
     <row r="15" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -3002,12 +3016,12 @@
       <c r="F40" s="4"/>
     </row>
     <row r="41" spans="1:6" ht="24" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="111" t="s">
+      <c r="A41" s="159" t="s">
         <v>27</v>
       </c>
-      <c r="B41" s="112"/>
-      <c r="C41" s="112"/>
-      <c r="D41" s="113"/>
+      <c r="B41" s="160"/>
+      <c r="C41" s="160"/>
+      <c r="D41" s="161"/>
       <c r="E41" s="47">
         <f>(AVERAGE(E2,E5))</f>
         <v>33.333333333333329</v>

</xml_diff>

<commit_message>
Edited Workplan - Day 4
</commit_message>
<xml_diff>
--- a/Workplan.xlsx
+++ b/Workplan.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="69">
   <si>
     <t>ACTIVITIES</t>
   </si>
@@ -303,6 +303,9 @@
   </si>
   <si>
     <t>Second actual commit will be done on the presentation day</t>
+  </si>
+  <si>
+    <t>In Progress</t>
   </si>
 </sst>
 </file>
@@ -1002,7 +1005,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="176">
+  <cellXfs count="172">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1231,8 +1234,6 @@
     <xf numFmtId="0" fontId="5" fillId="8" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1243,12 +1244,6 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1336,8 +1331,6 @@
     <xf numFmtId="0" fontId="5" fillId="8" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="8" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1345,6 +1338,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -1459,8 +1460,6 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1764,8 +1763,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1782,30 +1781,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="48" customFormat="1" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="148" t="s">
+      <c r="A1" s="146" t="s">
         <v>64</v>
       </c>
-      <c r="B1" s="148"/>
-      <c r="C1" s="148"/>
-      <c r="D1" s="148"/>
-      <c r="E1" s="148"/>
-      <c r="F1" s="148"/>
-      <c r="G1" s="148"/>
-      <c r="H1" s="148"/>
-      <c r="I1" s="148"/>
+      <c r="B1" s="146"/>
+      <c r="C1" s="146"/>
+      <c r="D1" s="146"/>
+      <c r="E1" s="146"/>
+      <c r="F1" s="146"/>
+      <c r="G1" s="146"/>
+      <c r="H1" s="146"/>
+      <c r="I1" s="146"/>
     </row>
     <row r="2" spans="1:9" s="48" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A2" s="158" t="s">
+      <c r="A2" s="156" t="s">
         <v>45</v>
       </c>
-      <c r="B2" s="158"/>
-      <c r="C2" s="158"/>
-      <c r="D2" s="158"/>
-      <c r="E2" s="158"/>
-      <c r="F2" s="158"/>
-      <c r="G2" s="158"/>
-      <c r="H2" s="158"/>
-      <c r="I2" s="158"/>
+      <c r="B2" s="156"/>
+      <c r="C2" s="156"/>
+      <c r="D2" s="156"/>
+      <c r="E2" s="156"/>
+      <c r="F2" s="156"/>
+      <c r="G2" s="156"/>
+      <c r="H2" s="156"/>
+      <c r="I2" s="156"/>
     </row>
     <row r="3" spans="1:9" s="48" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="49"/>
@@ -1819,78 +1818,78 @@
     </row>
     <row r="4" spans="1:9" s="48" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="137" t="s">
+      <c r="A5" s="135" t="s">
         <v>49</v>
       </c>
-      <c r="B5" s="137" t="s">
+      <c r="B5" s="135" t="s">
         <v>38</v>
       </c>
-      <c r="C5" s="154" t="s">
+      <c r="C5" s="152" t="s">
         <v>40</v>
       </c>
-      <c r="D5" s="156" t="s">
+      <c r="D5" s="154" t="s">
         <v>41</v>
       </c>
-      <c r="E5" s="154" t="s">
+      <c r="E5" s="152" t="s">
         <v>42</v>
       </c>
-      <c r="F5" s="152" t="s">
+      <c r="F5" s="150" t="s">
         <v>43</v>
       </c>
-      <c r="G5" s="150" t="s">
+      <c r="G5" s="148" t="s">
         <v>60</v>
       </c>
-      <c r="H5" s="139" t="s">
+      <c r="H5" s="137" t="s">
         <v>44</v>
       </c>
-      <c r="I5" s="139" t="s">
+      <c r="I5" s="137" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="138"/>
-      <c r="B6" s="138"/>
-      <c r="C6" s="155"/>
-      <c r="D6" s="157"/>
-      <c r="E6" s="155"/>
-      <c r="F6" s="153"/>
-      <c r="G6" s="151"/>
-      <c r="H6" s="140"/>
-      <c r="I6" s="140"/>
+      <c r="A6" s="136"/>
+      <c r="B6" s="136"/>
+      <c r="C6" s="153"/>
+      <c r="D6" s="155"/>
+      <c r="E6" s="153"/>
+      <c r="F6" s="151"/>
+      <c r="G6" s="149"/>
+      <c r="H6" s="138"/>
+      <c r="I6" s="138"/>
     </row>
     <row r="7" spans="1:9" s="48" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="141">
+      <c r="A7" s="139">
         <v>1</v>
       </c>
       <c r="B7" s="59" t="s">
         <v>4</v>
       </c>
       <c r="C7" s="78"/>
-      <c r="D7" s="119"/>
-      <c r="E7" s="108"/>
-      <c r="F7" s="109"/>
-      <c r="G7" s="127"/>
+      <c r="D7" s="115"/>
+      <c r="E7" s="104"/>
+      <c r="F7" s="105"/>
+      <c r="G7" s="123"/>
       <c r="H7" s="67"/>
       <c r="I7" s="67"/>
     </row>
     <row r="8" spans="1:9" ht="75" x14ac:dyDescent="0.25">
-      <c r="A8" s="142"/>
+      <c r="A8" s="140"/>
       <c r="B8" s="60" t="s">
         <v>3</v>
       </c>
       <c r="C8" s="79">
         <v>42565</v>
       </c>
-      <c r="D8" s="117">
-        <v>42565</v>
-      </c>
-      <c r="E8" s="112">
-        <v>42565</v>
-      </c>
-      <c r="F8" s="113">
-        <v>42565</v>
-      </c>
-      <c r="G8" s="118">
+      <c r="D8" s="113">
+        <v>42565</v>
+      </c>
+      <c r="E8" s="108">
+        <v>42565</v>
+      </c>
+      <c r="F8" s="109">
+        <v>42565</v>
+      </c>
+      <c r="G8" s="114">
         <v>100</v>
       </c>
       <c r="H8" s="74" t="s">
@@ -1901,14 +1900,14 @@
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="142"/>
+      <c r="A9" s="140"/>
       <c r="B9" s="61" t="s">
         <v>5</v>
       </c>
       <c r="C9" s="79">
         <v>42565</v>
       </c>
-      <c r="D9" s="117">
+      <c r="D9" s="113">
         <v>42565</v>
       </c>
       <c r="E9" s="79">
@@ -1917,7 +1916,7 @@
       <c r="F9" s="80">
         <v>42565</v>
       </c>
-      <c r="G9" s="118">
+      <c r="G9" s="114">
         <v>100</v>
       </c>
       <c r="H9" s="74" t="s">
@@ -1926,14 +1925,14 @@
       <c r="I9" s="66"/>
     </row>
     <row r="10" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="142"/>
+      <c r="A10" s="140"/>
       <c r="B10" s="61" t="s">
         <v>6</v>
       </c>
       <c r="C10" s="79">
         <v>42565</v>
       </c>
-      <c r="D10" s="117">
+      <c r="D10" s="113">
         <v>42565</v>
       </c>
       <c r="E10" s="82">
@@ -1942,7 +1941,7 @@
       <c r="F10" s="83">
         <v>42565</v>
       </c>
-      <c r="G10" s="118">
+      <c r="G10" s="114">
         <v>100</v>
       </c>
       <c r="H10" s="74" t="s">
@@ -1951,42 +1950,42 @@
       <c r="I10" s="66"/>
     </row>
     <row r="11" spans="1:9" s="50" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="142"/>
+      <c r="A11" s="140"/>
       <c r="B11" s="62" t="s">
         <v>66</v>
       </c>
       <c r="C11" s="81"/>
-      <c r="D11" s="120"/>
-      <c r="E11" s="110">
-        <v>42565</v>
-      </c>
-      <c r="F11" s="111"/>
-      <c r="G11" s="128"/>
+      <c r="D11" s="116"/>
+      <c r="E11" s="106">
+        <v>42565</v>
+      </c>
+      <c r="F11" s="107"/>
+      <c r="G11" s="124"/>
       <c r="H11" s="75"/>
       <c r="I11" s="69"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="142"/>
+      <c r="A12" s="140"/>
       <c r="B12" s="61" t="s">
         <v>29</v>
       </c>
-      <c r="C12" s="145"/>
-      <c r="D12" s="146"/>
-      <c r="E12" s="146"/>
-      <c r="F12" s="146"/>
-      <c r="G12" s="146"/>
-      <c r="H12" s="146"/>
-      <c r="I12" s="147"/>
+      <c r="C12" s="143"/>
+      <c r="D12" s="144"/>
+      <c r="E12" s="144"/>
+      <c r="F12" s="144"/>
+      <c r="G12" s="144"/>
+      <c r="H12" s="144"/>
+      <c r="I12" s="145"/>
     </row>
     <row r="13" spans="1:9" s="48" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="142"/>
+      <c r="A13" s="140"/>
       <c r="B13" s="77" t="s">
         <v>30</v>
       </c>
       <c r="C13" s="79">
         <v>42565</v>
       </c>
-      <c r="D13" s="117">
+      <c r="D13" s="113">
         <v>42565</v>
       </c>
       <c r="E13" s="79">
@@ -1995,7 +1994,7 @@
       <c r="F13" s="80">
         <v>42565</v>
       </c>
-      <c r="G13" s="118">
+      <c r="G13" s="114">
         <v>100</v>
       </c>
       <c r="H13" s="74" t="s">
@@ -2004,14 +2003,14 @@
       <c r="I13" s="66"/>
     </row>
     <row r="14" spans="1:9" s="48" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="142"/>
+      <c r="A14" s="140"/>
       <c r="B14" s="77" t="s">
         <v>31</v>
       </c>
       <c r="C14" s="79">
         <v>42565</v>
       </c>
-      <c r="D14" s="117">
+      <c r="D14" s="113">
         <v>42565</v>
       </c>
       <c r="E14" s="79">
@@ -2020,7 +2019,7 @@
       <c r="F14" s="80">
         <v>42565</v>
       </c>
-      <c r="G14" s="118">
+      <c r="G14" s="114">
         <v>100</v>
       </c>
       <c r="H14" s="74" t="s">
@@ -2029,14 +2028,14 @@
       <c r="I14" s="66"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="142"/>
+      <c r="A15" s="140"/>
       <c r="B15" s="77" t="s">
         <v>35</v>
       </c>
       <c r="C15" s="79">
         <v>42565</v>
       </c>
-      <c r="D15" s="117">
+      <c r="D15" s="113">
         <v>42565</v>
       </c>
       <c r="E15" s="79">
@@ -2045,7 +2044,7 @@
       <c r="F15" s="80">
         <v>42565</v>
       </c>
-      <c r="G15" s="118">
+      <c r="G15" s="114">
         <v>100</v>
       </c>
       <c r="H15" s="74" t="s">
@@ -2054,14 +2053,14 @@
       <c r="I15" s="66"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="142"/>
+      <c r="A16" s="140"/>
       <c r="B16" s="77" t="s">
         <v>36</v>
       </c>
       <c r="C16" s="79">
         <v>42565</v>
       </c>
-      <c r="D16" s="117">
+      <c r="D16" s="113">
         <v>42565</v>
       </c>
       <c r="E16" s="79">
@@ -2070,7 +2069,7 @@
       <c r="F16" s="80">
         <v>42565</v>
       </c>
-      <c r="G16" s="118">
+      <c r="G16" s="114">
         <v>100</v>
       </c>
       <c r="H16" s="74" t="s">
@@ -2079,14 +2078,14 @@
       <c r="I16" s="66"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="142"/>
+      <c r="A17" s="140"/>
       <c r="B17" s="77" t="s">
         <v>37</v>
       </c>
       <c r="C17" s="79">
         <v>42565</v>
       </c>
-      <c r="D17" s="117">
+      <c r="D17" s="113">
         <v>42565</v>
       </c>
       <c r="E17" s="79">
@@ -2095,7 +2094,7 @@
       <c r="F17" s="80">
         <v>42565</v>
       </c>
-      <c r="G17" s="118">
+      <c r="G17" s="114">
         <v>100</v>
       </c>
       <c r="H17" s="74" t="s">
@@ -2104,14 +2103,14 @@
       <c r="I17" s="66"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="142"/>
+      <c r="A18" s="140"/>
       <c r="B18" s="61" t="s">
         <v>26</v>
       </c>
       <c r="C18" s="79">
         <v>42565</v>
       </c>
-      <c r="D18" s="117">
+      <c r="D18" s="113">
         <v>42565</v>
       </c>
       <c r="E18" s="79">
@@ -2120,7 +2119,7 @@
       <c r="F18" s="80">
         <v>42565</v>
       </c>
-      <c r="G18" s="118">
+      <c r="G18" s="114">
         <v>100</v>
       </c>
       <c r="H18" s="74" t="s">
@@ -2129,251 +2128,267 @@
       <c r="I18" s="66"/>
     </row>
     <row r="19" spans="1:9" s="50" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="142"/>
+      <c r="A19" s="140"/>
       <c r="B19" s="63" t="s">
         <v>50</v>
       </c>
       <c r="C19" s="81"/>
-      <c r="D19" s="120"/>
-      <c r="E19" s="114"/>
-      <c r="F19" s="115"/>
-      <c r="G19" s="128"/>
+      <c r="D19" s="116"/>
+      <c r="E19" s="110"/>
+      <c r="F19" s="111"/>
+      <c r="G19" s="124"/>
       <c r="H19" s="71"/>
       <c r="I19" s="69"/>
     </row>
     <row r="20" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="143"/>
-      <c r="B20" s="97" t="s">
+      <c r="A20" s="141"/>
+      <c r="B20" s="93" t="s">
         <v>51</v>
       </c>
       <c r="C20" s="82">
         <v>42565</v>
       </c>
-      <c r="D20" s="121">
+      <c r="D20" s="117">
         <v>42573</v>
       </c>
-      <c r="E20" s="116">
+      <c r="E20" s="112">
         <v>42565</v>
       </c>
       <c r="F20" s="83">
         <v>42566</v>
       </c>
-      <c r="G20" s="129">
+      <c r="G20" s="125">
         <v>100</v>
       </c>
       <c r="H20" s="72" t="s">
         <v>48</v>
       </c>
-      <c r="I20" s="96" t="s">
+      <c r="I20" s="92" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="141">
+      <c r="A21" s="139">
         <v>2</v>
       </c>
       <c r="B21" s="65" t="s">
         <v>52</v>
       </c>
       <c r="C21" s="84"/>
-      <c r="D21" s="122"/>
+      <c r="D21" s="118"/>
       <c r="E21" s="84"/>
       <c r="F21" s="85"/>
-      <c r="G21" s="130"/>
+      <c r="G21" s="126"/>
       <c r="H21" s="73"/>
       <c r="I21" s="70"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="142"/>
+      <c r="A22" s="140"/>
       <c r="B22" s="61" t="s">
         <v>53</v>
       </c>
-      <c r="C22" s="102">
+      <c r="C22" s="98">
         <v>42566</v>
       </c>
-      <c r="D22" s="123">
+      <c r="D22" s="119">
         <v>42566</v>
       </c>
-      <c r="E22" s="95">
+      <c r="E22" s="91">
         <v>42566</v>
       </c>
-      <c r="F22" s="98">
+      <c r="F22" s="94">
         <v>42566</v>
       </c>
-      <c r="G22" s="107">
+      <c r="G22" s="103">
         <v>100</v>
       </c>
-      <c r="H22" s="99" t="s">
+      <c r="H22" s="95" t="s">
         <v>48</v>
       </c>
       <c r="I22" s="66"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="142"/>
+      <c r="A23" s="140"/>
       <c r="B23" s="61" t="s">
         <v>54</v>
       </c>
-      <c r="C23" s="102">
+      <c r="C23" s="98">
         <v>42566</v>
       </c>
-      <c r="D23" s="123">
+      <c r="D23" s="119">
         <v>42566</v>
       </c>
-      <c r="E23" s="95">
+      <c r="E23" s="91">
         <v>42566</v>
       </c>
-      <c r="F23" s="98">
+      <c r="F23" s="94">
         <v>42566</v>
       </c>
-      <c r="G23" s="107">
+      <c r="G23" s="103">
         <v>100</v>
       </c>
-      <c r="H23" s="99" t="s">
+      <c r="H23" s="95" t="s">
         <v>48</v>
       </c>
       <c r="I23" s="66"/>
     </row>
     <row r="24" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="143"/>
+      <c r="A24" s="141"/>
       <c r="B24" s="76" t="s">
         <v>55</v>
       </c>
-      <c r="C24" s="106">
+      <c r="C24" s="102">
         <v>42566</v>
       </c>
-      <c r="D24" s="124">
+      <c r="D24" s="120">
         <v>42566</v>
       </c>
-      <c r="E24" s="95">
+      <c r="E24" s="91">
         <v>42566</v>
       </c>
-      <c r="F24" s="98">
+      <c r="F24" s="94">
         <v>42566</v>
       </c>
-      <c r="G24" s="107">
+      <c r="G24" s="103">
         <v>100</v>
       </c>
-      <c r="H24" s="100" t="s">
+      <c r="H24" s="96" t="s">
         <v>48</v>
       </c>
       <c r="I24" s="64"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" s="144">
+      <c r="A25" s="142">
         <v>3</v>
       </c>
-      <c r="B25" s="103" t="s">
+      <c r="B25" s="99" t="s">
         <v>56</v>
       </c>
-      <c r="C25" s="104">
+      <c r="C25" s="100">
         <v>42569</v>
       </c>
-      <c r="D25" s="125">
+      <c r="D25" s="121">
         <v>42569</v>
       </c>
-      <c r="E25" s="95">
+      <c r="E25" s="91">
         <v>42566</v>
       </c>
-      <c r="F25" s="174">
+      <c r="F25" s="131">
         <v>42569</v>
       </c>
-      <c r="G25" s="134">
+      <c r="G25" s="128">
         <v>100</v>
       </c>
-      <c r="H25" s="135" t="s">
+      <c r="H25" s="129" t="s">
         <v>48</v>
       </c>
-      <c r="I25" s="105"/>
+      <c r="I25" s="101"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" s="142"/>
+      <c r="A26" s="140"/>
       <c r="B26" s="61" t="s">
         <v>57</v>
       </c>
-      <c r="C26" s="95">
+      <c r="C26" s="91">
         <v>42569</v>
       </c>
-      <c r="D26" s="123">
+      <c r="D26" s="119">
         <v>42569</v>
       </c>
-      <c r="E26" s="95">
+      <c r="E26" s="91">
         <v>42569</v>
       </c>
-      <c r="F26" s="98">
-        <v>42569</v>
-      </c>
-      <c r="G26" s="118">
-        <v>100</v>
-      </c>
-      <c r="H26" s="93" t="s">
-        <v>48</v>
+      <c r="F26" s="94"/>
+      <c r="G26" s="114">
+        <v>86</v>
+      </c>
+      <c r="H26" s="130" t="s">
+        <v>68</v>
       </c>
       <c r="I26" s="66"/>
     </row>
     <row r="27" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="143"/>
+      <c r="A27" s="141"/>
       <c r="B27" s="76" t="s">
         <v>58</v>
       </c>
-      <c r="C27" s="101">
+      <c r="C27" s="97">
         <v>42569</v>
       </c>
-      <c r="D27" s="124">
+      <c r="D27" s="120">
         <v>42569</v>
       </c>
-      <c r="E27" s="101"/>
-      <c r="F27" s="175"/>
-      <c r="G27" s="129"/>
-      <c r="H27" s="94"/>
+      <c r="E27" s="97">
+        <v>42569</v>
+      </c>
+      <c r="F27" s="132"/>
+      <c r="G27" s="125">
+        <v>70</v>
+      </c>
+      <c r="H27" s="130" t="s">
+        <v>68</v>
+      </c>
       <c r="I27" s="64"/>
     </row>
     <row r="28" spans="1:9" s="48" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A28" s="141">
+      <c r="A28" s="139">
         <v>4</v>
       </c>
       <c r="B28" s="65" t="s">
         <v>59</v>
       </c>
-      <c r="C28" s="88"/>
-      <c r="D28" s="126"/>
-      <c r="E28" s="88"/>
+      <c r="C28" s="86"/>
+      <c r="D28" s="122"/>
+      <c r="E28" s="86"/>
       <c r="F28" s="58"/>
-      <c r="G28" s="133"/>
+      <c r="G28" s="127"/>
       <c r="H28" s="70"/>
       <c r="I28" s="70"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="142"/>
+    <row r="29" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="140"/>
       <c r="B29" s="61" t="s">
         <v>62</v>
       </c>
-      <c r="C29" s="95">
+      <c r="C29" s="91">
         <v>42570</v>
       </c>
-      <c r="D29" s="123">
+      <c r="D29" s="119">
         <v>42570</v>
       </c>
-      <c r="E29" s="86"/>
+      <c r="E29" s="97">
+        <v>42569</v>
+      </c>
       <c r="F29" s="56"/>
-      <c r="G29" s="131"/>
-      <c r="H29" s="66"/>
+      <c r="G29" s="103">
+        <v>70</v>
+      </c>
+      <c r="H29" s="130" t="s">
+        <v>68</v>
+      </c>
       <c r="I29" s="66"/>
     </row>
     <row r="30" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="143"/>
+      <c r="A30" s="141"/>
       <c r="B30" s="76" t="s">
         <v>63</v>
       </c>
-      <c r="C30" s="101">
+      <c r="C30" s="97">
         <v>42570</v>
       </c>
-      <c r="D30" s="124">
+      <c r="D30" s="120">
         <v>42570</v>
       </c>
-      <c r="E30" s="87"/>
+      <c r="E30" s="97">
+        <v>42570</v>
+      </c>
       <c r="F30" s="57"/>
-      <c r="G30" s="132"/>
-      <c r="H30" s="64"/>
+      <c r="G30" s="133">
+        <v>62</v>
+      </c>
+      <c r="H30" s="130" t="s">
+        <v>68</v>
+      </c>
       <c r="I30" s="64"/>
     </row>
     <row r="31" spans="1:9" s="48" customFormat="1" x14ac:dyDescent="0.25">
@@ -2388,14 +2403,14 @@
       <c r="I31" s="52"/>
     </row>
     <row r="33" spans="2:9" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B33" s="89" t="s">
+      <c r="B33" s="87" t="s">
         <v>46</v>
       </c>
       <c r="C33" s="54"/>
       <c r="D33" s="54"/>
       <c r="E33" s="54"/>
       <c r="F33" s="54"/>
-      <c r="G33" s="89" t="s">
+      <c r="G33" s="87" t="s">
         <v>47</v>
       </c>
       <c r="H33" s="54"/>
@@ -2422,33 +2437,33 @@
       <c r="I35" s="54"/>
     </row>
     <row r="36" spans="2:9" s="48" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B36" s="91" t="s">
+      <c r="B36" s="89" t="s">
         <v>12</v>
       </c>
-      <c r="C36" s="149" t="s">
+      <c r="C36" s="147" t="s">
         <v>8</v>
       </c>
-      <c r="D36" s="149"/>
-      <c r="E36" s="149"/>
+      <c r="D36" s="147"/>
+      <c r="E36" s="147"/>
       <c r="F36" s="54"/>
       <c r="G36" s="53"/>
-      <c r="H36" s="92" t="s">
+      <c r="H36" s="90" t="s">
         <v>10</v>
       </c>
       <c r="I36" s="54"/>
     </row>
     <row r="37" spans="2:9" s="48" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B37" s="90" t="s">
+      <c r="B37" s="88" t="s">
         <v>52</v>
       </c>
-      <c r="C37" s="136" t="s">
+      <c r="C37" s="134" t="s">
         <v>61</v>
       </c>
-      <c r="D37" s="136"/>
-      <c r="E37" s="136"/>
+      <c r="D37" s="134"/>
+      <c r="E37" s="134"/>
       <c r="F37" s="54"/>
       <c r="G37" s="54"/>
-      <c r="H37" s="90" t="s">
+      <c r="H37" s="88" t="s">
         <v>18</v>
       </c>
       <c r="I37" s="54"/>
@@ -2474,28 +2489,28 @@
       <c r="I39" s="54"/>
     </row>
     <row r="40" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B40" s="91" t="s">
+      <c r="B40" s="89" t="s">
         <v>9</v>
       </c>
-      <c r="C40" s="149" t="s">
+      <c r="C40" s="147" t="s">
         <v>11</v>
       </c>
-      <c r="D40" s="149"/>
-      <c r="E40" s="149"/>
+      <c r="D40" s="147"/>
+      <c r="E40" s="147"/>
       <c r="F40" s="54"/>
       <c r="G40" s="54"/>
       <c r="H40" s="54"/>
       <c r="I40" s="54"/>
     </row>
     <row r="41" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B41" s="90" t="s">
+      <c r="B41" s="88" t="s">
         <v>20</v>
       </c>
-      <c r="C41" s="136" t="s">
+      <c r="C41" s="134" t="s">
         <v>20</v>
       </c>
-      <c r="D41" s="136"/>
-      <c r="E41" s="136"/>
+      <c r="D41" s="134"/>
+      <c r="E41" s="134"/>
       <c r="F41" s="54"/>
       <c r="G41" s="54"/>
       <c r="H41" s="54"/>
@@ -2605,7 +2620,7 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="162" t="s">
+      <c r="A2" s="160" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="16" t="s">
@@ -2618,14 +2633,14 @@
         <f>((C2/3)*100)</f>
         <v>33.333333333333329</v>
       </c>
-      <c r="E2" s="165">
+      <c r="E2" s="163">
         <f>(AVERAGE(C2:C4))*100</f>
         <v>66.666666666666657</v>
       </c>
       <c r="F2" s="4"/>
     </row>
     <row r="3" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="163"/>
+      <c r="A3" s="161"/>
       <c r="B3" s="7" t="s">
         <v>5</v>
       </c>
@@ -2636,11 +2651,11 @@
         <f t="shared" ref="D3:D4" si="0">((C3/3)*100)</f>
         <v>33.333333333333329</v>
       </c>
-      <c r="E3" s="166"/>
+      <c r="E3" s="164"/>
       <c r="F3" s="4"/>
     </row>
     <row r="4" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="164"/>
+      <c r="A4" s="162"/>
       <c r="B4" s="18" t="s">
         <v>6</v>
       </c>
@@ -2651,11 +2666,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E4" s="167"/>
+      <c r="E4" s="165"/>
       <c r="F4" s="4"/>
     </row>
     <row r="5" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="168" t="s">
+      <c r="A5" s="166" t="s">
         <v>7</v>
       </c>
       <c r="B5" s="27" t="s">
@@ -2666,14 +2681,14 @@
         <f>(AVERAGE(C6:C13)*100)*0.5</f>
         <v>0</v>
       </c>
-      <c r="E5" s="171">
+      <c r="E5" s="169">
         <f>D5+D14</f>
         <v>0</v>
       </c>
       <c r="F5" s="4"/>
     </row>
     <row r="6" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="169"/>
+      <c r="A6" s="167"/>
       <c r="B6" s="31" t="s">
         <v>30</v>
       </c>
@@ -2684,11 +2699,11 @@
         <f>(C6/8)*100</f>
         <v>0</v>
       </c>
-      <c r="E6" s="172"/>
+      <c r="E6" s="170"/>
       <c r="F6" s="4"/>
     </row>
     <row r="7" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="169"/>
+      <c r="A7" s="167"/>
       <c r="B7" s="31" t="s">
         <v>31</v>
       </c>
@@ -2699,11 +2714,11 @@
         <f t="shared" ref="D7:D13" si="1">(C7/8)*100</f>
         <v>0</v>
       </c>
-      <c r="E7" s="172"/>
+      <c r="E7" s="170"/>
       <c r="F7" s="4"/>
     </row>
     <row r="8" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="169"/>
+      <c r="A8" s="167"/>
       <c r="B8" s="31" t="s">
         <v>32</v>
       </c>
@@ -2714,11 +2729,11 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="E8" s="172"/>
+      <c r="E8" s="170"/>
       <c r="F8" s="4"/>
     </row>
     <row r="9" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="169"/>
+      <c r="A9" s="167"/>
       <c r="B9" s="31" t="s">
         <v>33</v>
       </c>
@@ -2729,11 +2744,11 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="E9" s="172"/>
+      <c r="E9" s="170"/>
       <c r="F9" s="4"/>
     </row>
     <row r="10" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="169"/>
+      <c r="A10" s="167"/>
       <c r="B10" s="31" t="s">
         <v>34</v>
       </c>
@@ -2744,11 +2759,11 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="E10" s="172"/>
+      <c r="E10" s="170"/>
       <c r="F10" s="4"/>
     </row>
     <row r="11" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="169"/>
+      <c r="A11" s="167"/>
       <c r="B11" s="31" t="s">
         <v>35</v>
       </c>
@@ -2759,11 +2774,11 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="E11" s="172"/>
+      <c r="E11" s="170"/>
       <c r="F11" s="4"/>
     </row>
     <row r="12" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="169"/>
+      <c r="A12" s="167"/>
       <c r="B12" s="31" t="s">
         <v>36</v>
       </c>
@@ -2774,11 +2789,11 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="E12" s="172"/>
+      <c r="E12" s="170"/>
       <c r="F12" s="4"/>
     </row>
     <row r="13" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="169"/>
+      <c r="A13" s="167"/>
       <c r="B13" s="31" t="s">
         <v>37</v>
       </c>
@@ -2789,11 +2804,11 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="E13" s="172"/>
+      <c r="E13" s="170"/>
       <c r="F13" s="4"/>
     </row>
     <row r="14" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="170"/>
+      <c r="A14" s="168"/>
       <c r="B14" s="29" t="s">
         <v>26</v>
       </c>
@@ -2804,7 +2819,7 @@
         <f>(C14/2)*100</f>
         <v>0</v>
       </c>
-      <c r="E14" s="173"/>
+      <c r="E14" s="171"/>
       <c r="F14" s="4"/>
     </row>
     <row r="15" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -3016,12 +3031,12 @@
       <c r="F40" s="4"/>
     </row>
     <row r="41" spans="1:6" ht="24" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="159" t="s">
+      <c r="A41" s="157" t="s">
         <v>27</v>
       </c>
-      <c r="B41" s="160"/>
-      <c r="C41" s="160"/>
-      <c r="D41" s="161"/>
+      <c r="B41" s="158"/>
+      <c r="C41" s="158"/>
+      <c r="D41" s="159"/>
       <c r="E41" s="47">
         <f>(AVERAGE(E2,E5))</f>
         <v>33.333333333333329</v>

</xml_diff>